<commit_message>
Hands On Demos - Day 1.
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="22" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <t>Core Java 8</t>
   </si>
   <si>
-    <t xml:space="preserve"> Database &amp; PostGreSQL with DevOps (Git, Sonarqube, Gradle, Jenkin)</t>
+    <t>Database &amp; PostGreSQL with DevOps (Git, Sonarqube, Gradle, Jenkin)</t>
   </si>
   <si>
     <t>Core Java Assignments</t>
@@ -1137,10 +1137,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -1270,22 +1270,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1302,6 +1286,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1311,7 +1303,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1333,16 +1325,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1355,9 +1363,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1372,7 +1379,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1380,13 +1387,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1432,7 +1432,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1444,49 +1462,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1504,7 +1480,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1516,13 +1498,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1540,43 +1588,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1589,30 +1613,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1756,15 +1756,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1776,6 +1767,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1827,127 +1827,127 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2385,8 +2385,8 @@
   <sheetPr/>
   <dimension ref="A7:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:F40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2777,7 +2777,7 @@
   <sheetPr/>
   <dimension ref="A1:D413"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C309" sqref="C309"/>

</xml_diff>

<commit_message>
Added Course Materials - Week 2.
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="22" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="433">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Core Java 8</t>
   </si>
   <si>
-    <t>Database &amp; PostGreSQL with DevOps (Git, Sonarqube, Gradle, Jenkin)</t>
+    <t xml:space="preserve"> Database &amp; PostGreSQL with DevOps (Git, Sonarqube, Gradle, Jenkin)</t>
   </si>
   <si>
     <t>Core Java Assignments</t>
@@ -74,7 +74,7 @@
     <t>React Assignments</t>
   </si>
   <si>
-    <t>Sprint 2 + HTML 5, CSS 3 with bootstrap 4, Javascript, Typescript &amp;React MCQ</t>
+    <t>Sprint 2 + HTML 5, CSS 3 with bootstrap 4, Javascript, Typescript &amp; React MCQ</t>
   </si>
   <si>
     <t>Total Training Duration</t>
@@ -501,7 +501,7 @@
     <t>Java Loops</t>
   </si>
   <si>
-    <t>Hands On Exercises - Java Loops</t>
+    <t>Hands-On Exercises - Java Loops, Strings, Numbers and Dates</t>
   </si>
   <si>
     <t>Day 3</t>
@@ -1017,8 +1017,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">                                                                First, you will discover why you would want to use collections instead of arrays.                                                                     Then, you will cover the capabilities of lists, sets, maps, queues and also the different data structure tradeoffs. Finally, you will explore important collection algorithms and how different collection implementations work.                                                                               By the end of this course, you will know how to use Java Collections to process data.</t>
+      <t xml:space="preserve">                                                                First, you will discover why you would want to use collections instead of arrays.                                                                     Then, you will cover the capabilities of lists, sets, maps, queues and also the different data structure tradeoffs. Finally, you will explore important collection algorithms and how different collection implementations work.                                                                               By the end of this course, you will know how to use Java Collections to process data.                                                     </t>
     </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Regular Expressions in Java   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                      Learn how to define a search pattern for strings  that can then be used to search for data in a text. </t>
+    </r>
   </si>
   <si>
     <t>2. Working with Collections</t>
@@ -1078,9 +1100,6 @@
     <t>4. Collection with Uniqueness - Sets</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Introduction </t>
-  </si>
-  <si>
     <t>2. Set Features (Live Coding)</t>
   </si>
   <si>
@@ -1120,10 +1139,535 @@
     <t>9. Core Java Queues</t>
   </si>
   <si>
+    <t>6. Regular Expressions</t>
+  </si>
+  <si>
+    <t>1. String Matching with Regular Expressions</t>
+  </si>
+  <si>
+    <t>2. String Class Support for Regular Expressions</t>
+  </si>
+  <si>
+    <t>3. Dedicated Regular Expression Classes</t>
+  </si>
+  <si>
+    <t>4. Summary</t>
+  </si>
+  <si>
     <t>Java Collections</t>
   </si>
   <si>
-    <t>Hands On Exercises - Collections</t>
+    <t>Hands On Exercises - Collections and Regular Expressions</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - List</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Map</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Set</t>
+  </si>
+  <si>
+    <t>Day 7</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">At the core of every project, there is always extensive testing.                                          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Learn the benefits of TDD (Test-driven Development) and  create TDD applications using the JUnit 5 testing framework.                                                              First, you'll learn how to develop TDD applications and how to use mock objects with JUnit 5.                                                                Next, you'll discover how to move a non-TDD application into the platform.                                                          Finally, you'll dive into how to integrate JUnit5 into your workflow.                                             By the end of this course, you'll have the know how to develop safe and flexible Java applications using TDD with JUnit 5.</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Introducing TDD and JUnit5</t>
+  </si>
+  <si>
+    <t>2. Code Coverage</t>
+  </si>
+  <si>
+    <t>3. JUnit 5 Architecture</t>
+  </si>
+  <si>
+    <t>4. The Flights Management Application</t>
+  </si>
+  <si>
+    <t>3. Adding New Features to the Application Using TDD and JUnit 5</t>
+  </si>
+  <si>
+    <t>1. Use JUnit 5 More Effectively</t>
+  </si>
+  <si>
+    <t>2. Adding a Premium Flight</t>
+  </si>
+  <si>
+    <t>3. Adding a Passenger Only Once</t>
+  </si>
+  <si>
+    <t>4. Adding a Policy for Bonus Points</t>
+  </si>
+  <si>
+    <t>4. Introduction to Mockito</t>
+  </si>
+  <si>
+    <t>5. What Is Mocking?</t>
+  </si>
+  <si>
+    <t>6. Why Mock?</t>
+  </si>
+  <si>
+    <t>7. Test Doubles</t>
+  </si>
+  <si>
+    <t>8. What Is a Unit?</t>
+  </si>
+  <si>
+    <t>9. Mock Classes or Mock Interfaces?</t>
+  </si>
+  <si>
+    <t>5. TDD by Integrating JUnit 5 with Mockito</t>
+  </si>
+  <si>
+    <t>1. Introduction to Integration</t>
+  </si>
+  <si>
+    <t>2. Implement the Air Conditioning Functionality</t>
+  </si>
+  <si>
+    <t>3. Implement the Database Access Functionality</t>
+  </si>
+  <si>
+    <t>4. Implement the Statistics Functionality</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - JUnit 4</t>
+  </si>
+  <si>
+    <t>Hands On Lab 1 -  Test Cases and Test Fixtures</t>
+  </si>
+  <si>
+    <t>Day 8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">File Navigation and I/O    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learn about working with streams, files, and the file system.                              You'll also learn about I/O topics specific to working with files such open/closing files, detecting end-of-file, and buffering.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Input and Output with Streams and Files</t>
+  </si>
+  <si>
+    <t>2. Streams Overview</t>
+  </si>
+  <si>
+    <t>3. Reading and Writing with Streams</t>
+  </si>
+  <si>
+    <t>4. Common Stream Classes</t>
+  </si>
+  <si>
+    <t>5. Stream Errors and Cleanup</t>
+  </si>
+  <si>
+    <t>6. Demo: Working with Try-with-resources Part 1</t>
+  </si>
+  <si>
+    <t>7. Demo: Working with Try-with-resources Part 2</t>
+  </si>
+  <si>
+    <t>8. Chaining Streams</t>
+  </si>
+  <si>
+    <t>9. File and Buffered Streams</t>
+  </si>
+  <si>
+    <t>10. Random Access File class</t>
+  </si>
+  <si>
+    <t>11. Class Declaration</t>
+  </si>
+  <si>
+    <t>12. RandomAccessFile Methods in Java</t>
+  </si>
+  <si>
+    <t>13. Demo: Creating and Using a Random Access File object</t>
+  </si>
+  <si>
+    <t>14. Java.io.Console class</t>
+  </si>
+  <si>
+    <t>15. Java.io.Console methods</t>
+  </si>
+  <si>
+    <t>16. Demo: ConsoleDemo.java</t>
+  </si>
+  <si>
+    <t>17. Summary</t>
+  </si>
+  <si>
+    <t>Java IO</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Input and Output</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Serialization                                        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learn how to serialize an object out to a serialization stream, and then restore that object information back from that serialization stream.</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Persisting Objects with Serialization</t>
+  </si>
+  <si>
+    <t>2. Java Serialization Overview</t>
+  </si>
+  <si>
+    <t>3. Being Serializable</t>
+  </si>
+  <si>
+    <t>4. Serializing/Deserializing an Object</t>
+  </si>
+  <si>
+    <t>5. Transient Fields</t>
+  </si>
+  <si>
+    <t>6. Demo: Serialize and deserialize an object</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Serialization</t>
+  </si>
+  <si>
+    <t>Multithreading in Java                          Java Thread Join                                                   Java Thread Sleep                                                Thread Pools                                       Concurrency Issues                                    Thread Safety and Synchronization                                       
+Thread Exceptions                                 Analyze Deadlock Condition
+Java Thread States                                    Prevent Thread Execution                               Set the Priority for Threads
+ Using wait, notify and notifyAll</t>
+  </si>
+  <si>
+    <t>3. Multithreading and Concurrency</t>
+  </si>
+  <si>
+    <t>2. A Quick Look at the Basics</t>
+  </si>
+  <si>
+    <t>3. The Move to Multithreading</t>
+  </si>
+  <si>
+    <t>4. Java Threading Foundation</t>
+  </si>
+  <si>
+    <t>5. Thread Pools</t>
+  </si>
+  <si>
+    <t>6. Creating a Closer Relationship Between Thread Tasks</t>
+  </si>
+  <si>
+    <t>7. Concurrency Issues</t>
+  </si>
+  <si>
+    <t>8. Coordinating Method Access</t>
+  </si>
+  <si>
+    <t>9. Manual Synchronization</t>
+  </si>
+  <si>
+    <t>10. Manually Synchronized Code</t>
+  </si>
+  <si>
+    <t>11. More Concurrency-related Types</t>
+  </si>
+  <si>
+    <t>12. How to Analyze Deadlock and avoid it in Java</t>
+  </si>
+  <si>
+    <t>13. Demo: Deadlock Example and Solution</t>
+  </si>
+  <si>
+    <t>14.  Avoid Dead Lock condition</t>
+  </si>
+  <si>
+    <t>15. Thread States and Transitions</t>
+  </si>
+  <si>
+    <t>16. Runnable and Running States</t>
+  </si>
+  <si>
+    <t>17. Relinquishing control using suspend method</t>
+  </si>
+  <si>
+    <t>18. Methods to prevent Thread Execution</t>
+  </si>
+  <si>
+    <t>19. Demo : Methods to prevent Thread Execution</t>
+  </si>
+  <si>
+    <t>20. Thread Priorities</t>
+  </si>
+  <si>
+    <t>21. Demo: Set the Priority for Threads</t>
+  </si>
+  <si>
+    <t>22. wait notify notifyall</t>
+  </si>
+  <si>
+    <t>23. Demo: Printing Threads in Sequence in Java</t>
+  </si>
+  <si>
+    <t>24. Summary</t>
+  </si>
+  <si>
+    <t>Multithreading and Concurrency</t>
+  </si>
+  <si>
+    <t>Hands On Lab 1 - Extending Thread class</t>
+  </si>
+  <si>
+    <t>Hands On Lab 2 - Implement Runnable interface</t>
+  </si>
+  <si>
+    <t>Hands On Lab 3  - ThreadGroup, ThreadPriority, View all threads</t>
+  </si>
+  <si>
+    <t>Hands On Lab 4 - Synchronization</t>
+  </si>
+  <si>
+    <t>Hands On Lab 5 - Inter-thread communication</t>
+  </si>
+  <si>
+    <t>Hands On Lab 6 -Timer and TimerTask</t>
+  </si>
+  <si>
+    <t>Day 9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lambda expressions and the Stream API bring new fundamental patterns to the Java platform.    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                  Develop the skills to  iterate, filter and extract data from collections using Lambda Expressions.                                 Learn to solve problems much more efficiently with the patterns brought by the Stream API.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Introduction to Lambda Expressions in Java 8</t>
+  </si>
+  <si>
+    <t>2. Module Outline</t>
+  </si>
+  <si>
+    <t>3. The FileFilter Example</t>
+  </si>
+  <si>
+    <t>4. A First Lambda Expression</t>
+  </si>
+  <si>
+    <t>5. Live Coding: A First Lambda Expression</t>
+  </si>
+  <si>
+    <t>6. Live Coding: Runnable and Comparator Examples</t>
+  </si>
+  <si>
+    <t>7. Several Ways of Writing Lambda Expressions</t>
+  </si>
+  <si>
+    <t>8. Three Questions About Lambda Expressions</t>
+  </si>
+  <si>
+    <t>9. Functional Interfaces</t>
+  </si>
+  <si>
+    <t>10. Is a Lambda Expression an Object?</t>
+  </si>
+  <si>
+    <t>11. The Functional Interfaces Toolbox</t>
+  </si>
+  <si>
+    <t>12. Method References</t>
+  </si>
+  <si>
+    <t>13. Processing Collections with Lambdas</t>
+  </si>
+  <si>
+    <t>14. Changing the Way Interfaces Work?</t>
+  </si>
+  <si>
+    <t>15. Default and Static Methods in Java 8 Interfaces</t>
+  </si>
+  <si>
+    <t>16. New Patterns: The Predicate Interface Example</t>
+  </si>
+  <si>
+    <t>17. Live Coding: New Patterns Examples</t>
+  </si>
+  <si>
+    <t>18. Module Wrap Up</t>
+  </si>
+  <si>
+    <t>2. Java 8 Stream API and Collectors I</t>
+  </si>
+  <si>
+    <t>1. Introduction, Module Outline</t>
+  </si>
+  <si>
+    <t>2. The Map / Filter / Reduce Algorithm</t>
+  </si>
+  <si>
+    <t>3. What Is a Stream?</t>
+  </si>
+  <si>
+    <t>4. Definition of a Stream in Java 8</t>
+  </si>
+  <si>
+    <t>5. Building and Consuming a Stream</t>
+  </si>
+  <si>
+    <t>6. Filtering a Stream</t>
+  </si>
+  <si>
+    <t>7. Live Coding: Consuming and Filtering a Stream</t>
+  </si>
+  <si>
+    <t>8. Lazy Operations on a Stream</t>
+  </si>
+  <si>
+    <t>9. Live Coding: Intermediary and Terminal Operations</t>
+  </si>
+  <si>
+    <t>11. Wrapping up Intermediary and Terminal Operations</t>
+  </si>
+  <si>
+    <t>12. The Map Operation</t>
+  </si>
+  <si>
+    <t>13. The Flatmap Operation</t>
+  </si>
+  <si>
+    <t>14. Live Coding: Map and Flatmap Examples</t>
+  </si>
+  <si>
+    <t>15. Wrapping up Map and Filter on a Stream</t>
+  </si>
+  <si>
+    <t>16.Reduction, Functions, and Bifunctions</t>
+  </si>
+  <si>
+    <t>17. Reduction of the Empty Set: Identity Element</t>
+  </si>
+  <si>
+    <t>3. Java 8 Stream API and Collectors II</t>
+  </si>
+  <si>
+    <t>18. Optionals</t>
+  </si>
+  <si>
+    <t>19. Pattern for the Optionals</t>
+  </si>
+  <si>
+    <t>20. Wrapping up Reduction Operations</t>
+  </si>
+  <si>
+    <t>21. Terminal Operations</t>
+  </si>
+  <si>
+    <t>22. Live Coding: Reductions, Optionals</t>
+  </si>
+  <si>
+    <t>23. Wrapping up Operations and Optionals</t>
+  </si>
+  <si>
+    <t>24. Collectors, Collecting in a String, in a List</t>
+  </si>
+  <si>
+    <t>25. Collecting in a Map</t>
+  </si>
+  <si>
+    <t>26. Live Coding: Processing Streams</t>
+  </si>
+  <si>
+    <t>27. Wrapping Module</t>
+  </si>
+  <si>
+    <t>1.  Introduction to Lambda Expressions in Java 8</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Lambda Expressions</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Stream API and Collectors I</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Stream API and Collectors II</t>
   </si>
   <si>
     <t>Total # of Days for Core Java 8</t>
@@ -1138,11 +1682,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="39">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1209,6 +1753,20 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1248,9 +1806,54 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1263,8 +1866,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1279,18 +1899,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1304,60 +1916,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1370,9 +1929,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1385,18 +1950,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="14"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="37">
@@ -1432,103 +2002,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1546,7 +2020,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1558,61 +2182,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1706,56 +2276,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1798,6 +2318,56 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1806,7 +2376,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1824,134 +2394,134 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2005,47 +2575,76 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2061,7 +2660,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2385,8 +2984,8 @@
   <sheetPr/>
   <dimension ref="A7:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2399,316 +2998,316 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="25">
+      <c r="F9" s="36">
         <v>1</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="38">
+        <v>10.5</v>
+      </c>
+      <c r="I9" s="38">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" ht="30.75" spans="6:9">
+      <c r="F10" s="39">
+        <v>2</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="38">
+        <v>2</v>
+      </c>
+      <c r="I10" s="38">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="6:9">
+      <c r="F11" s="39">
+        <v>3</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="38">
+        <v>4</v>
+      </c>
+      <c r="I11" s="38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" spans="6:9">
+      <c r="F12" s="39">
+        <v>4</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" spans="6:9">
+      <c r="F13" s="39">
+        <v>5</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="38">
+        <v>2</v>
+      </c>
+      <c r="I13" s="38">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" spans="6:9">
+      <c r="F14" s="39">
+        <v>6</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="38">
+        <v>2</v>
+      </c>
+      <c r="I14" s="38">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" spans="6:9">
+      <c r="F15" s="39">
+        <v>7</v>
+      </c>
+      <c r="G15" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="27">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" ht="30.75" spans="6:9">
-      <c r="F10" s="28">
+      <c r="H15" s="38">
+        <v>1</v>
+      </c>
+      <c r="I15" s="38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" spans="6:9">
+      <c r="F16" s="39">
+        <v>8</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="38">
+        <v>6</v>
+      </c>
+      <c r="I16" s="38">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" ht="14" customHeight="1" spans="6:9">
+      <c r="F17" s="39">
+        <v>9</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="38">
+        <v>3</v>
+      </c>
+      <c r="I17" s="38">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" ht="14" customHeight="1" spans="6:9">
+      <c r="F18" s="39">
+        <v>10</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="38">
+        <v>5</v>
+      </c>
+      <c r="I18" s="38">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" spans="6:9">
+      <c r="F19" s="39">
+        <v>11</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="38">
+        <v>1</v>
+      </c>
+      <c r="I19" s="38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" spans="6:9">
+      <c r="F20" s="39">
+        <v>12</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="38">
+        <v>4</v>
+      </c>
+      <c r="I20" s="38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" spans="6:9">
+      <c r="F21" s="39">
+        <v>13</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="38">
+        <v>1</v>
+      </c>
+      <c r="I21" s="38">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" spans="6:9">
+      <c r="F22" s="39">
+        <v>14</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="38">
+        <v>6</v>
+      </c>
+      <c r="I22" s="38">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" spans="6:9">
+      <c r="F23" s="39">
+        <v>15</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="38">
         <v>2</v>
       </c>
-      <c r="G10" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="27">
-        <v>2.5</v>
-      </c>
-      <c r="I10" s="27">
+      <c r="I23" s="38">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" ht="30.75" spans="6:9">
+      <c r="F24" s="39">
+        <v>16</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="38">
+        <v>4</v>
+      </c>
+      <c r="I24" s="38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" spans="6:9">
+      <c r="F25" s="42"/>
+      <c r="G25" s="43" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="28">
-        <v>3</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="27">
-        <v>4</v>
-      </c>
-      <c r="I11" s="27">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" spans="6:9">
-      <c r="F12" s="28">
-        <v>4</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="I12" s="27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" spans="6:9">
-      <c r="F13" s="28">
-        <v>5</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="27">
-        <v>2</v>
-      </c>
-      <c r="I13" s="27">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" spans="6:9">
-      <c r="F14" s="28">
-        <v>6</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="27">
-        <v>2</v>
-      </c>
-      <c r="I14" s="27">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" spans="6:9">
-      <c r="F15" s="28">
-        <v>7</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="27">
-        <v>1</v>
-      </c>
-      <c r="I15" s="27">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" spans="6:9">
-      <c r="F16" s="28">
-        <v>8</v>
-      </c>
-      <c r="G16" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="27">
-        <v>6</v>
-      </c>
-      <c r="I16" s="27">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" ht="14" customHeight="1" spans="6:9">
-      <c r="F17" s="28">
-        <v>9</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="27">
-        <v>3</v>
-      </c>
-      <c r="I17" s="27">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" ht="14" customHeight="1" spans="6:9">
-      <c r="F18" s="28">
-        <v>10</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="27">
-        <v>5</v>
-      </c>
-      <c r="I18" s="27">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" spans="6:9">
-      <c r="F19" s="28">
-        <v>11</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="27">
-        <v>1</v>
-      </c>
-      <c r="I19" s="27">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" spans="6:9">
-      <c r="F20" s="28">
-        <v>12</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="27">
-        <v>4</v>
-      </c>
-      <c r="I20" s="27">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" spans="6:9">
-      <c r="F21" s="28">
-        <v>13</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="27">
-        <v>1</v>
-      </c>
-      <c r="I21" s="27">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" spans="6:9">
-      <c r="F22" s="28">
-        <v>14</v>
-      </c>
-      <c r="G22" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="27">
-        <v>6</v>
-      </c>
-      <c r="I22" s="27">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" spans="6:9">
-      <c r="F23" s="28">
-        <v>15</v>
-      </c>
-      <c r="G23" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="27">
-        <v>2</v>
-      </c>
-      <c r="I23" s="27">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" ht="30.75" spans="6:9">
-      <c r="F24" s="28">
-        <v>16</v>
-      </c>
-      <c r="G24" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="27">
-        <v>4</v>
-      </c>
-      <c r="I24" s="27">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" spans="6:9">
-      <c r="F25" s="31"/>
-      <c r="G25" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="33">
+      <c r="H25" s="44">
         <f>SUM(H9:H24)</f>
         <v>54</v>
       </c>
-      <c r="I25" s="41">
+      <c r="I25" s="52">
         <f>SUM(I9:I24)</f>
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="45" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35" t="s">
+      <c r="A31" s="45"/>
+      <c r="B31" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="36">
+      <c r="A32" s="47">
         <v>1</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="36">
+      <c r="A33" s="47">
         <v>2</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
     </row>
     <row r="34" ht="15" customHeight="1" spans="1:6">
-      <c r="A34" s="36">
+      <c r="A34" s="47">
         <v>3</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
     </row>
     <row r="36" customFormat="1" spans="1:4">
-      <c r="A36" s="34"/>
-      <c r="B36" s="35" t="s">
+      <c r="A36" s="45"/>
+      <c r="B36" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
     </row>
     <row r="37" customFormat="1" ht="30" customHeight="1" spans="1:6">
-      <c r="A37" s="36">
+      <c r="A37" s="47">
         <v>1</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -2720,40 +3319,40 @@
       <c r="F37" s="17"/>
     </row>
     <row r="38" customFormat="1" ht="29" customHeight="1" spans="1:6">
-      <c r="A38" s="40">
+      <c r="A38" s="51">
         <v>2</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
     </row>
     <row r="39" customFormat="1" ht="15" customHeight="1" spans="1:6">
-      <c r="A39" s="40">
+      <c r="A39" s="51">
         <v>3</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
     </row>
     <row r="40" ht="54" customHeight="1" spans="1:6">
-      <c r="A40" s="40">
+      <c r="A40" s="51">
         <v>4</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2775,15 +3374,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D413"/>
+  <dimension ref="A1:C572"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C309" sqref="C309"/>
+      <selection pane="bottomLeft" activeCell="F309" sqref="F309"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="38.625" customWidth="1"/>
     <col min="2" max="2" width="35.125" customWidth="1"/>
@@ -4694,14 +5293,11 @@
         <v>264</v>
       </c>
     </row>
-    <row r="271" ht="15" spans="1:4">
+    <row r="271" ht="15" spans="1:3">
       <c r="A271" s="3"/>
       <c r="B271" s="7"/>
       <c r="C271" s="10" t="s">
         <v>265</v>
-      </c>
-      <c r="D271">
-        <v>20</v>
       </c>
     </row>
     <row r="272" ht="15" spans="1:3">
@@ -4741,28 +5337,28 @@
         <v>270</v>
       </c>
       <c r="C277" s="10" t="s">
-        <v>271</v>
+        <v>73</v>
       </c>
     </row>
     <row r="278" ht="15" spans="1:3">
       <c r="A278" s="3"/>
       <c r="B278" s="7"/>
       <c r="C278" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="279" ht="15" spans="1:3">
       <c r="A279" s="3"/>
       <c r="B279" s="7"/>
       <c r="C279" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="280" ht="15" spans="1:3">
       <c r="A280" s="3"/>
       <c r="B280" s="7"/>
       <c r="C280" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="281" ht="15" spans="1:3">
@@ -4783,7 +5379,7 @@
       <c r="A283" s="3"/>
       <c r="B283" s="7"/>
       <c r="C283" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="284" spans="1:1">
@@ -4792,66 +5388,66 @@
     <row r="285" ht="15" spans="1:3">
       <c r="A285" s="3"/>
       <c r="B285" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C285" s="10" t="s">
-        <v>271</v>
+        <v>73</v>
       </c>
     </row>
     <row r="286" ht="15" spans="1:3">
       <c r="A286" s="3"/>
       <c r="B286" s="7"/>
       <c r="C286" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="287" ht="15" spans="1:3">
       <c r="A287" s="3"/>
       <c r="B287" s="7"/>
       <c r="C287" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="288" ht="15" spans="1:3">
       <c r="A288" s="3"/>
       <c r="B288" s="7"/>
       <c r="C288" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="289" ht="15" spans="1:3">
       <c r="A289" s="3"/>
       <c r="B289" s="7"/>
       <c r="C289" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="290" ht="15" spans="1:3">
       <c r="A290" s="3"/>
       <c r="B290" s="7"/>
       <c r="C290" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="291" ht="15" spans="1:3">
       <c r="A291" s="3"/>
       <c r="B291" s="7"/>
       <c r="C291" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="292" ht="15" spans="1:3">
       <c r="A292" s="3"/>
       <c r="B292" s="7"/>
       <c r="C292" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="293" ht="15" spans="1:3">
       <c r="A293" s="3"/>
       <c r="B293" s="7"/>
       <c r="C293" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="294" ht="15" spans="1:3">
@@ -4866,49 +5462,1160 @@
     </row>
     <row r="296" ht="15" spans="1:3">
       <c r="A296" s="3"/>
-      <c r="B296" s="14" t="s">
+      <c r="B296" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C296" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="297" ht="15" spans="1:3">
+      <c r="A297" s="3"/>
+      <c r="B297" s="7"/>
+      <c r="C297" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="298" ht="15" spans="1:3">
+      <c r="A298" s="3"/>
+      <c r="B298" s="7"/>
+      <c r="C298" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="299" ht="15" spans="1:3">
+      <c r="A299" s="3"/>
+      <c r="B299" s="7"/>
+      <c r="C299" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" s="3"/>
+    </row>
+    <row r="301" ht="15" spans="1:3">
+      <c r="A301" s="3"/>
+      <c r="B301" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C296" s="15" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3">
-      <c r="A297" s="3"/>
-      <c r="B297" s="14"/>
-      <c r="C297" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="298" ht="9" customHeight="1" spans="1:3">
-      <c r="A298" s="18"/>
-      <c r="B298" s="16"/>
-      <c r="C298" s="16"/>
-    </row>
-    <row r="412" ht="18.75" spans="1:2">
-      <c r="A412" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="B412" s="22">
+      <c r="C301" s="15" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" s="3"/>
+      <c r="B302" s="14"/>
+      <c r="C302" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="303" ht="15" customHeight="1" spans="1:3">
+      <c r="A303" s="21"/>
+      <c r="B303" s="22"/>
+      <c r="C303" s="23" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="304" ht="12" customHeight="1" spans="1:3">
+      <c r="A304" s="21"/>
+      <c r="B304" s="22"/>
+      <c r="C304" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="305" ht="15" customHeight="1" spans="1:3">
+      <c r="A305" s="21"/>
+      <c r="B305" s="22"/>
+      <c r="C305" s="23" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="306" ht="9" customHeight="1" spans="1:3">
+      <c r="A306" s="18"/>
+      <c r="B306" s="16"/>
+      <c r="C306" s="16"/>
+    </row>
+    <row r="307" ht="24.75" spans="1:3">
+      <c r="A307" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B307" s="2"/>
+      <c r="C307" s="2"/>
+    </row>
+    <row r="308" ht="15.75" spans="1:3">
+      <c r="A308" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B308" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C308" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="309" ht="15.75" spans="1:3">
+      <c r="A309" s="3"/>
+      <c r="B309" s="4"/>
+      <c r="C309" s="5"/>
+    </row>
+    <row r="310" ht="15" spans="1:3">
+      <c r="A310" s="3"/>
+      <c r="B310" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C310" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="311" ht="15" spans="1:3">
+      <c r="A311" s="3"/>
+      <c r="B311" s="7"/>
+      <c r="C311" s="10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="312" ht="15" spans="1:3">
+      <c r="A312" s="3"/>
+      <c r="B312" s="7"/>
+      <c r="C312" s="10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="313" ht="15" spans="1:3">
+      <c r="A313" s="3"/>
+      <c r="B313" s="7"/>
+      <c r="C313" s="10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="314" customFormat="1" spans="1:1">
+      <c r="A314" s="3"/>
+    </row>
+    <row r="315" ht="15" spans="1:3">
+      <c r="A315" s="3"/>
+      <c r="B315" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C315" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="316" ht="15" spans="1:3">
+      <c r="A316" s="3"/>
+      <c r="B316" s="7"/>
+      <c r="C316" s="10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="317" ht="15" spans="1:3">
+      <c r="A317" s="3"/>
+      <c r="B317" s="7"/>
+      <c r="C317" s="10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="318" ht="15" spans="1:3">
+      <c r="A318" s="3"/>
+      <c r="B318" s="7"/>
+      <c r="C318" s="10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="319" customFormat="1" ht="15.75" spans="1:3">
+      <c r="A319" s="3"/>
+      <c r="B319" s="7"/>
+      <c r="C319" s="10"/>
+    </row>
+    <row r="320" customFormat="1" ht="15" spans="1:3">
+      <c r="A320" s="3"/>
+      <c r="B320" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C320" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="321" customFormat="1" ht="15" spans="1:3">
+      <c r="A321" s="3"/>
+      <c r="B321" s="7"/>
+      <c r="C321" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="322" customFormat="1" ht="15" spans="1:3">
+      <c r="A322" s="3"/>
+      <c r="B322" s="7"/>
+      <c r="C322" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="323" customFormat="1" ht="15" spans="1:3">
+      <c r="A323" s="3"/>
+      <c r="B323" s="7"/>
+      <c r="C323" s="11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="324" customFormat="1" ht="15" spans="1:3">
+      <c r="A324" s="3"/>
+      <c r="B324" s="7"/>
+      <c r="C324" s="11" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="325" customFormat="1" ht="15" spans="1:3">
+      <c r="A325" s="3"/>
+      <c r="B325" s="7"/>
+      <c r="C325" s="11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="326" customFormat="1" ht="15" spans="1:3">
+      <c r="A326" s="3"/>
+      <c r="B326" s="7"/>
+      <c r="C326" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="327" customFormat="1" spans="1:1">
+      <c r="A327" s="3"/>
+    </row>
+    <row r="328" ht="15" spans="1:3">
+      <c r="A328" s="3"/>
+      <c r="B328" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C328" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="329" ht="15" spans="1:3">
+      <c r="A329" s="3"/>
+      <c r="B329" s="7"/>
+      <c r="C329" s="10" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="330" ht="15" spans="1:3">
+      <c r="A330" s="3"/>
+      <c r="B330" s="7"/>
+      <c r="C330" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="331" ht="15" spans="1:3">
+      <c r="A331" s="3"/>
+      <c r="B331" s="7"/>
+      <c r="C331" s="10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="332" customFormat="1" spans="1:1">
+      <c r="A332" s="3"/>
+    </row>
+    <row r="333" ht="15" spans="1:3">
+      <c r="A333" s="3"/>
+      <c r="B333" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C333" s="15" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3">
+      <c r="A334" s="3"/>
+      <c r="B334" s="14"/>
+      <c r="C334" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3">
+      <c r="A335" s="3"/>
+      <c r="B335" s="14"/>
+      <c r="C335" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="336" ht="9" customHeight="1" spans="1:3">
+      <c r="A336" s="18"/>
+      <c r="B336" s="16"/>
+      <c r="C336" s="16"/>
+    </row>
+    <row r="337" ht="24.75" spans="1:3">
+      <c r="A337" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B337" s="2"/>
+      <c r="C337" s="2"/>
+    </row>
+    <row r="338" ht="15" spans="1:3">
+      <c r="A338" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="B338" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="C338" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3">
+      <c r="A339" s="24"/>
+      <c r="B339" s="19"/>
+      <c r="C339" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="340" ht="15" spans="1:3">
+      <c r="A340" s="24"/>
+      <c r="B340" s="19"/>
+      <c r="C340" s="13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="341" ht="15" spans="1:3">
+      <c r="A341" s="24"/>
+      <c r="B341" s="19"/>
+      <c r="C341" s="13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="342" ht="15" spans="1:3">
+      <c r="A342" s="24"/>
+      <c r="B342" s="19"/>
+      <c r="C342" s="13" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="343" ht="15" spans="1:3">
+      <c r="A343" s="24"/>
+      <c r="B343" s="19"/>
+      <c r="C343" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="344" ht="15" spans="1:3">
+      <c r="A344" s="24"/>
+      <c r="B344" s="19"/>
+      <c r="C344" s="13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="345" ht="15" spans="1:3">
+      <c r="A345" s="24"/>
+      <c r="B345" s="19"/>
+      <c r="C345" s="13" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="346" ht="15" spans="1:3">
+      <c r="A346" s="24"/>
+      <c r="B346" s="19"/>
+      <c r="C346" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="347" ht="15" spans="1:3">
+      <c r="A347" s="24"/>
+      <c r="B347" s="19"/>
+      <c r="C347" s="13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="348" ht="15" spans="1:3">
+      <c r="A348" s="24"/>
+      <c r="B348" s="19"/>
+      <c r="C348" s="13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="349" ht="15" spans="1:3">
+      <c r="A349" s="24"/>
+      <c r="B349" s="19"/>
+      <c r="C349" s="13" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="350" ht="15" spans="1:3">
+      <c r="A350" s="24"/>
+      <c r="B350" s="19"/>
+      <c r="C350" s="13" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="351" ht="15" spans="1:3">
+      <c r="A351" s="24"/>
+      <c r="B351" s="19"/>
+      <c r="C351" s="13" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3">
+      <c r="A352" s="24"/>
+      <c r="B352" s="19"/>
+      <c r="C352" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3">
+      <c r="A353" s="24"/>
+      <c r="B353" s="19"/>
+      <c r="C353" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3">
+      <c r="A354" s="24"/>
+      <c r="B354" s="19"/>
+      <c r="C354" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="355" customFormat="1" ht="15.75" spans="1:2">
+      <c r="A355" s="24"/>
+      <c r="B355" s="19"/>
+    </row>
+    <row r="356" ht="15" spans="1:3">
+      <c r="A356" s="24"/>
+      <c r="B356" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C356" s="15" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3">
+      <c r="A357" s="24"/>
+      <c r="B357" s="14"/>
+      <c r="C357" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="359" ht="15" spans="1:3">
+      <c r="A359" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="B359" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="C359" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3">
+      <c r="A360" s="24"/>
+      <c r="B360" s="19"/>
+      <c r="C360" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="361" ht="15" spans="1:3">
+      <c r="A361" s="24"/>
+      <c r="B361" s="19"/>
+      <c r="C361" s="13" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="362" ht="15" spans="1:3">
+      <c r="A362" s="24"/>
+      <c r="B362" s="19"/>
+      <c r="C362" s="13" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="363" ht="15" spans="1:3">
+      <c r="A363" s="24"/>
+      <c r="B363" s="19"/>
+      <c r="C363" s="13" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="364" ht="15" spans="1:3">
+      <c r="A364" s="24"/>
+      <c r="B364" s="19"/>
+      <c r="C364" s="13" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3">
+      <c r="A365" s="24"/>
+      <c r="B365" s="19"/>
+      <c r="C365" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="366" customFormat="1" ht="15.75" spans="1:2">
+      <c r="A366" s="24"/>
+      <c r="B366" s="19"/>
+    </row>
+    <row r="367" ht="15" spans="1:3">
+      <c r="A367" s="24"/>
+      <c r="B367" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C367" s="15" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3">
+      <c r="A368" s="24"/>
+      <c r="B368" s="14"/>
+      <c r="C368" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="370" ht="15" spans="1:3">
+      <c r="A370" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="B370" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="C370" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="371" ht="15" spans="1:3">
+      <c r="A371" s="27"/>
+      <c r="B371" s="26"/>
+      <c r="C371" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="372" ht="15" spans="1:3">
+      <c r="A372" s="27"/>
+      <c r="B372" s="26"/>
+      <c r="C372" s="13" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="373" ht="15" spans="1:3">
+      <c r="A373" s="27"/>
+      <c r="B373" s="26"/>
+      <c r="C373" s="13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="374" ht="15" spans="1:3">
+      <c r="A374" s="27"/>
+      <c r="B374" s="26"/>
+      <c r="C374" s="13" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="375" ht="15" spans="1:3">
+      <c r="A375" s="27"/>
+      <c r="B375" s="26"/>
+      <c r="C375" s="28" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="376" ht="15" spans="1:3">
+      <c r="A376" s="27"/>
+      <c r="B376" s="26"/>
+      <c r="C376" s="13" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="377" ht="15" spans="1:3">
+      <c r="A377" s="27"/>
+      <c r="B377" s="26"/>
+      <c r="C377" s="28" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="378" ht="15" spans="1:3">
+      <c r="A378" s="27"/>
+      <c r="B378" s="26"/>
+      <c r="C378" s="13" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="379" ht="15" spans="1:3">
+      <c r="A379" s="27"/>
+      <c r="B379" s="26"/>
+      <c r="C379" s="28" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="380" ht="15" spans="1:3">
+      <c r="A380" s="27"/>
+      <c r="B380" s="26"/>
+      <c r="C380" s="13" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="381" ht="15" spans="1:3">
+      <c r="A381" s="27"/>
+      <c r="B381" s="26"/>
+      <c r="C381" s="28" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="382" ht="15" spans="1:3">
+      <c r="A382" s="27"/>
+      <c r="B382" s="26"/>
+      <c r="C382" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="383" ht="15" spans="1:3">
+      <c r="A383" s="27"/>
+      <c r="B383" s="26"/>
+      <c r="C383" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="384" ht="15" spans="1:3">
+      <c r="A384" s="27"/>
+      <c r="B384" s="26"/>
+      <c r="C384" s="13" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="385" ht="15" spans="1:3">
+      <c r="A385" s="27"/>
+      <c r="B385" s="26"/>
+      <c r="C385" s="13" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="386" ht="15" spans="1:3">
+      <c r="A386" s="27"/>
+      <c r="B386" s="26"/>
+      <c r="C386" s="13" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="387" ht="15" spans="1:3">
+      <c r="A387" s="27"/>
+      <c r="B387" s="26"/>
+      <c r="C387" s="13" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="388" ht="15" spans="1:3">
+      <c r="A388" s="27"/>
+      <c r="B388" s="26"/>
+      <c r="C388" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="389" ht="15" spans="1:3">
+      <c r="A389" s="27"/>
+      <c r="B389" s="26"/>
+      <c r="C389" s="13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3">
+      <c r="A390" s="27"/>
+      <c r="B390" s="26"/>
+      <c r="C390" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3">
+      <c r="A391" s="27"/>
+      <c r="B391" s="26"/>
+      <c r="C391" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3">
+      <c r="A392" s="27"/>
+      <c r="B392" s="26"/>
+      <c r="C392" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3">
+      <c r="A393" s="27"/>
+      <c r="B393" s="26"/>
+      <c r="C393" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="394" customFormat="1" spans="1:1">
+      <c r="A394" s="27"/>
+    </row>
+    <row r="395" ht="15" spans="1:3">
+      <c r="A395" s="27"/>
+      <c r="B395" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C395" s="15" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="396" ht="15" spans="1:3">
+      <c r="A396" s="27"/>
+      <c r="B396" s="14"/>
+      <c r="C396" s="10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="397" ht="15" spans="1:3">
+      <c r="A397" s="27"/>
+      <c r="B397" s="14"/>
+      <c r="C397" s="10" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="398" ht="15" spans="1:3">
+      <c r="A398" s="27"/>
+      <c r="B398" s="14"/>
+      <c r="C398" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="399" ht="15" spans="1:3">
+      <c r="A399" s="27"/>
+      <c r="B399" s="14"/>
+      <c r="C399" s="10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="400" ht="15" spans="1:3">
+      <c r="A400" s="27"/>
+      <c r="B400" s="14"/>
+      <c r="C400" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="401" ht="15" spans="1:3">
+      <c r="A401" s="27"/>
+      <c r="B401" s="14"/>
+      <c r="C401" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="402" ht="9" customHeight="1" spans="1:3">
+      <c r="A402" s="18"/>
+      <c r="B402" s="16"/>
+      <c r="C402" s="16"/>
+    </row>
+    <row r="403" ht="24.75" spans="1:3">
+      <c r="A403" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B403" s="2"/>
+      <c r="C403" s="2"/>
+    </row>
+    <row r="404" ht="15" spans="1:3">
+      <c r="A404" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="B404" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="C404" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="405" ht="15" spans="1:3">
+      <c r="A405" s="29"/>
+      <c r="B405" s="26"/>
+      <c r="C405" s="13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="406" ht="15" spans="1:3">
+      <c r="A406" s="29"/>
+      <c r="B406" s="26"/>
+      <c r="C406" s="13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="407" ht="15" spans="1:3">
+      <c r="A407" s="29"/>
+      <c r="B407" s="26"/>
+      <c r="C407" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="408" ht="15" spans="1:3">
+      <c r="A408" s="29"/>
+      <c r="B408" s="26"/>
+      <c r="C408" s="13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="409" ht="15" spans="1:3">
+      <c r="A409" s="29"/>
+      <c r="B409" s="26"/>
+      <c r="C409" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="410" ht="15" spans="1:3">
+      <c r="A410" s="29"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="411" ht="15" spans="1:3">
+      <c r="A411" s="29"/>
+      <c r="B411" s="26"/>
+      <c r="C411" s="13" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="412" ht="15" spans="1:3">
+      <c r="A412" s="29"/>
+      <c r="B412" s="26"/>
+      <c r="C412" s="13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="413" ht="15" spans="1:3">
+      <c r="A413" s="29"/>
+      <c r="B413" s="26"/>
+      <c r="C413" s="13" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="414" ht="15" spans="1:3">
+      <c r="A414" s="29"/>
+      <c r="B414" s="26"/>
+      <c r="C414" s="13" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="415" ht="15" spans="1:3">
+      <c r="A415" s="29"/>
+      <c r="B415" s="26"/>
+      <c r="C415" s="13" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="416" ht="15" spans="1:3">
+      <c r="A416" s="29"/>
+      <c r="B416" s="26"/>
+      <c r="C416" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="417" ht="15" spans="1:3">
+      <c r="A417" s="29"/>
+      <c r="B417" s="26"/>
+      <c r="C417" s="13" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="418" ht="15" spans="1:3">
+      <c r="A418" s="29"/>
+      <c r="B418" s="26"/>
+      <c r="C418" s="13" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="419" ht="15" spans="1:3">
+      <c r="A419" s="29"/>
+      <c r="B419" s="26"/>
+      <c r="C419" s="13" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="420" ht="15" spans="1:3">
+      <c r="A420" s="29"/>
+      <c r="B420" s="26"/>
+      <c r="C420" s="13" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="421" ht="15" spans="1:3">
+      <c r="A421" s="29"/>
+      <c r="B421" s="26"/>
+      <c r="C421" s="13" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="422" ht="18" spans="1:3">
+      <c r="A422" s="29"/>
+      <c r="B422" s="26"/>
+      <c r="C422" s="13"/>
+    </row>
+    <row r="423" ht="15" spans="1:3">
+      <c r="A423" s="29"/>
+      <c r="B423" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="C423" s="13" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="424" ht="15" spans="1:3">
+      <c r="A424" s="29"/>
+      <c r="B424" s="26"/>
+      <c r="C424" s="13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="425" ht="15" spans="1:3">
+      <c r="A425" s="29"/>
+      <c r="B425" s="26"/>
+      <c r="C425" s="13" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="426" ht="15" spans="1:3">
+      <c r="A426" s="29"/>
+      <c r="B426" s="26"/>
+      <c r="C426" s="13" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="427" ht="15" spans="1:3">
+      <c r="A427" s="29"/>
+      <c r="B427" s="26"/>
+      <c r="C427" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="428" ht="15" spans="1:3">
+      <c r="A428" s="29"/>
+      <c r="B428" s="26"/>
+      <c r="C428" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="429" ht="15" spans="1:3">
+      <c r="A429" s="29"/>
+      <c r="B429" s="26"/>
+      <c r="C429" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="430" ht="15" spans="1:3">
+      <c r="A430" s="29"/>
+      <c r="B430" s="26"/>
+      <c r="C430" s="13" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="431" ht="15" spans="1:3">
+      <c r="A431" s="29"/>
+      <c r="B431" s="26"/>
+      <c r="C431" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="432" ht="15" spans="1:3">
+      <c r="A432" s="29"/>
+      <c r="B432" s="26"/>
+      <c r="C432" s="13" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="433" ht="15" spans="1:3">
+      <c r="A433" s="29"/>
+      <c r="B433" s="26"/>
+      <c r="C433" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="434" ht="15" spans="1:3">
+      <c r="A434" s="29"/>
+      <c r="B434" s="26"/>
+      <c r="C434" s="13" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="435" ht="15" spans="1:3">
+      <c r="A435" s="29"/>
+      <c r="B435" s="26"/>
+      <c r="C435" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="436" ht="15" spans="1:3">
+      <c r="A436" s="29"/>
+      <c r="B436" s="26"/>
+      <c r="C436" s="13" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="437" ht="15" spans="1:3">
+      <c r="A437" s="29"/>
+      <c r="B437" s="26"/>
+      <c r="C437" s="13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="438" ht="15" spans="1:3">
+      <c r="A438" s="29"/>
+      <c r="B438" s="26"/>
+      <c r="C438" s="13" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="439" ht="15" spans="1:3">
+      <c r="A439" s="29"/>
+      <c r="B439" s="26"/>
+      <c r="C439" s="13" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="440" ht="18" spans="1:3">
+      <c r="A440" s="29"/>
+      <c r="B440" s="26"/>
+      <c r="C440" s="13"/>
+    </row>
+    <row r="441" ht="15" spans="1:3">
+      <c r="A441" s="29"/>
+      <c r="B441" s="26" t="s">
+        <v>416</v>
+      </c>
+      <c r="C441" s="13" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="442" ht="15" spans="1:3">
+      <c r="A442" s="29"/>
+      <c r="B442" s="26"/>
+      <c r="C442" s="13" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="443" ht="15" spans="1:3">
+      <c r="A443" s="29"/>
+      <c r="B443" s="26"/>
+      <c r="C443" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="444" ht="15" spans="1:3">
+      <c r="A444" s="29"/>
+      <c r="B444" s="26"/>
+      <c r="C444" s="13" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="445" ht="15" spans="1:3">
+      <c r="A445" s="29"/>
+      <c r="B445" s="26"/>
+      <c r="C445" s="13" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="446" ht="15" spans="1:3">
+      <c r="A446" s="29"/>
+      <c r="B446" s="26"/>
+      <c r="C446" s="13" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="447" ht="15" spans="1:3">
+      <c r="A447" s="29"/>
+      <c r="B447" s="26"/>
+      <c r="C447" s="13" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="448" ht="15" spans="1:3">
+      <c r="A448" s="29"/>
+      <c r="B448" s="26"/>
+      <c r="C448" s="13" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="449" ht="15" spans="1:3">
+      <c r="A449" s="29"/>
+      <c r="B449" s="26"/>
+      <c r="C449" s="13" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="450" ht="15" spans="1:3">
+      <c r="A450" s="29"/>
+      <c r="B450" s="26"/>
+      <c r="C450" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="451" ht="18" spans="1:3">
+      <c r="A451" s="29"/>
+      <c r="B451" s="30"/>
+      <c r="C451" s="13"/>
+    </row>
+    <row r="452" ht="15" spans="1:3">
+      <c r="A452" s="29"/>
+      <c r="B452" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C452" s="15" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="453" ht="15" spans="1:3">
+      <c r="A453" s="29"/>
+      <c r="B453" s="14"/>
+      <c r="C453" s="10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="454" ht="15" spans="1:3">
+      <c r="A454" s="29"/>
+      <c r="B454" s="14"/>
+      <c r="C454" s="15" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="455" ht="15" spans="1:3">
+      <c r="A455" s="29"/>
+      <c r="B455" s="14"/>
+      <c r="C455" s="10" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="456" ht="15" spans="1:3">
+      <c r="A456" s="29"/>
+      <c r="B456" s="14"/>
+      <c r="C456" s="15" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="457" ht="15" spans="1:3">
+      <c r="A457" s="29"/>
+      <c r="B457" s="14"/>
+      <c r="C457" s="10" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3">
+      <c r="A458" s="31"/>
+      <c r="B458" s="31"/>
+      <c r="C458" s="31"/>
+    </row>
+    <row r="571" ht="18.75" spans="1:2">
+      <c r="A571" s="32" t="s">
+        <v>431</v>
+      </c>
+      <c r="B571" s="33">
         <v>10.5</v>
       </c>
     </row>
-    <row r="413" ht="18.75" spans="1:2">
-      <c r="A413" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="B413" s="22">
+    <row r="572" ht="18.75" spans="1:2">
+      <c r="A572" s="32" t="s">
+        <v>432</v>
+      </c>
+      <c r="B572" s="33">
         <v>84</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="75">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A51:C51"/>
     <mergeCell ref="A100:C100"/>
     <mergeCell ref="A145:C145"/>
     <mergeCell ref="A198:C198"/>
     <mergeCell ref="A255:C255"/>
+    <mergeCell ref="A307:C307"/>
+    <mergeCell ref="A337:C337"/>
+    <mergeCell ref="A403:C403"/>
     <mergeCell ref="A3:A14"/>
     <mergeCell ref="A16:A24"/>
     <mergeCell ref="A26:A35"/>
@@ -4919,7 +6626,12 @@
     <mergeCell ref="A146:A196"/>
     <mergeCell ref="A199:A230"/>
     <mergeCell ref="A232:A253"/>
-    <mergeCell ref="A256:A297"/>
+    <mergeCell ref="A256:A305"/>
+    <mergeCell ref="A308:A335"/>
+    <mergeCell ref="A338:A357"/>
+    <mergeCell ref="A359:A368"/>
+    <mergeCell ref="A370:A401"/>
+    <mergeCell ref="A404:A457"/>
     <mergeCell ref="B5:B14"/>
     <mergeCell ref="B16:B24"/>
     <mergeCell ref="B26:B35"/>
@@ -4953,8 +6665,28 @@
     <mergeCell ref="B269:B275"/>
     <mergeCell ref="B277:B283"/>
     <mergeCell ref="B285:B294"/>
-    <mergeCell ref="B296:B297"/>
+    <mergeCell ref="B296:B299"/>
+    <mergeCell ref="B301:B305"/>
+    <mergeCell ref="B310:B313"/>
+    <mergeCell ref="B315:B318"/>
+    <mergeCell ref="B320:B326"/>
+    <mergeCell ref="B328:B331"/>
+    <mergeCell ref="B333:B335"/>
+    <mergeCell ref="B338:B354"/>
+    <mergeCell ref="B356:B357"/>
+    <mergeCell ref="B359:B365"/>
+    <mergeCell ref="B367:B368"/>
+    <mergeCell ref="B370:B393"/>
+    <mergeCell ref="B395:B401"/>
+    <mergeCell ref="B404:B421"/>
+    <mergeCell ref="B423:B439"/>
+    <mergeCell ref="B441:B450"/>
+    <mergeCell ref="B452:B457"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C405" r:id="rId1" display="2. Module Outline"/>
+    <hyperlink ref="C419" r:id="rId2" display="16. New Patterns: The Predicate Interface Example"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Added Hands On Demos - Day 7.
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="22" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <t>Core Java 8</t>
   </si>
   <si>
-    <t xml:space="preserve"> Database &amp; PostGreSQL with DevOps (Git, Sonarqube, Gradle, Jenkin)</t>
+    <t>Database &amp; PostGreSQL with DevOps (Git, Sonarqube, Gradle, Jenkin)</t>
   </si>
   <si>
     <t>Core Java Assignments</t>
@@ -1681,10 +1681,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -1807,23 +1807,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1837,16 +1821,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1859,8 +1835,93 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1875,69 +1936,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2002,7 +2002,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2014,7 +2014,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2026,13 +2056,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2044,13 +2068,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2068,7 +2110,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2080,43 +2164,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2128,61 +2176,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2277,30 +2277,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -2318,19 +2294,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2346,6 +2311,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2368,15 +2342,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2394,134 +2394,134 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2575,13 +2575,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2984,8 +2977,8 @@
   <sheetPr/>
   <dimension ref="A7:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:I10"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2998,316 +2991,316 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="32" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="36">
+      <c r="F9" s="33">
         <v>1</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="35">
         <v>10.5</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="35">
         <v>84</v>
       </c>
     </row>
     <row r="10" ht="30.75" spans="6:9">
-      <c r="F10" s="39">
+      <c r="F10" s="36">
         <v>2</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="35">
         <v>2</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="35">
         <v>16</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="39">
+      <c r="F11" s="36">
         <v>3</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="35">
         <v>4</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="35">
         <v>32</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="6:9">
-      <c r="F12" s="39">
+      <c r="F12" s="36">
         <v>4</v>
       </c>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="35">
         <v>0.5</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I12" s="35">
         <v>4</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="6:9">
-      <c r="F13" s="39">
+      <c r="F13" s="36">
         <v>5</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="35">
         <v>2</v>
       </c>
-      <c r="I13" s="38">
+      <c r="I13" s="35">
         <v>16</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="6:9">
-      <c r="F14" s="39">
+      <c r="F14" s="36">
         <v>6</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="35">
         <v>2</v>
       </c>
-      <c r="I14" s="38">
+      <c r="I14" s="35">
         <v>16</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="6:9">
-      <c r="F15" s="39">
+      <c r="F15" s="36">
         <v>7</v>
       </c>
-      <c r="G15" s="40" t="s">
+      <c r="G15" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="35">
         <v>1</v>
       </c>
-      <c r="I15" s="38">
+      <c r="I15" s="35">
         <v>8</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="6:9">
-      <c r="F16" s="39">
+      <c r="F16" s="36">
         <v>8</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="35">
         <v>6</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="35">
         <v>40</v>
       </c>
     </row>
     <row r="17" ht="14" customHeight="1" spans="6:9">
-      <c r="F17" s="39">
+      <c r="F17" s="36">
         <v>9</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="35">
         <v>3</v>
       </c>
-      <c r="I17" s="38">
+      <c r="I17" s="35">
         <v>24</v>
       </c>
     </row>
     <row r="18" ht="14" customHeight="1" spans="6:9">
-      <c r="F18" s="39">
+      <c r="F18" s="36">
         <v>10</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="35">
         <v>5</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I18" s="35">
         <v>40</v>
       </c>
     </row>
     <row r="19" ht="15.75" spans="6:9">
-      <c r="F19" s="39">
+      <c r="F19" s="36">
         <v>11</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="35">
         <v>1</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="35">
         <v>8</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="6:9">
-      <c r="F20" s="39">
+      <c r="F20" s="36">
         <v>12</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="35">
         <v>4</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="35">
         <v>32</v>
       </c>
     </row>
     <row r="21" ht="15.75" spans="6:9">
-      <c r="F21" s="39">
+      <c r="F21" s="36">
         <v>13</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="35">
         <v>1</v>
       </c>
-      <c r="I21" s="38">
+      <c r="I21" s="35">
         <v>16</v>
       </c>
     </row>
     <row r="22" ht="15.75" spans="6:9">
-      <c r="F22" s="39">
+      <c r="F22" s="36">
         <v>14</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="35">
         <v>6</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="35">
         <v>48</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="6:9">
-      <c r="F23" s="39">
+      <c r="F23" s="36">
         <v>15</v>
       </c>
-      <c r="G23" s="41" t="s">
+      <c r="G23" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="35">
         <v>2</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="35">
         <v>16</v>
       </c>
     </row>
     <row r="24" ht="30.75" spans="6:9">
-      <c r="F24" s="39">
+      <c r="F24" s="36">
         <v>16</v>
       </c>
-      <c r="G24" s="41" t="s">
+      <c r="G24" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="35">
         <v>4</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="35">
         <v>32</v>
       </c>
     </row>
     <row r="25" ht="15.75" spans="6:9">
-      <c r="F25" s="42"/>
-      <c r="G25" s="43" t="s">
+      <c r="F25" s="39"/>
+      <c r="G25" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="44">
+      <c r="H25" s="41">
         <f>SUM(H9:H24)</f>
         <v>54</v>
       </c>
-      <c r="I25" s="52">
+      <c r="I25" s="49">
         <f>SUM(I9:I24)</f>
         <v>432</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="42" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="45"/>
-      <c r="B31" s="46" t="s">
+      <c r="A31" s="42"/>
+      <c r="B31" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="47">
+      <c r="A32" s="44">
         <v>1</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="47">
+      <c r="A33" s="44">
         <v>2</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
     </row>
     <row r="34" ht="15" customHeight="1" spans="1:6">
-      <c r="A34" s="47">
+      <c r="A34" s="44">
         <v>3</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
     </row>
     <row r="36" customFormat="1" spans="1:4">
-      <c r="A36" s="45"/>
-      <c r="B36" s="46" t="s">
+      <c r="A36" s="42"/>
+      <c r="B36" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
     </row>
     <row r="37" customFormat="1" ht="30" customHeight="1" spans="1:6">
-      <c r="A37" s="47">
+      <c r="A37" s="44">
         <v>1</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -3319,40 +3312,40 @@
       <c r="F37" s="17"/>
     </row>
     <row r="38" customFormat="1" ht="29" customHeight="1" spans="1:6">
-      <c r="A38" s="51">
+      <c r="A38" s="48">
         <v>2</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
     </row>
     <row r="39" customFormat="1" ht="15" customHeight="1" spans="1:6">
-      <c r="A39" s="51">
+      <c r="A39" s="48">
         <v>3</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
     </row>
     <row r="40" ht="54" customHeight="1" spans="1:6">
-      <c r="A40" s="51">
+      <c r="A40" s="48">
         <v>4</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3376,8 +3369,8 @@
   <sheetPr/>
   <dimension ref="A1:C572"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A393" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F309" sqref="F309"/>
     </sheetView>
@@ -5510,23 +5503,23 @@
       </c>
     </row>
     <row r="303" ht="15" customHeight="1" spans="1:3">
-      <c r="A303" s="21"/>
-      <c r="B303" s="22"/>
-      <c r="C303" s="23" t="s">
+      <c r="A303" s="3"/>
+      <c r="B303" s="14"/>
+      <c r="C303" s="10" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="304" ht="12" customHeight="1" spans="1:3">
-      <c r="A304" s="21"/>
-      <c r="B304" s="22"/>
-      <c r="C304" s="23" t="s">
+      <c r="A304" s="3"/>
+      <c r="B304" s="14"/>
+      <c r="C304" s="10" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="305" ht="15" customHeight="1" spans="1:3">
-      <c r="A305" s="21"/>
-      <c r="B305" s="22"/>
-      <c r="C305" s="23" t="s">
+      <c r="A305" s="3"/>
+      <c r="B305" s="14"/>
+      <c r="C305" s="10" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5749,7 +5742,7 @@
       <c r="C337" s="2"/>
     </row>
     <row r="338" ht="15" spans="1:3">
-      <c r="A338" s="24" t="s">
+      <c r="A338" s="21" t="s">
         <v>319</v>
       </c>
       <c r="B338" s="19" t="s">
@@ -5760,123 +5753,123 @@
       </c>
     </row>
     <row r="339" spans="1:3">
-      <c r="A339" s="24"/>
+      <c r="A339" s="21"/>
       <c r="B339" s="19"/>
       <c r="C339" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="340" ht="15" spans="1:3">
-      <c r="A340" s="24"/>
+      <c r="A340" s="21"/>
       <c r="B340" s="19"/>
       <c r="C340" s="13" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="341" ht="15" spans="1:3">
-      <c r="A341" s="24"/>
+      <c r="A341" s="21"/>
       <c r="B341" s="19"/>
       <c r="C341" s="13" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="342" ht="15" spans="1:3">
-      <c r="A342" s="24"/>
+      <c r="A342" s="21"/>
       <c r="B342" s="19"/>
       <c r="C342" s="13" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="343" ht="15" spans="1:3">
-      <c r="A343" s="24"/>
+      <c r="A343" s="21"/>
       <c r="B343" s="19"/>
       <c r="C343" s="13" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="344" ht="15" spans="1:3">
-      <c r="A344" s="24"/>
+      <c r="A344" s="21"/>
       <c r="B344" s="19"/>
       <c r="C344" s="13" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="345" ht="15" spans="1:3">
-      <c r="A345" s="24"/>
+      <c r="A345" s="21"/>
       <c r="B345" s="19"/>
       <c r="C345" s="13" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="346" ht="15" spans="1:3">
-      <c r="A346" s="24"/>
+      <c r="A346" s="21"/>
       <c r="B346" s="19"/>
       <c r="C346" s="13" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="347" ht="15" spans="1:3">
-      <c r="A347" s="24"/>
+      <c r="A347" s="21"/>
       <c r="B347" s="19"/>
       <c r="C347" s="13" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="348" ht="15" spans="1:3">
-      <c r="A348" s="24"/>
+      <c r="A348" s="21"/>
       <c r="B348" s="19"/>
       <c r="C348" s="13" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="349" ht="15" spans="1:3">
-      <c r="A349" s="24"/>
+      <c r="A349" s="21"/>
       <c r="B349" s="19"/>
       <c r="C349" s="13" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="350" ht="15" spans="1:3">
-      <c r="A350" s="24"/>
+      <c r="A350" s="21"/>
       <c r="B350" s="19"/>
       <c r="C350" s="13" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="351" ht="15" spans="1:3">
-      <c r="A351" s="24"/>
+      <c r="A351" s="21"/>
       <c r="B351" s="19"/>
       <c r="C351" s="13" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="352" spans="1:3">
-      <c r="A352" s="24"/>
+      <c r="A352" s="21"/>
       <c r="B352" s="19"/>
       <c r="C352" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="353" spans="1:3">
-      <c r="A353" s="24"/>
+      <c r="A353" s="21"/>
       <c r="B353" s="19"/>
       <c r="C353" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="354" spans="1:3">
-      <c r="A354" s="24"/>
+      <c r="A354" s="21"/>
       <c r="B354" s="19"/>
       <c r="C354" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="355" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A355" s="24"/>
+      <c r="A355" s="21"/>
       <c r="B355" s="19"/>
     </row>
     <row r="356" ht="15" spans="1:3">
-      <c r="A356" s="24"/>
+      <c r="A356" s="21"/>
       <c r="B356" s="14" t="s">
         <v>22</v>
       </c>
@@ -5885,14 +5878,14 @@
       </c>
     </row>
     <row r="357" spans="1:3">
-      <c r="A357" s="24"/>
+      <c r="A357" s="21"/>
       <c r="B357" s="14"/>
       <c r="C357" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="359" ht="15" spans="1:3">
-      <c r="A359" s="24" t="s">
+      <c r="A359" s="21" t="s">
         <v>339</v>
       </c>
       <c r="B359" s="19" t="s">
@@ -5903,53 +5896,53 @@
       </c>
     </row>
     <row r="360" spans="1:3">
-      <c r="A360" s="24"/>
+      <c r="A360" s="21"/>
       <c r="B360" s="19"/>
       <c r="C360" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="361" ht="15" spans="1:3">
-      <c r="A361" s="24"/>
+      <c r="A361" s="21"/>
       <c r="B361" s="19"/>
       <c r="C361" s="13" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="362" ht="15" spans="1:3">
-      <c r="A362" s="24"/>
+      <c r="A362" s="21"/>
       <c r="B362" s="19"/>
       <c r="C362" s="13" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="363" ht="15" spans="1:3">
-      <c r="A363" s="24"/>
+      <c r="A363" s="21"/>
       <c r="B363" s="19"/>
       <c r="C363" s="13" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="364" ht="15" spans="1:3">
-      <c r="A364" s="24"/>
+      <c r="A364" s="21"/>
       <c r="B364" s="19"/>
       <c r="C364" s="13" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="365" spans="1:3">
-      <c r="A365" s="24"/>
+      <c r="A365" s="21"/>
       <c r="B365" s="19"/>
       <c r="C365" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="366" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A366" s="24"/>
+      <c r="A366" s="21"/>
       <c r="B366" s="19"/>
     </row>
     <row r="367" ht="15" spans="1:3">
-      <c r="A367" s="24"/>
+      <c r="A367" s="21"/>
       <c r="B367" s="14" t="s">
         <v>22</v>
       </c>
@@ -5958,17 +5951,17 @@
       </c>
     </row>
     <row r="368" spans="1:3">
-      <c r="A368" s="24"/>
+      <c r="A368" s="21"/>
       <c r="B368" s="14"/>
       <c r="C368" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="370" ht="15" spans="1:3">
-      <c r="A370" s="25" t="s">
+      <c r="A370" s="22" t="s">
         <v>347</v>
       </c>
-      <c r="B370" s="26" t="s">
+      <c r="B370" s="23" t="s">
         <v>348</v>
       </c>
       <c r="C370" s="13" t="s">
@@ -5976,171 +5969,171 @@
       </c>
     </row>
     <row r="371" ht="15" spans="1:3">
-      <c r="A371" s="27"/>
-      <c r="B371" s="26"/>
+      <c r="A371" s="24"/>
+      <c r="B371" s="23"/>
       <c r="C371" s="13" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="372" ht="15" spans="1:3">
-      <c r="A372" s="27"/>
-      <c r="B372" s="26"/>
+      <c r="A372" s="24"/>
+      <c r="B372" s="23"/>
       <c r="C372" s="13" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="373" ht="15" spans="1:3">
-      <c r="A373" s="27"/>
-      <c r="B373" s="26"/>
+      <c r="A373" s="24"/>
+      <c r="B373" s="23"/>
       <c r="C373" s="13" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="374" ht="15" spans="1:3">
-      <c r="A374" s="27"/>
-      <c r="B374" s="26"/>
+      <c r="A374" s="24"/>
+      <c r="B374" s="23"/>
       <c r="C374" s="13" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="375" ht="15" spans="1:3">
-      <c r="A375" s="27"/>
-      <c r="B375" s="26"/>
-      <c r="C375" s="28" t="s">
+      <c r="A375" s="24"/>
+      <c r="B375" s="23"/>
+      <c r="C375" s="25" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="376" ht="15" spans="1:3">
-      <c r="A376" s="27"/>
-      <c r="B376" s="26"/>
+      <c r="A376" s="24"/>
+      <c r="B376" s="23"/>
       <c r="C376" s="13" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="377" ht="15" spans="1:3">
-      <c r="A377" s="27"/>
-      <c r="B377" s="26"/>
-      <c r="C377" s="28" t="s">
+      <c r="A377" s="24"/>
+      <c r="B377" s="23"/>
+      <c r="C377" s="25" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="378" ht="15" spans="1:3">
-      <c r="A378" s="27"/>
-      <c r="B378" s="26"/>
+      <c r="A378" s="24"/>
+      <c r="B378" s="23"/>
       <c r="C378" s="13" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="379" ht="15" spans="1:3">
-      <c r="A379" s="27"/>
-      <c r="B379" s="26"/>
-      <c r="C379" s="28" t="s">
+      <c r="A379" s="24"/>
+      <c r="B379" s="23"/>
+      <c r="C379" s="25" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="380" ht="15" spans="1:3">
-      <c r="A380" s="27"/>
-      <c r="B380" s="26"/>
+      <c r="A380" s="24"/>
+      <c r="B380" s="23"/>
       <c r="C380" s="13" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="381" ht="15" spans="1:3">
-      <c r="A381" s="27"/>
-      <c r="B381" s="26"/>
-      <c r="C381" s="28" t="s">
+      <c r="A381" s="24"/>
+      <c r="B381" s="23"/>
+      <c r="C381" s="25" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="382" ht="15" spans="1:3">
-      <c r="A382" s="27"/>
-      <c r="B382" s="26"/>
+      <c r="A382" s="24"/>
+      <c r="B382" s="23"/>
       <c r="C382" s="13" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="383" ht="15" spans="1:3">
-      <c r="A383" s="27"/>
-      <c r="B383" s="26"/>
+      <c r="A383" s="24"/>
+      <c r="B383" s="23"/>
       <c r="C383" s="13" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="384" ht="15" spans="1:3">
-      <c r="A384" s="27"/>
-      <c r="B384" s="26"/>
+      <c r="A384" s="24"/>
+      <c r="B384" s="23"/>
       <c r="C384" s="13" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="385" ht="15" spans="1:3">
-      <c r="A385" s="27"/>
-      <c r="B385" s="26"/>
+      <c r="A385" s="24"/>
+      <c r="B385" s="23"/>
       <c r="C385" s="13" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="386" ht="15" spans="1:3">
-      <c r="A386" s="27"/>
-      <c r="B386" s="26"/>
+      <c r="A386" s="24"/>
+      <c r="B386" s="23"/>
       <c r="C386" s="13" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="387" ht="15" spans="1:3">
-      <c r="A387" s="27"/>
-      <c r="B387" s="26"/>
+      <c r="A387" s="24"/>
+      <c r="B387" s="23"/>
       <c r="C387" s="13" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="388" ht="15" spans="1:3">
-      <c r="A388" s="27"/>
-      <c r="B388" s="26"/>
+      <c r="A388" s="24"/>
+      <c r="B388" s="23"/>
       <c r="C388" s="13" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="389" ht="15" spans="1:3">
-      <c r="A389" s="27"/>
-      <c r="B389" s="26"/>
+      <c r="A389" s="24"/>
+      <c r="B389" s="23"/>
       <c r="C389" s="13" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="390" spans="1:3">
-      <c r="A390" s="27"/>
-      <c r="B390" s="26"/>
+      <c r="A390" s="24"/>
+      <c r="B390" s="23"/>
       <c r="C390" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="391" spans="1:3">
-      <c r="A391" s="27"/>
-      <c r="B391" s="26"/>
+      <c r="A391" s="24"/>
+      <c r="B391" s="23"/>
       <c r="C391" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="392" spans="1:3">
-      <c r="A392" s="27"/>
-      <c r="B392" s="26"/>
+      <c r="A392" s="24"/>
+      <c r="B392" s="23"/>
       <c r="C392" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="393" spans="1:3">
-      <c r="A393" s="27"/>
-      <c r="B393" s="26"/>
+      <c r="A393" s="24"/>
+      <c r="B393" s="23"/>
       <c r="C393" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="394" customFormat="1" spans="1:1">
-      <c r="A394" s="27"/>
+      <c r="A394" s="24"/>
     </row>
     <row r="395" ht="15" spans="1:3">
-      <c r="A395" s="27"/>
+      <c r="A395" s="24"/>
       <c r="B395" s="14" t="s">
         <v>22</v>
       </c>
@@ -6149,42 +6142,42 @@
       </c>
     </row>
     <row r="396" ht="15" spans="1:3">
-      <c r="A396" s="27"/>
+      <c r="A396" s="24"/>
       <c r="B396" s="14"/>
       <c r="C396" s="10" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="397" ht="15" spans="1:3">
-      <c r="A397" s="27"/>
+      <c r="A397" s="24"/>
       <c r="B397" s="14"/>
       <c r="C397" s="10" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="398" ht="15" spans="1:3">
-      <c r="A398" s="27"/>
+      <c r="A398" s="24"/>
       <c r="B398" s="14"/>
       <c r="C398" s="10" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="399" ht="15" spans="1:3">
-      <c r="A399" s="27"/>
+      <c r="A399" s="24"/>
       <c r="B399" s="14"/>
       <c r="C399" s="10" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="400" ht="15" spans="1:3">
-      <c r="A400" s="27"/>
+      <c r="A400" s="24"/>
       <c r="B400" s="14"/>
       <c r="C400" s="10" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="401" ht="15" spans="1:3">
-      <c r="A401" s="27"/>
+      <c r="A401" s="24"/>
       <c r="B401" s="14"/>
       <c r="C401" s="10" t="s">
         <v>378</v>
@@ -6203,10 +6196,10 @@
       <c r="C403" s="2"/>
     </row>
     <row r="404" ht="15" spans="1:3">
-      <c r="A404" s="29" t="s">
+      <c r="A404" s="26" t="s">
         <v>380</v>
       </c>
-      <c r="B404" s="26" t="s">
+      <c r="B404" s="23" t="s">
         <v>381</v>
       </c>
       <c r="C404" s="13" t="s">
@@ -6214,132 +6207,132 @@
       </c>
     </row>
     <row r="405" ht="15" spans="1:3">
-      <c r="A405" s="29"/>
-      <c r="B405" s="26"/>
+      <c r="A405" s="26"/>
+      <c r="B405" s="23"/>
       <c r="C405" s="13" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="406" ht="15" spans="1:3">
-      <c r="A406" s="29"/>
-      <c r="B406" s="26"/>
+      <c r="A406" s="26"/>
+      <c r="B406" s="23"/>
       <c r="C406" s="13" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="407" ht="15" spans="1:3">
-      <c r="A407" s="29"/>
-      <c r="B407" s="26"/>
+      <c r="A407" s="26"/>
+      <c r="B407" s="23"/>
       <c r="C407" s="13" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="408" ht="15" spans="1:3">
-      <c r="A408" s="29"/>
-      <c r="B408" s="26"/>
+      <c r="A408" s="26"/>
+      <c r="B408" s="23"/>
       <c r="C408" s="13" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="409" ht="15" spans="1:3">
-      <c r="A409" s="29"/>
-      <c r="B409" s="26"/>
+      <c r="A409" s="26"/>
+      <c r="B409" s="23"/>
       <c r="C409" s="13" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="410" ht="15" spans="1:3">
-      <c r="A410" s="29"/>
-      <c r="B410" s="26"/>
+      <c r="A410" s="26"/>
+      <c r="B410" s="23"/>
       <c r="C410" s="13" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="411" ht="15" spans="1:3">
-      <c r="A411" s="29"/>
-      <c r="B411" s="26"/>
+      <c r="A411" s="26"/>
+      <c r="B411" s="23"/>
       <c r="C411" s="13" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="412" ht="15" spans="1:3">
-      <c r="A412" s="29"/>
-      <c r="B412" s="26"/>
+      <c r="A412" s="26"/>
+      <c r="B412" s="23"/>
       <c r="C412" s="13" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="413" ht="15" spans="1:3">
-      <c r="A413" s="29"/>
-      <c r="B413" s="26"/>
+      <c r="A413" s="26"/>
+      <c r="B413" s="23"/>
       <c r="C413" s="13" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="414" ht="15" spans="1:3">
-      <c r="A414" s="29"/>
-      <c r="B414" s="26"/>
+      <c r="A414" s="26"/>
+      <c r="B414" s="23"/>
       <c r="C414" s="13" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="415" ht="15" spans="1:3">
-      <c r="A415" s="29"/>
-      <c r="B415" s="26"/>
+      <c r="A415" s="26"/>
+      <c r="B415" s="23"/>
       <c r="C415" s="13" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="416" ht="15" spans="1:3">
-      <c r="A416" s="29"/>
-      <c r="B416" s="26"/>
+      <c r="A416" s="26"/>
+      <c r="B416" s="23"/>
       <c r="C416" s="13" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="417" ht="15" spans="1:3">
-      <c r="A417" s="29"/>
-      <c r="B417" s="26"/>
+      <c r="A417" s="26"/>
+      <c r="B417" s="23"/>
       <c r="C417" s="13" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="418" ht="15" spans="1:3">
-      <c r="A418" s="29"/>
-      <c r="B418" s="26"/>
+      <c r="A418" s="26"/>
+      <c r="B418" s="23"/>
       <c r="C418" s="13" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="419" ht="15" spans="1:3">
-      <c r="A419" s="29"/>
-      <c r="B419" s="26"/>
+      <c r="A419" s="26"/>
+      <c r="B419" s="23"/>
       <c r="C419" s="13" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="420" ht="15" spans="1:3">
-      <c r="A420" s="29"/>
-      <c r="B420" s="26"/>
+      <c r="A420" s="26"/>
+      <c r="B420" s="23"/>
       <c r="C420" s="13" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="421" ht="15" spans="1:3">
-      <c r="A421" s="29"/>
-      <c r="B421" s="26"/>
+      <c r="A421" s="26"/>
+      <c r="B421" s="23"/>
       <c r="C421" s="13" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="422" ht="18" spans="1:3">
-      <c r="A422" s="29"/>
-      <c r="B422" s="26"/>
+      <c r="A422" s="26"/>
+      <c r="B422" s="23"/>
       <c r="C422" s="13"/>
     </row>
     <row r="423" ht="15" spans="1:3">
-      <c r="A423" s="29"/>
-      <c r="B423" s="26" t="s">
+      <c r="A423" s="26"/>
+      <c r="B423" s="23" t="s">
         <v>399</v>
       </c>
       <c r="C423" s="13" t="s">
@@ -6347,125 +6340,125 @@
       </c>
     </row>
     <row r="424" ht="15" spans="1:3">
-      <c r="A424" s="29"/>
-      <c r="B424" s="26"/>
+      <c r="A424" s="26"/>
+      <c r="B424" s="23"/>
       <c r="C424" s="13" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="425" ht="15" spans="1:3">
-      <c r="A425" s="29"/>
-      <c r="B425" s="26"/>
+      <c r="A425" s="26"/>
+      <c r="B425" s="23"/>
       <c r="C425" s="13" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="426" ht="15" spans="1:3">
-      <c r="A426" s="29"/>
-      <c r="B426" s="26"/>
+      <c r="A426" s="26"/>
+      <c r="B426" s="23"/>
       <c r="C426" s="13" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="427" ht="15" spans="1:3">
-      <c r="A427" s="29"/>
-      <c r="B427" s="26"/>
+      <c r="A427" s="26"/>
+      <c r="B427" s="23"/>
       <c r="C427" s="13" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="428" ht="15" spans="1:3">
-      <c r="A428" s="29"/>
-      <c r="B428" s="26"/>
+      <c r="A428" s="26"/>
+      <c r="B428" s="23"/>
       <c r="C428" s="13" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="429" ht="15" spans="1:3">
-      <c r="A429" s="29"/>
-      <c r="B429" s="26"/>
+      <c r="A429" s="26"/>
+      <c r="B429" s="23"/>
       <c r="C429" s="13" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="430" ht="15" spans="1:3">
-      <c r="A430" s="29"/>
-      <c r="B430" s="26"/>
+      <c r="A430" s="26"/>
+      <c r="B430" s="23"/>
       <c r="C430" s="13" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="431" ht="15" spans="1:3">
-      <c r="A431" s="29"/>
-      <c r="B431" s="26"/>
+      <c r="A431" s="26"/>
+      <c r="B431" s="23"/>
       <c r="C431" s="13" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="432" ht="15" spans="1:3">
-      <c r="A432" s="29"/>
-      <c r="B432" s="26"/>
+      <c r="A432" s="26"/>
+      <c r="B432" s="23"/>
       <c r="C432" s="13" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="433" ht="15" spans="1:3">
-      <c r="A433" s="29"/>
-      <c r="B433" s="26"/>
+      <c r="A433" s="26"/>
+      <c r="B433" s="23"/>
       <c r="C433" s="13" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="434" ht="15" spans="1:3">
-      <c r="A434" s="29"/>
-      <c r="B434" s="26"/>
+      <c r="A434" s="26"/>
+      <c r="B434" s="23"/>
       <c r="C434" s="13" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="435" ht="15" spans="1:3">
-      <c r="A435" s="29"/>
-      <c r="B435" s="26"/>
+      <c r="A435" s="26"/>
+      <c r="B435" s="23"/>
       <c r="C435" s="13" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="436" ht="15" spans="1:3">
-      <c r="A436" s="29"/>
-      <c r="B436" s="26"/>
+      <c r="A436" s="26"/>
+      <c r="B436" s="23"/>
       <c r="C436" s="13" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="437" ht="15" spans="1:3">
-      <c r="A437" s="29"/>
-      <c r="B437" s="26"/>
+      <c r="A437" s="26"/>
+      <c r="B437" s="23"/>
       <c r="C437" s="13" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="438" ht="15" spans="1:3">
-      <c r="A438" s="29"/>
-      <c r="B438" s="26"/>
+      <c r="A438" s="26"/>
+      <c r="B438" s="23"/>
       <c r="C438" s="13" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="439" ht="15" spans="1:3">
-      <c r="A439" s="29"/>
-      <c r="B439" s="26"/>
+      <c r="A439" s="26"/>
+      <c r="B439" s="23"/>
       <c r="C439" s="13" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="440" ht="18" spans="1:3">
-      <c r="A440" s="29"/>
-      <c r="B440" s="26"/>
+      <c r="A440" s="26"/>
+      <c r="B440" s="23"/>
       <c r="C440" s="13"/>
     </row>
     <row r="441" ht="15" spans="1:3">
-      <c r="A441" s="29"/>
-      <c r="B441" s="26" t="s">
+      <c r="A441" s="26"/>
+      <c r="B441" s="23" t="s">
         <v>416</v>
       </c>
       <c r="C441" s="13" t="s">
@@ -6473,75 +6466,75 @@
       </c>
     </row>
     <row r="442" ht="15" spans="1:3">
-      <c r="A442" s="29"/>
-      <c r="B442" s="26"/>
+      <c r="A442" s="26"/>
+      <c r="B442" s="23"/>
       <c r="C442" s="13" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="443" ht="15" spans="1:3">
-      <c r="A443" s="29"/>
-      <c r="B443" s="26"/>
+      <c r="A443" s="26"/>
+      <c r="B443" s="23"/>
       <c r="C443" s="13" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="444" ht="15" spans="1:3">
-      <c r="A444" s="29"/>
-      <c r="B444" s="26"/>
+      <c r="A444" s="26"/>
+      <c r="B444" s="23"/>
       <c r="C444" s="13" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="445" ht="15" spans="1:3">
-      <c r="A445" s="29"/>
-      <c r="B445" s="26"/>
+      <c r="A445" s="26"/>
+      <c r="B445" s="23"/>
       <c r="C445" s="13" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="446" ht="15" spans="1:3">
-      <c r="A446" s="29"/>
-      <c r="B446" s="26"/>
+      <c r="A446" s="26"/>
+      <c r="B446" s="23"/>
       <c r="C446" s="13" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="447" ht="15" spans="1:3">
-      <c r="A447" s="29"/>
-      <c r="B447" s="26"/>
+      <c r="A447" s="26"/>
+      <c r="B447" s="23"/>
       <c r="C447" s="13" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="448" ht="15" spans="1:3">
-      <c r="A448" s="29"/>
-      <c r="B448" s="26"/>
+      <c r="A448" s="26"/>
+      <c r="B448" s="23"/>
       <c r="C448" s="13" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="449" ht="15" spans="1:3">
-      <c r="A449" s="29"/>
-      <c r="B449" s="26"/>
+      <c r="A449" s="26"/>
+      <c r="B449" s="23"/>
       <c r="C449" s="13" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="450" ht="15" spans="1:3">
-      <c r="A450" s="29"/>
-      <c r="B450" s="26"/>
+      <c r="A450" s="26"/>
+      <c r="B450" s="23"/>
       <c r="C450" s="13" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="451" ht="18" spans="1:3">
-      <c r="A451" s="29"/>
-      <c r="B451" s="30"/>
+      <c r="A451" s="26"/>
+      <c r="B451" s="27"/>
       <c r="C451" s="13"/>
     </row>
     <row r="452" ht="15" spans="1:3">
-      <c r="A452" s="29"/>
+      <c r="A452" s="26"/>
       <c r="B452" s="14" t="s">
         <v>22</v>
       </c>
@@ -6550,58 +6543,58 @@
       </c>
     </row>
     <row r="453" ht="15" spans="1:3">
-      <c r="A453" s="29"/>
+      <c r="A453" s="26"/>
       <c r="B453" s="14"/>
       <c r="C453" s="10" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="454" ht="15" spans="1:3">
-      <c r="A454" s="29"/>
+      <c r="A454" s="26"/>
       <c r="B454" s="14"/>
       <c r="C454" s="15" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="455" ht="15" spans="1:3">
-      <c r="A455" s="29"/>
+      <c r="A455" s="26"/>
       <c r="B455" s="14"/>
       <c r="C455" s="10" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="456" ht="15" spans="1:3">
-      <c r="A456" s="29"/>
+      <c r="A456" s="26"/>
       <c r="B456" s="14"/>
       <c r="C456" s="15" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="457" ht="15" spans="1:3">
-      <c r="A457" s="29"/>
+      <c r="A457" s="26"/>
       <c r="B457" s="14"/>
       <c r="C457" s="10" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="458" spans="1:3">
-      <c r="A458" s="31"/>
-      <c r="B458" s="31"/>
-      <c r="C458" s="31"/>
+      <c r="A458" s="28"/>
+      <c r="B458" s="28"/>
+      <c r="C458" s="28"/>
     </row>
     <row r="571" ht="18.75" spans="1:2">
-      <c r="A571" s="32" t="s">
+      <c r="A571" s="29" t="s">
         <v>431</v>
       </c>
-      <c r="B571" s="33">
+      <c r="B571" s="30">
         <v>10.5</v>
       </c>
     </row>
     <row r="572" ht="18.75" spans="1:2">
-      <c r="A572" s="32" t="s">
+      <c r="A572" s="29" t="s">
         <v>432</v>
       </c>
-      <c r="B572" s="33">
+      <c r="B572" s="30">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
uploaded Course MAterials - Day 10.
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="22" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="472">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -1670,6 +1670,146 @@
     <t>Hands On Exercises - Stream API and Collectors II</t>
   </si>
   <si>
+    <t>Day 10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Advanced Java Concurrent Patterns.                                                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Advanced fundamentals you'll need to understand to write efficient concurrent applications, that support heavy concurrency and provide high throughput.                                                     Learn about how you can improve the quality of your concurrent code, by using sophisticated concurrent tools that allow for smooth lock acquisition and fault tolerance.                              Get introduced to advanced data structures, such as the copy on write arrays, the concurrent blocking queues, the concurrent skip lists and concurrent hashmaps.               </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                    </t>
+    </r>
+  </si>
+  <si>
+    <t>2. Leveraging Concurrent Collections to Simplify Application Design</t>
+  </si>
+  <si>
+    <t>1. Introduction, Module Agenda</t>
+  </si>
+  <si>
+    <t>2. Implementing Concurrency at the API Level</t>
+  </si>
+  <si>
+    <t>3. Hierarchy of Collection and Map, Concurrent Interfaces</t>
+  </si>
+  <si>
+    <t>4. What Does It Mean for an Interface to Be Concurrent?</t>
+  </si>
+  <si>
+    <t>5. Why You Should Avoid Vectors and Stacks</t>
+  </si>
+  <si>
+    <t>6. Understanding Copy On Write Arrays</t>
+  </si>
+  <si>
+    <t>7. Wrapping up CopyOnWriteArrayList</t>
+  </si>
+  <si>
+    <t>8.  Introducing Queue and Deque, and Their Implementation</t>
+  </si>
+  <si>
+    <t>9. Understanding How Queue Works in a Concurrent Environment</t>
+  </si>
+  <si>
+    <t>10. Adding Elements to a Queue That Is Full: How Can It Fail?</t>
+  </si>
+  <si>
+    <t>11. Understanding Error Handling in Queue and Deque</t>
+  </si>
+  <si>
+    <t>12. Wrapping up Queue, Deque, and Their Blocking Versions</t>
+  </si>
+  <si>
+    <t>13.  Introducing Concurrent Maps and Their Implementations</t>
+  </si>
+  <si>
+    <t>14. Atomic Operations Defined by the ConcurrentMap Interface</t>
+  </si>
+  <si>
+    <t>15. Understanding Concurrency for a HashMap</t>
+  </si>
+  <si>
+    <t>16. Understanding the Structure of the ConcurrentHashMap from Java 7</t>
+  </si>
+  <si>
+    <t>17. Introducing the Java 8 ConcurrentHashMap and Its Parallel Methods</t>
+  </si>
+  <si>
+    <t>18. Parallel Search on a Java 8 ConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>19. Parallel Map / Reduce on a Java 8 ConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>20. Parallel ForEach on a Java 8 ConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>21. Creating a Concurrent Set on a Java 8 ConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>22. Wrapping up the Java 8 ConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>23. Introducing Skip Lists to Implement ConcurrentMap</t>
+  </si>
+  <si>
+    <t>24. Understanding How Linked Lists Can Be Improved by Skip Lists</t>
+  </si>
+  <si>
+    <t>25. Wrapping up the Skip List Structure</t>
+  </si>
+  <si>
+    <t>26. How to Make a Skip List Concurrent Without Synchronization</t>
+  </si>
+  <si>
+    <t>27. Wrapping up ConcurrentSkipList</t>
+  </si>
+  <si>
+    <t>28. Live Coding: Producer / Consumer Built on an ArrayBlockingQueue</t>
+  </si>
+  <si>
+    <t>29. Live Coding: Parallel Reduce in Action on a ConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>30. Live Coding: Parallel Search in Action on a ConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>31. Live Coding: Computing an Average on a ConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>32. Live Coding Wrap-up</t>
+  </si>
+  <si>
+    <t>33. Module Wrap-up</t>
+  </si>
+  <si>
+    <t>34. Course Wrap-up</t>
+  </si>
+  <si>
+    <t>Java 8 Advanced Concurrent Patterns</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - Java 8 Advanced Concurrent Patterns</t>
+  </si>
+  <si>
     <t>Total # of Days for Core Java 8</t>
   </si>
   <si>
@@ -1682,9 +1822,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -1806,8 +1946,23 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1822,14 +1977,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1843,23 +2006,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1874,17 +2045,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1905,29 +2069,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1935,9 +2076,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2002,7 +2142,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2014,7 +2160,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2026,31 +2250,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2062,13 +2268,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2080,109 +2316,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2291,6 +2431,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2315,15 +2499,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2338,186 +2513,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2977,7 +3117,7 @@
   <sheetPr/>
   <dimension ref="A7:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B37" sqref="B37:F40"/>
     </sheetView>
   </sheetViews>
@@ -3367,19 +3507,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C572"/>
+  <dimension ref="A1:C502"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A393" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A452" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F309" sqref="F309"/>
+      <selection pane="bottomLeft" activeCell="E471" sqref="E471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="38.625" customWidth="1"/>
     <col min="2" max="2" width="35.125" customWidth="1"/>
-    <col min="3" max="3" width="55.125" customWidth="1"/>
+    <col min="3" max="3" width="67.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" spans="1:3">
@@ -6582,24 +6722,312 @@
       <c r="B458" s="28"/>
       <c r="C458" s="28"/>
     </row>
-    <row r="571" ht="18.75" spans="1:2">
-      <c r="A571" s="29" t="s">
+    <row r="459" ht="24.75" spans="1:3">
+      <c r="A459" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B571" s="30">
+      <c r="B459" s="2"/>
+      <c r="C459" s="2"/>
+    </row>
+    <row r="460" ht="15.75" spans="1:3">
+      <c r="A460" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B460" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C460" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="461" ht="12" customHeight="1" spans="1:3">
+      <c r="A461" s="3"/>
+      <c r="B461" s="4"/>
+      <c r="C461" s="5"/>
+    </row>
+    <row r="462" ht="16" customHeight="1" spans="1:3">
+      <c r="A462" s="3"/>
+      <c r="B462" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="C462" s="10" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="463" ht="20" customHeight="1" spans="1:3">
+      <c r="A463" s="3"/>
+      <c r="B463" s="7"/>
+      <c r="C463" s="10" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="464" ht="15" spans="1:3">
+      <c r="A464" s="3"/>
+      <c r="B464" s="7"/>
+      <c r="C464" s="10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="465" ht="21" customHeight="1" spans="1:3">
+      <c r="A465" s="3"/>
+      <c r="B465" s="7"/>
+      <c r="C465" s="10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="466" ht="15" customHeight="1" spans="1:3">
+      <c r="A466" s="3"/>
+      <c r="B466" s="7"/>
+      <c r="C466" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="467" ht="15" spans="1:3">
+      <c r="A467" s="3"/>
+      <c r="B467" s="7"/>
+      <c r="C467" s="10" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="468" ht="17" customHeight="1" spans="1:3">
+      <c r="A468" s="3"/>
+      <c r="B468" s="7"/>
+      <c r="C468" s="10" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="469" ht="13" customHeight="1" spans="1:3">
+      <c r="A469" s="3"/>
+      <c r="B469" s="7"/>
+      <c r="C469" s="10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="470" ht="13" customHeight="1" spans="1:3">
+      <c r="A470" s="3"/>
+      <c r="B470" s="7"/>
+      <c r="C470" s="10" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="471" ht="15" spans="1:3">
+      <c r="A471" s="3"/>
+      <c r="B471" s="7"/>
+      <c r="C471" s="10" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="472" ht="15" spans="1:3">
+      <c r="A472" s="3"/>
+      <c r="B472" s="7"/>
+      <c r="C472" s="10" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="473" ht="15" spans="1:3">
+      <c r="A473" s="3"/>
+      <c r="B473" s="7"/>
+      <c r="C473" s="10" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="474" ht="15" spans="1:3">
+      <c r="A474" s="3"/>
+      <c r="B474" s="7"/>
+      <c r="C474" s="10" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="475" ht="15" spans="1:3">
+      <c r="A475" s="3"/>
+      <c r="B475" s="7"/>
+      <c r="C475" s="10" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="476" ht="15" spans="1:3">
+      <c r="A476" s="3"/>
+      <c r="B476" s="7"/>
+      <c r="C476" s="10" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="477" ht="15" customHeight="1" spans="1:3">
+      <c r="A477" s="3"/>
+      <c r="B477" s="7"/>
+      <c r="C477" s="10" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="478" ht="15" spans="1:3">
+      <c r="A478" s="3"/>
+      <c r="B478" s="7"/>
+      <c r="C478" s="10" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="479" ht="15" spans="1:3">
+      <c r="A479" s="3"/>
+      <c r="B479" s="7"/>
+      <c r="C479" s="10" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="480" ht="15" spans="1:3">
+      <c r="A480" s="3"/>
+      <c r="B480" s="7"/>
+      <c r="C480" s="10" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="481" ht="18" customHeight="1" spans="1:3">
+      <c r="A481" s="3"/>
+      <c r="B481" s="7"/>
+      <c r="C481" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="482" ht="18" customHeight="1" spans="1:3">
+      <c r="A482" s="3"/>
+      <c r="B482" s="7"/>
+      <c r="C482" s="10" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="483" ht="18" customHeight="1" spans="1:3">
+      <c r="A483" s="3"/>
+      <c r="B483" s="7"/>
+      <c r="C483" s="10" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="484" ht="16" customHeight="1" spans="1:3">
+      <c r="A484" s="3"/>
+      <c r="B484" s="7"/>
+      <c r="C484" s="10" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="485" ht="16" customHeight="1" spans="1:3">
+      <c r="A485" s="3"/>
+      <c r="B485" s="7"/>
+      <c r="C485" s="10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="486" ht="16" customHeight="1" spans="1:3">
+      <c r="A486" s="3"/>
+      <c r="B486" s="7"/>
+      <c r="C486" s="10" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="487" ht="16" customHeight="1" spans="1:3">
+      <c r="A487" s="3"/>
+      <c r="B487" s="7"/>
+      <c r="C487" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="488" ht="16" customHeight="1" spans="1:3">
+      <c r="A488" s="3"/>
+      <c r="B488" s="7"/>
+      <c r="C488" s="10" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="489" ht="16" customHeight="1" spans="1:3">
+      <c r="A489" s="3"/>
+      <c r="B489" s="7"/>
+      <c r="C489" s="10" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="490" ht="16" customHeight="1" spans="1:3">
+      <c r="A490" s="3"/>
+      <c r="B490" s="7"/>
+      <c r="C490" s="10" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="491" ht="16" customHeight="1" spans="1:3">
+      <c r="A491" s="3"/>
+      <c r="B491" s="7"/>
+      <c r="C491" s="10" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="492" ht="16" customHeight="1" spans="1:3">
+      <c r="A492" s="3"/>
+      <c r="B492" s="7"/>
+      <c r="C492" s="10" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="493" ht="16" customHeight="1" spans="1:3">
+      <c r="A493" s="3"/>
+      <c r="B493" s="7"/>
+      <c r="C493" s="10" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="494" ht="16" customHeight="1" spans="1:3">
+      <c r="A494" s="3"/>
+      <c r="B494" s="7"/>
+      <c r="C494" s="10" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="495" ht="16" customHeight="1" spans="1:3">
+      <c r="A495" s="3"/>
+      <c r="B495" s="7"/>
+      <c r="C495" s="10" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="496" customFormat="1" ht="15.75" spans="1:2">
+      <c r="A496" s="3"/>
+      <c r="B496" s="7"/>
+    </row>
+    <row r="497" ht="15" spans="1:3">
+      <c r="A497" s="3"/>
+      <c r="B497" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C497" s="15" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="498" ht="15" spans="1:3">
+      <c r="A498" s="3"/>
+      <c r="B498" s="14"/>
+      <c r="C498" s="10" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="499" ht="9" customHeight="1" spans="1:3">
+      <c r="A499" s="18"/>
+      <c r="B499" s="16"/>
+      <c r="C499" s="16"/>
+    </row>
+    <row r="501" ht="18.75" spans="1:2">
+      <c r="A501" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="B501" s="30">
         <v>10.5</v>
       </c>
     </row>
-    <row r="572" ht="18.75" spans="1:2">
-      <c r="A572" s="29" t="s">
-        <v>432</v>
-      </c>
-      <c r="B572" s="30">
+    <row r="502" ht="18.75" spans="1:2">
+      <c r="A502" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="B502" s="30">
         <v>84</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="79">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A51:C51"/>
     <mergeCell ref="A100:C100"/>
@@ -6609,6 +7037,7 @@
     <mergeCell ref="A307:C307"/>
     <mergeCell ref="A337:C337"/>
     <mergeCell ref="A403:C403"/>
+    <mergeCell ref="A459:C459"/>
     <mergeCell ref="A3:A14"/>
     <mergeCell ref="A16:A24"/>
     <mergeCell ref="A26:A35"/>
@@ -6625,6 +7054,7 @@
     <mergeCell ref="A359:A368"/>
     <mergeCell ref="A370:A401"/>
     <mergeCell ref="A404:A457"/>
+    <mergeCell ref="A460:A498"/>
     <mergeCell ref="B5:B14"/>
     <mergeCell ref="B16:B24"/>
     <mergeCell ref="B26:B35"/>
@@ -6675,6 +7105,8 @@
     <mergeCell ref="B423:B439"/>
     <mergeCell ref="B441:B450"/>
     <mergeCell ref="B452:B457"/>
+    <mergeCell ref="B462:B495"/>
+    <mergeCell ref="B497:B498"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C405" r:id="rId1" display="2. Module Outline"/>

</xml_diff>

<commit_message>
Added Course Materials - Day 12
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="556">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -2012,6 +2012,9 @@
     <t>Total # of Hours for Core Java 8</t>
   </si>
   <si>
+    <t>Day 12</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -2139,8 +2142,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -2265,15 +2268,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2286,30 +2296,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2318,22 +2306,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2349,14 +2321,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2372,25 +2336,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2402,7 +2351,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2460,7 +2463,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2472,13 +2559,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2490,85 +2607,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2580,43 +2619,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2634,13 +2643,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2736,11 +2739,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2749,16 +2765,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2778,17 +2785,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2808,41 +2809,43 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2852,130 +2855,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7841,9 +7844,9 @@
   <dimension ref="A1:C159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -7866,14 +7869,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>470</v>
+        <v>521</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>36</v>
@@ -7890,31 +7893,31 @@
     <row r="5" ht="19" customHeight="1" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="7" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="9" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="9" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:3">
@@ -7925,31 +7928,31 @@
     <row r="10" ht="18" customHeight="1" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="7" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="11" ht="16" customHeight="1" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="10" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="12" ht="17" customHeight="1" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="10" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="11" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
@@ -7967,59 +7970,59 @@
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="12" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="12" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="12" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="12" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="12" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="12" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="12" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="1:3">
@@ -8030,59 +8033,59 @@
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="7" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="12" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="12" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="12" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="12" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="12" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="12" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="33" ht="12" customHeight="1" spans="1:3">
@@ -8093,31 +8096,31 @@
     <row r="34" ht="16" customHeight="1" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="7" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1" spans="1:3">
       <c r="A35" s="3"/>
       <c r="B35" s="7"/>
       <c r="C35" s="10" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="7"/>
       <c r="C36" s="10" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="37" ht="21" customHeight="1" spans="1:3">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="9" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" spans="1:3">
@@ -8138,7 +8141,7 @@
         <v>149</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="41" customFormat="1" ht="15.75" spans="1:2">
@@ -8151,14 +8154,14 @@
         <v>22</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="3"/>
       <c r="B43" s="14"/>
       <c r="C43" s="10" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="44" ht="9" customHeight="1" spans="1:3">
@@ -8168,7 +8171,7 @@
     </row>
     <row r="158" ht="18.75" spans="1:2">
       <c r="A158" s="18" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B158" s="19">
         <v>2</v>
@@ -8176,7 +8179,7 @@
     </row>
     <row r="159" ht="18.75" spans="1:2">
       <c r="A159" s="18" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B159" s="19">
         <v>16</v>

</xml_diff>

<commit_message>
Added Course Materials - Day 13 and 14
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="610">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -2129,21 +2129,19 @@
     <t>PostgreSQL Queries</t>
   </si>
   <si>
-    <t>Hands On Exercises - PostgreSQL Basic Queries</t>
+    <t>1.  Hands On Exercises - PostgreSQL Basic Queries</t>
+  </si>
+  <si>
+    <t>2. Hands On Exercises - PostgreSQL  Joins and Subqueries</t>
+  </si>
+  <si>
+    <t>3. Hands On Exercises - PostgreSQL  Aggregation</t>
   </si>
   <si>
     <t>Day 13</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">PostgreSQL is commonly known as Postgres and is is often referred to as a the world's most advanced open source database.                                                    </t>
     </r>
     <r>
@@ -2154,130 +2152,130 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">In this course, we will go over the basics of  DML, DDL and TCL PostgreSQL commands.                                                                Learn how to restore a database from a tar file.                                                 Understand the basic Data Types in PostgreSQL and how to use Array Functions and Operators.         </t>
+      <t>In this course, we will go over the basics of  DML, DDL and TCL PostgreSQL commands.                                                                Learn how to restore a database from a tar file.                                                 Understand the basic Data Types in PostgreSQL and how to use Array Functions and Operators.</t>
     </r>
+  </si>
+  <si>
+    <t>1. PostgreSQL Data Operations - Insert, Update, Delete</t>
+  </si>
+  <si>
+    <t>1. Loading Sample Data</t>
+  </si>
+  <si>
+    <t>2. Getting Started</t>
+  </si>
+  <si>
+    <t>3. Scenario 1 Task 1: Update Table With New Data</t>
+  </si>
+  <si>
+    <t>4. Scenario 1 Task 2: Insert Data Into Table</t>
+  </si>
+  <si>
+    <t>5. Scenario 4: Delete Rows From Table</t>
+  </si>
+  <si>
+    <t>2. Data Types in PostgreSQL</t>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Date/Time</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>3. Arrays Functions and Operators</t>
+  </si>
+  <si>
+    <t>2. Array  Operators</t>
+  </si>
+  <si>
+    <t>3. Array Functions</t>
+  </si>
+  <si>
+    <t>4. Demo : Array Functions and Operators</t>
+  </si>
+  <si>
+    <t>4. PostgreSQL DDL, Transactions and Constraints</t>
+  </si>
+  <si>
+    <t>1. Data Definition (DDL) Commands</t>
+  </si>
+  <si>
+    <t>CREATE  Database</t>
+  </si>
+  <si>
+    <t>CREATE  Table</t>
+  </si>
+  <si>
+    <t>ALTER</t>
+  </si>
+  <si>
+    <t>DROP</t>
+  </si>
+  <si>
+    <t>TRUNCATE</t>
+  </si>
+  <si>
+    <t>RENAME</t>
+  </si>
+  <si>
+    <t>2. Transaction Control (TCL) Commands</t>
+  </si>
+  <si>
+    <t>BEGIN</t>
+  </si>
+  <si>
+    <t>COMMIT</t>
+  </si>
+  <si>
+    <t>ROLLBACK</t>
+  </si>
+  <si>
+    <t>3. Constraints Used In Database</t>
+  </si>
+  <si>
+    <t>NOT NULL Constraint</t>
+  </si>
+  <si>
+    <t>UNIQUE Constraint</t>
+  </si>
+  <si>
+    <t>CHECK Constraint</t>
+  </si>
+  <si>
+    <t>Hands On Exercises - PostgreSQL Modifying data</t>
+  </si>
+  <si>
+    <t>Total # of Days for PostgreSQL</t>
+  </si>
+  <si>
+    <t>Total # of Hours for PostgreSQL</t>
+  </si>
+  <si>
+    <t>Total # of Days for JPA with Hibernate</t>
+  </si>
+  <si>
+    <t>Total # of Hours for JPA with Hibernate</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="14"/>
+        <sz val="10"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-  </si>
-  <si>
-    <t>1. PostgreSQL Data Operations - Insert, Update, Delete</t>
-  </si>
-  <si>
-    <t>1. Loading Sample Data</t>
-  </si>
-  <si>
-    <t>2. Getting Started</t>
-  </si>
-  <si>
-    <t>3. Scenario 1 Task 1: Update Table With New Data</t>
-  </si>
-  <si>
-    <t>4. Scenario 1 Task 2: Insert Data Into Table</t>
-  </si>
-  <si>
-    <t>5. Scenario 4: Delete Rows From Table</t>
-  </si>
-  <si>
-    <t>2. Data Types in PostgreSQL</t>
-  </si>
-  <si>
-    <t>Character</t>
-  </si>
-  <si>
-    <t>Numeric</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Date/Time</t>
-  </si>
-  <si>
-    <t>Array</t>
-  </si>
-  <si>
-    <t>3. Arrays Functions and Operators</t>
-  </si>
-  <si>
-    <t>2. Array  Operators</t>
-  </si>
-  <si>
-    <t>3. Array Functions</t>
-  </si>
-  <si>
-    <t>4. Demo : Array Functions and Operators</t>
-  </si>
-  <si>
-    <t>4. PostgreSQL DDL, Transactions and Constraints</t>
-  </si>
-  <si>
-    <t>1. Data Definition (DDL) Commands</t>
-  </si>
-  <si>
-    <t>CREATE  Database</t>
-  </si>
-  <si>
-    <t>CREATE  Table</t>
-  </si>
-  <si>
-    <t>ALTER</t>
-  </si>
-  <si>
-    <t>DROP</t>
-  </si>
-  <si>
-    <t>TRUNCATE</t>
-  </si>
-  <si>
-    <t>RENAME</t>
-  </si>
-  <si>
-    <t>2. Transaction Control (TCL) Commands</t>
-  </si>
-  <si>
-    <t>BEGIN</t>
-  </si>
-  <si>
-    <t>COMMIT</t>
-  </si>
-  <si>
-    <t>ROLLBACK</t>
-  </si>
-  <si>
-    <t>3. Constraints Used In Database</t>
-  </si>
-  <si>
-    <t>NOT NULL Constraint</t>
-  </si>
-  <si>
-    <t>UNIQUE Constraint</t>
-  </si>
-  <si>
-    <t>CHECK Constraint</t>
-  </si>
-  <si>
-    <t>Total # of Days for PostgreSQL</t>
-  </si>
-  <si>
-    <t>Total # of Hours for PostgreSQL</t>
-  </si>
-  <si>
-    <t>Total # of Days for JPA with Hibernate</t>
-  </si>
-  <si>
-    <t>Total # of Hours for JPA with Hibernate</t>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">DevOps may not mean the same thing to everyone you ask but there are a set of principles that can be distilled.                                                                                                  </t>
     </r>
     <r>
@@ -2339,10 +2337,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -2472,6 +2470,37 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2480,7 +2509,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2494,16 +2538,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2517,9 +2553,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2534,35 +2570,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -2570,9 +2577,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2586,14 +2593,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -2601,16 +2600,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2675,7 +2673,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2687,19 +2727,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2711,7 +2739,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2723,7 +2751,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2735,121 +2841,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2949,30 +2947,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2992,33 +2966,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3042,22 +2999,63 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -3067,130 +3065,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -8065,12 +8063,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C159"/>
+  <dimension ref="A1:C162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -8388,67 +8386,69 @@
         <v>553</v>
       </c>
     </row>
-    <row r="44" ht="9" customHeight="1" spans="1:3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-    </row>
-    <row r="45" ht="24.75" spans="1:3">
-      <c r="A45" s="2" t="s">
+    <row r="44" ht="18.75" spans="1:3">
+      <c r="A44" s="16"/>
+      <c r="B44" s="22"/>
+      <c r="C44" t="s">
         <v>554</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" ht="15" spans="1:3">
-      <c r="A46" s="16" t="s">
+    </row>
+    <row r="45" ht="18.75" spans="1:3">
+      <c r="A45" s="16"/>
+      <c r="B45" s="22"/>
+      <c r="C45" t="s">
         <v>555</v>
       </c>
-      <c r="B46" s="4" t="s">
+    </row>
+    <row r="46" ht="9" customHeight="1" spans="1:3">
+      <c r="A46" s="12"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" ht="24.75" spans="1:3">
+      <c r="A47" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="C46" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" ht="24.75" spans="1:3">
-      <c r="A47" s="16"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="19"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" ht="15" spans="1:3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="4"/>
+      <c r="A48" s="16" t="s">
+        <v>557</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>558</v>
+      </c>
       <c r="C48" s="18" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="16"/>
       <c r="B49" s="4"/>
       <c r="C49" s="20" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="16"/>
       <c r="B50" s="4"/>
       <c r="C50" s="9" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="16"/>
       <c r="B51" s="4"/>
       <c r="C51" s="9" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="16"/>
       <c r="B52" s="4"/>
       <c r="C52" s="10" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
@@ -8466,7 +8466,7 @@
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="16"/>
       <c r="B55" s="4" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>73</v>
@@ -8476,42 +8476,42 @@
       <c r="A56" s="16"/>
       <c r="B56" s="4"/>
       <c r="C56" s="11" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="16"/>
       <c r="B57" s="4"/>
       <c r="C57" s="11" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
       <c r="A58" s="16"/>
       <c r="B58" s="4"/>
       <c r="C58" s="11" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="59" ht="15" spans="1:3">
       <c r="A59" s="16"/>
       <c r="B59" s="4"/>
       <c r="C59" s="11" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="16"/>
       <c r="B60" s="4"/>
       <c r="C60" s="11" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="16"/>
       <c r="B61" s="4"/>
       <c r="C61" s="11" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="62" ht="15.75" spans="1:3">
@@ -8522,7 +8522,7 @@
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="16"/>
       <c r="B63" s="4" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>524</v>
@@ -8532,21 +8532,21 @@
       <c r="A64" s="16"/>
       <c r="B64" s="4"/>
       <c r="C64" s="11" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:3">
       <c r="A65" s="16"/>
       <c r="B65" s="4"/>
       <c r="C65" s="11" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:3">
       <c r="A66" s="16"/>
       <c r="B66" s="4"/>
       <c r="C66" s="11" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="67" ht="15.75" spans="1:3">
@@ -8557,163 +8557,185 @@
     <row r="68" ht="15" spans="1:3">
       <c r="A68" s="16"/>
       <c r="B68" s="4" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:3">
       <c r="A69" s="16"/>
       <c r="B69" s="4"/>
       <c r="C69" s="11" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:3">
       <c r="A70" s="16"/>
       <c r="B70" s="4"/>
       <c r="C70" s="11" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="71" ht="15" spans="1:3">
       <c r="A71" s="16"/>
       <c r="B71" s="4"/>
       <c r="C71" s="11" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="72" ht="15" spans="1:3">
       <c r="A72" s="16"/>
       <c r="B72" s="4"/>
       <c r="C72" s="11" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="73" ht="15" spans="1:3">
       <c r="A73" s="16"/>
       <c r="B73" s="4"/>
       <c r="C73" s="11" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:3">
       <c r="A74" s="16"/>
       <c r="B74" s="4"/>
       <c r="C74" s="11" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="75" ht="15" spans="1:3">
       <c r="A75" s="16"/>
       <c r="B75" s="4"/>
       <c r="C75" s="24" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="76" ht="15" spans="1:3">
       <c r="A76" s="16"/>
       <c r="B76" s="4"/>
       <c r="C76" s="24" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="77" ht="15" spans="1:3">
       <c r="A77" s="16"/>
       <c r="B77" s="4"/>
       <c r="C77" s="24" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="78" ht="15" spans="1:3">
       <c r="A78" s="16"/>
       <c r="B78" s="4"/>
       <c r="C78" s="24" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="79" ht="15" spans="1:3">
       <c r="A79" s="16"/>
       <c r="B79" s="4"/>
       <c r="C79" s="24" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="80" ht="15" spans="1:3">
       <c r="A80" s="16"/>
       <c r="B80" s="4"/>
       <c r="C80" s="24" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="81" ht="15" spans="1:3">
       <c r="A81" s="16"/>
       <c r="B81" s="4"/>
       <c r="C81" s="24" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="82" ht="15" spans="1:3">
       <c r="A82" s="16"/>
       <c r="B82" s="4"/>
       <c r="C82" s="24" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="83" ht="18" spans="1:3">
-      <c r="A83" s="12"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-    </row>
-    <row r="85" ht="18.75" spans="1:2">
-      <c r="A85" s="14" t="s">
-        <v>588</v>
-      </c>
-      <c r="B85" s="15">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="83" ht="15.75" spans="1:3">
+      <c r="A83" s="16"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="24"/>
+    </row>
+    <row r="84" ht="15" spans="1:3">
+      <c r="A84" s="16"/>
+      <c r="B84" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="23" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="85" ht="15" spans="1:3">
+      <c r="A85" s="16"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="10" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="86" ht="10" customHeight="1" spans="1:3">
+      <c r="A86" s="12"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="13"/>
+    </row>
+    <row r="88" ht="18.75" spans="1:2">
+      <c r="A88" s="14" t="s">
+        <v>591</v>
+      </c>
+      <c r="B88" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="86" ht="18.75" spans="1:2">
-      <c r="A86" s="14" t="s">
-        <v>589</v>
-      </c>
-      <c r="B86" s="15">
+    <row r="89" ht="18.75" spans="1:2">
+      <c r="A89" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="B89" s="15">
         <v>16</v>
       </c>
     </row>
-    <row r="158" ht="18.75" spans="1:2">
-      <c r="A158" s="14" t="s">
-        <v>590</v>
-      </c>
-      <c r="B158" s="15">
+    <row r="161" ht="18.75" spans="1:2">
+      <c r="A161" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="B161" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="159" ht="18.75" spans="1:2">
-      <c r="A159" s="14" t="s">
-        <v>591</v>
-      </c>
-      <c r="B159" s="15">
+    <row r="162" ht="18.75" spans="1:2">
+      <c r="A162" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="B162" s="15">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A3:A43"/>
-    <mergeCell ref="A46:A82"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A3:A45"/>
+    <mergeCell ref="A48:A85"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B16:B23"/>
     <mergeCell ref="B25:B32"/>
     <mergeCell ref="B34:B38"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B46:B53"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B48:B53"/>
     <mergeCell ref="B55:B61"/>
     <mergeCell ref="B63:B66"/>
     <mergeCell ref="B68:B82"/>
+    <mergeCell ref="B84:B85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -8751,104 +8773,104 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="6" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="5" ht="18" customHeight="1" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="7" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="6" ht="17" customHeight="1" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="7" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="8" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="8" ht="18" customHeight="1" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="9" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="8" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="10" ht="17" customHeight="1" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="10" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11" ht="18" customHeight="1" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="10" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="11" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="11" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="16" ht="9" customHeight="1" spans="1:3">
@@ -8858,7 +8880,7 @@
     </row>
     <row r="118" ht="18.75" spans="1:2">
       <c r="A118" s="14" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="B118" s="15">
         <v>2</v>
@@ -8866,7 +8888,7 @@
     </row>
     <row r="119" ht="18.75" spans="1:2">
       <c r="A119" s="14" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="B119" s="15">
         <v>16</v>

</xml_diff>

<commit_message>
Added course materials for JPA Using Hibernate And  PostgreSQL
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="722">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -2681,6 +2681,9 @@
     <t>9. Demo: Embeddable Primary Key and ID Class</t>
   </si>
   <si>
+    <t>Day 17</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -2790,10 +2793,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -2931,55 +2934,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2990,6 +2947,44 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3009,21 +3004,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3037,18 +3041,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3060,16 +3057,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3141,25 +3144,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3171,7 +3186,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3183,79 +3234,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3279,13 +3264,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3297,31 +3312,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3418,26 +3421,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -3460,16 +3443,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3489,17 +3472,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3515,13 +3518,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3533,130 +3536,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -9219,7 +9222,7 @@
   <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
     </sheetView>
@@ -9905,9 +9908,9 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -10072,83 +10075,83 @@
     </row>
     <row r="22" ht="24.75" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>83</v>
+        <v>693</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" ht="38" customHeight="1" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="10" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="10" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="26" ht="21" customHeight="1" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="9" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="9" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="29" ht="17" customHeight="1" spans="1:3">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="10" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="30" ht="13" customHeight="1" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="10" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="31" ht="21" customHeight="1" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="9" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="12" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="1:3">
@@ -10159,59 +10162,59 @@
     <row r="34" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="7" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C34" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3"/>
       <c r="B35" s="7"/>
       <c r="C35" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="7"/>
       <c r="C36" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3"/>
       <c r="B38" s="7"/>
       <c r="C38" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3"/>
       <c r="B41" s="7"/>
       <c r="C41" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="42" spans="1:1">
@@ -10220,31 +10223,31 @@
     <row r="43" ht="18" customHeight="1" spans="1:3">
       <c r="A43" s="3"/>
       <c r="B43" s="7" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C43" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="44" ht="18" customHeight="1" spans="1:3">
       <c r="A44" s="3"/>
       <c r="B44" s="7"/>
       <c r="C44" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="45" ht="18" customHeight="1" spans="1:3">
       <c r="A45" s="3"/>
       <c r="B45" s="7"/>
       <c r="C45" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="46" ht="16" customHeight="1" spans="1:3">
       <c r="A46" s="3"/>
       <c r="B46" s="7"/>
       <c r="C46" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="47" spans="1:1">
@@ -10256,14 +10259,14 @@
         <v>22</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="3"/>
       <c r="B49" s="13"/>
       <c r="C49" s="10" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="50" ht="9" customHeight="1" spans="1:3">

</xml_diff>

<commit_message>
Added scripts for Spring Data REST
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4021,9 +4021,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="54">
@@ -4237,18 +4237,26 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4261,38 +4269,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4314,8 +4291,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4330,20 +4352,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -4352,28 +4360,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -4460,25 +4460,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4490,31 +4478,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4532,19 +4508,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4562,37 +4538,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4610,7 +4610,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4622,25 +4622,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4749,37 +4749,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4802,8 +4776,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4825,37 +4829,33 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4867,130 +4867,130 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="28" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6366,9 +6366,9 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -6813,9 +6813,9 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Added Hands On Demos for Days 23 and 24
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="8" activeTab="11"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="22" r:id="rId1"/>
@@ -3803,7 +3803,7 @@
     <t>Next, you’ll learn how to automate tasks with both Freestyle and Pipeline job types.                                             Finally, you’ll explore practical examples of compiling, testing, packaging, and deploying software.                                                When you’re finished with this course, you’ll have the skills and knowledge of Jenkins needed to markedly boost your productivity!</t>
   </si>
   <si>
-    <t>4. Building Applications with Freestyle Jobs</t>
+    <t>3. Building Applications with Freestyle Jobs</t>
   </si>
   <si>
     <t>1. Anatomy of the Build</t>
@@ -3917,7 +3917,7 @@
     <t>Demonstrate passing test cases in IDE.</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>4th-5th May, 2022</t>
   </si>
   <si>
     <t>Write correct code to pass JUnit test cases for various modules in Spring Data JPA.</t>
@@ -4021,10 +4021,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="54">
     <font>
@@ -4237,8 +4237,44 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -4253,25 +4289,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4292,23 +4330,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4329,8 +4352,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4343,9 +4367,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4353,29 +4376,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4460,13 +4460,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4478,13 +4478,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4496,7 +4514,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4508,13 +4526,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4532,13 +4556,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4550,97 +4628,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4749,11 +4749,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4797,36 +4818,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -4834,6 +4825,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4867,130 +4867,130 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5543,7 +5543,7 @@
   <dimension ref="A7:I40"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="$A16:$XFD17"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5935,7 +5935,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A57" sqref="A57:B58"/>
     </sheetView>
@@ -6366,9 +6366,9 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -6813,9 +6813,9 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="$A8:$XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Added course materials for API Development
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="1086">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -3887,6 +3887,9 @@
     <t>Total # of Hours for Jenkins</t>
   </si>
   <si>
+    <t>Day 28</t>
+  </si>
+  <si>
     <t>Serial Number</t>
   </si>
   <si>
@@ -4021,10 +4024,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="54">
     <font>
@@ -4237,21 +4240,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -4260,38 +4248,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4306,22 +4263,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -4329,9 +4270,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4345,8 +4302,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4355,6 +4328,35 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4374,8 +4376,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4460,13 +4463,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4478,13 +4517,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4496,31 +4553,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4532,31 +4583,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4568,73 +4625,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4750,16 +4753,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4779,6 +4782,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -4794,37 +4806,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4846,10 +4838,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4867,130 +4870,130 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6366,7 +6369,7 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="B20" sqref="B20:B42"/>
     </sheetView>
@@ -6815,7 +6818,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="$A8:$XFD8"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -6830,29 +6833,31 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="1" ht="24.75" spans="1:4">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>1059</v>
+      </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" ht="15" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:6">
@@ -6860,19 +6865,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="E4" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="5" spans="6:6">
@@ -6883,19 +6888,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>1070</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>1071</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>1072</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1068</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="7" spans="6:6">
@@ -6906,24 +6911,24 @@
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="11" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -6937,37 +6942,37 @@
     </row>
     <row r="19" ht="18" spans="1:1">
       <c r="A19" s="13" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="21" ht="25.5" spans="1:1">
       <c r="A21" s="14" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="22" ht="25.5" spans="1:1">
       <c r="A22" s="14" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="23" ht="25.5" spans="1:1">
       <c r="A23" s="15" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="24" ht="25.5" spans="1:1">
       <c r="A24" s="14" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="1:1">
       <c r="A25" s="16" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="27" ht="38.25" spans="1:1">
       <c r="A27" s="17" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Course Materials for HTML 5 - Creating Forms
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="1155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="1170">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -3970,6 +3970,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">At the core of web development is a thorough knowledge of HTML.                                </t>
     </r>
     <r>
@@ -4126,6 +4134,63 @@
   </si>
   <si>
     <t>2. Course Summary</t>
+  </si>
+  <si>
+    <t>Day 29</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A big part of HTML development involves creating forms for user input.                                  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Learn the skills you need to create useful input forms on your web pages.                                           First, you will discover how HTML forms work and how to configure your form.                           Then, you will explore the various types of form inputs and how to best apply them. </t>
+    </r>
+  </si>
+  <si>
+    <t>2. Understanding HTML Forms</t>
+  </si>
+  <si>
+    <t>1. Understanding HTML Forms</t>
+  </si>
+  <si>
+    <t>2. Demo: Setting up Your Editor</t>
+  </si>
+  <si>
+    <t>3. Demo: Creating the First Form</t>
+  </si>
+  <si>
+    <t>3. Using Form Input</t>
+  </si>
+  <si>
+    <t>1. Using Form Inputs</t>
+  </si>
+  <si>
+    <t>2. Demo: Text Inputs</t>
+  </si>
+  <si>
+    <t>3. Additional Data Types</t>
+  </si>
+  <si>
+    <t>4. Selection Inputs</t>
+  </si>
+  <si>
+    <t>5. Demo: Select List</t>
+  </si>
+  <si>
+    <t>6. Demo: Checkboxes and Radio Buttons</t>
+  </si>
+  <si>
+    <t>Total # of Days for HTML 5</t>
+  </si>
+  <si>
+    <t>Total # of Hours for HTML 5</t>
   </si>
   <si>
     <t>Day 31</t>
@@ -4265,10 +4330,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="54">
     <font>
@@ -4481,16 +4546,30 @@
       <charset val="134"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4503,87 +4582,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4603,8 +4612,64 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4619,7 +4684,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4704,7 +4769,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4716,37 +4823,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4758,25 +4859,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4794,19 +4883,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4818,31 +4919,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4854,37 +4949,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4995,41 +5060,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5058,21 +5106,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -5084,22 +5117,54 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5111,130 +5176,130 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="47" fillId="29" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="48" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5306,17 +5371,17 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6573,18 +6638,18 @@
       <c r="C53" s="24"/>
     </row>
     <row r="57" customFormat="1" ht="37.5" spans="1:2">
-      <c r="A57" s="27" t="s">
+      <c r="A57" s="25" t="s">
         <v>1011</v>
       </c>
-      <c r="B57" s="28">
+      <c r="B57" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="1" ht="37.5" spans="1:2">
-      <c r="A58" s="27" t="s">
+      <c r="A58" s="25" t="s">
         <v>1012</v>
       </c>
-      <c r="B58" s="28">
+      <c r="B58" s="26">
         <v>8</v>
       </c>
     </row>
@@ -6853,7 +6918,7 @@
     <row r="32" customFormat="1" ht="27" customHeight="1" spans="1:3">
       <c r="A32" s="29"/>
       <c r="B32" s="23"/>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="27" t="s">
         <v>1044</v>
       </c>
     </row>
@@ -6952,18 +7017,18 @@
       <c r="A46" s="19"/>
     </row>
     <row r="47" ht="18.75" spans="1:2">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="25" t="s">
         <v>1057</v>
       </c>
-      <c r="B47" s="28">
+      <c r="B47" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="48" ht="18.75" spans="1:2">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="25" t="s">
         <v>1058</v>
       </c>
-      <c r="B48" s="28">
+      <c r="B48" s="26">
         <v>16</v>
       </c>
     </row>
@@ -7059,7 +7124,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="$A20:$XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -7095,21 +7160,21 @@
       <c r="B3" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>1061</v>
       </c>
     </row>
     <row r="4" ht="30" spans="1:3">
       <c r="A4" s="19"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="27" t="s">
         <v>1062</v>
       </c>
     </row>
     <row r="5" ht="22" customHeight="1" spans="1:3">
       <c r="A5" s="19"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="27" t="s">
         <v>1063</v>
       </c>
     </row>
@@ -7123,14 +7188,14 @@
       <c r="B7" s="23" t="s">
         <v>1064</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="28" t="s">
         <v>1065</v>
       </c>
     </row>
     <row r="8" ht="27" customHeight="1" spans="1:3">
       <c r="A8" s="19"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="26"/>
+      <c r="C8" s="28"/>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="19"/>
@@ -7141,49 +7206,49 @@
       <c r="B10" s="23" t="s">
         <v>1066</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="27" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="19"/>
       <c r="B11" s="23"/>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="27" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="19"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="27" t="s">
         <v>1069</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="19"/>
       <c r="B13" s="23"/>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="27" t="s">
         <v>1070</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="19"/>
       <c r="B14" s="23"/>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="27" t="s">
         <v>1071</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="1:3">
       <c r="A15" s="19"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="25"/>
+      <c r="C15" s="27"/>
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="19"/>
       <c r="B16" s="23" t="s">
         <v>1072</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="27" t="s">
         <v>1073</v>
       </c>
     </row>
@@ -7216,18 +7281,18 @@
       <c r="A22" s="19"/>
     </row>
     <row r="23" customFormat="1" ht="37.5" spans="1:2">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="25" t="s">
         <v>1076</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="1" ht="37.5" spans="1:2">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="25" t="s">
         <v>1077</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="26">
         <v>8</v>
       </c>
     </row>
@@ -7327,12 +7392,12 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61:C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -7762,74 +7827,215 @@
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
     </row>
-    <row r="60" ht="18.75" spans="1:1">
-      <c r="A60" s="19"/>
-    </row>
-    <row r="61" ht="18.75" spans="1:1">
-      <c r="A61" s="19"/>
-    </row>
-    <row r="62" ht="18.75" spans="1:3">
+    <row r="60" customFormat="1" ht="24.75" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" customFormat="1" ht="15.75" spans="1:3">
+      <c r="A61" s="19" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" customFormat="1" ht="15.75" spans="1:3">
       <c r="A62" s="19"/>
-      <c r="C62" s="21"/>
-    </row>
-    <row r="63" ht="18.75" spans="1:1">
+      <c r="B62" s="20"/>
+      <c r="C62" s="22"/>
+    </row>
+    <row r="63" customFormat="1" ht="15" spans="1:3">
       <c r="A63" s="19"/>
-    </row>
-    <row r="64" ht="18.75" spans="1:1">
+      <c r="B63" s="23" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="64" customFormat="1" ht="15" spans="1:3">
       <c r="A64" s="19"/>
-    </row>
-    <row r="65" ht="18.75" spans="1:1">
+      <c r="B64" s="23"/>
+      <c r="C64" s="21" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="65" customFormat="1" ht="15" spans="1:3">
       <c r="A65" s="19"/>
-    </row>
-    <row r="66" ht="18.75" spans="1:1">
+      <c r="B65" s="23"/>
+      <c r="C65" s="21" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="66" customFormat="1" ht="15" spans="1:3">
       <c r="A66" s="19"/>
-    </row>
-    <row r="67" ht="18.75" spans="1:1">
+      <c r="B66" s="23"/>
+      <c r="C66" s="21" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="67" customFormat="1" ht="15.75" spans="1:3">
       <c r="A67" s="19"/>
-    </row>
-    <row r="68" ht="18.75" spans="1:1">
+      <c r="B67" s="23"/>
+      <c r="C67" s="21"/>
+    </row>
+    <row r="68" customFormat="1" ht="15" spans="1:3">
       <c r="A68" s="19"/>
-    </row>
-    <row r="69" ht="18.75" spans="1:1">
+      <c r="B68" s="23" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="69" customFormat="1" ht="21" customHeight="1" spans="1:3">
       <c r="A69" s="19"/>
-    </row>
-    <row r="70" ht="18.75" spans="1:1">
+      <c r="B69" s="23"/>
+      <c r="C69" s="21" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="70" customFormat="1" ht="21" customHeight="1" spans="1:3">
       <c r="A70" s="19"/>
-    </row>
-    <row r="71" ht="18.75" spans="1:1">
+      <c r="B70" s="23"/>
+      <c r="C70" s="21" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="71" customFormat="1" ht="19" customHeight="1" spans="1:3">
       <c r="A71" s="19"/>
-    </row>
-    <row r="72" ht="18.75" spans="1:1">
+      <c r="B71" s="23"/>
+      <c r="C71" s="21" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" ht="15" spans="1:3">
       <c r="A72" s="19"/>
-    </row>
-    <row r="73" ht="18.75" spans="1:1">
+      <c r="B72" s="23"/>
+      <c r="C72" s="21" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="73" customFormat="1" ht="22" customHeight="1" spans="1:3">
       <c r="A73" s="19"/>
-    </row>
-    <row r="74" ht="18.75" spans="1:1">
+      <c r="B73" s="23"/>
+      <c r="C73" s="21" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="74" customFormat="1" ht="16" customHeight="1" spans="1:3">
       <c r="A74" s="19"/>
-    </row>
-    <row r="75" ht="18.75" spans="1:1">
-      <c r="A75" s="19"/>
-    </row>
-    <row r="76" ht="18.75" spans="1:1">
+      <c r="B74" s="23"/>
+      <c r="C74" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" customFormat="1" ht="8" customHeight="1" spans="1:3">
+      <c r="A75" s="24"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="24"/>
+    </row>
+    <row r="76" customFormat="1" ht="18.75" spans="1:1">
       <c r="A76" s="19"/>
     </row>
-    <row r="77" ht="18.75" spans="1:1">
+    <row r="77" customFormat="1" ht="18.75" spans="1:1">
       <c r="A77" s="19"/>
     </row>
-    <row r="78" ht="18.75" spans="1:1">
+    <row r="78" customFormat="1" ht="18.75" spans="1:1">
       <c r="A78" s="19"/>
     </row>
-    <row r="79" ht="18.75" spans="1:1">
-      <c r="A79" s="19"/>
-    </row>
-    <row r="80" ht="18.75" spans="1:1">
-      <c r="A80" s="19"/>
+    <row r="79" customFormat="1" ht="18.75" spans="1:2">
+      <c r="A79" s="25" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B79" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" customFormat="1" ht="18.75" spans="1:2">
+      <c r="A80" s="25" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B80" s="26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" ht="18.75" spans="1:1">
+      <c r="A81" s="19"/>
+    </row>
+    <row r="82" ht="18.75" spans="1:1">
+      <c r="A82" s="19"/>
+    </row>
+    <row r="83" ht="18.75" spans="1:3">
+      <c r="A83" s="19"/>
+      <c r="C83" s="21"/>
+    </row>
+    <row r="84" ht="18.75" spans="1:1">
+      <c r="A84" s="19"/>
+    </row>
+    <row r="85" ht="18.75" spans="1:1">
+      <c r="A85" s="19"/>
+    </row>
+    <row r="86" ht="18.75" spans="1:1">
+      <c r="A86" s="19"/>
+    </row>
+    <row r="87" ht="18.75" spans="1:1">
+      <c r="A87" s="19"/>
+    </row>
+    <row r="88" ht="18.75" spans="1:1">
+      <c r="A88" s="19"/>
+    </row>
+    <row r="89" ht="18.75" spans="1:1">
+      <c r="A89" s="19"/>
+    </row>
+    <row r="90" ht="18.75" spans="1:1">
+      <c r="A90" s="19"/>
+    </row>
+    <row r="91" ht="18.75" spans="1:1">
+      <c r="A91" s="19"/>
+    </row>
+    <row r="92" ht="18.75" spans="1:1">
+      <c r="A92" s="19"/>
+    </row>
+    <row r="93" ht="18.75" spans="1:1">
+      <c r="A93" s="19"/>
+    </row>
+    <row r="94" ht="18.75" spans="1:1">
+      <c r="A94" s="19"/>
+    </row>
+    <row r="95" ht="18.75" spans="1:1">
+      <c r="A95" s="19"/>
+    </row>
+    <row r="96" ht="18.75" spans="1:1">
+      <c r="A96" s="19"/>
+    </row>
+    <row r="97" ht="18.75" spans="1:1">
+      <c r="A97" s="19"/>
+    </row>
+    <row r="98" ht="18.75" spans="1:1">
+      <c r="A98" s="19"/>
+    </row>
+    <row r="99" ht="18.75" spans="1:1">
+      <c r="A99" s="19"/>
+    </row>
+    <row r="100" ht="18.75" spans="1:1">
+      <c r="A100" s="19"/>
+    </row>
+    <row r="101" ht="18.75" spans="1:1">
+      <c r="A101" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A60:C60"/>
     <mergeCell ref="A3:A58"/>
+    <mergeCell ref="A61:A74"/>
     <mergeCell ref="B5:B12"/>
     <mergeCell ref="B14:B23"/>
     <mergeCell ref="B25:B30"/>
@@ -7837,6 +8043,8 @@
     <mergeCell ref="B40:B47"/>
     <mergeCell ref="B49:B55"/>
     <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="B68:B74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -7867,7 +8075,7 @@
   <sheetData>
     <row r="1" customFormat="1" ht="24.75" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>1128</v>
+        <v>1143</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -7875,22 +8083,22 @@
     </row>
     <row r="2" ht="15" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>1129</v>
+        <v>1144</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1130</v>
+        <v>1145</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1131</v>
+        <v>1146</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1132</v>
+        <v>1147</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1133</v>
+        <v>1148</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1134</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:6">
@@ -7898,19 +8106,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1135</v>
+        <v>1150</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1136</v>
+        <v>1151</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1137</v>
+        <v>1152</v>
       </c>
       <c r="E4" t="s">
-        <v>1138</v>
+        <v>1153</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>1139</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="5" spans="6:6">
@@ -7921,19 +8129,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1140</v>
+        <v>1155</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>1141</v>
+        <v>1156</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1142</v>
+        <v>1157</v>
       </c>
       <c r="E6" t="s">
-        <v>1138</v>
+        <v>1153</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>1139</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="7" spans="6:6">
@@ -7944,24 +8152,24 @@
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>1143</v>
+        <v>1158</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1144</v>
+        <v>1159</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>1145</v>
+        <v>1160</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>1146</v>
+        <v>1161</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>1139</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="11" t="s">
-        <v>1147</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -7975,37 +8183,37 @@
     </row>
     <row r="19" ht="18" spans="1:1">
       <c r="A19" s="13" t="s">
-        <v>1148</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="21" ht="25.5" spans="1:1">
       <c r="A21" s="14" t="s">
-        <v>1149</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="22" ht="25.5" spans="1:1">
       <c r="A22" s="14" t="s">
-        <v>1150</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="23" ht="25.5" spans="1:1">
       <c r="A23" s="15" t="s">
-        <v>1151</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="24" ht="25.5" spans="1:1">
       <c r="A24" s="14" t="s">
-        <v>1152</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="1:1">
       <c r="A25" s="16" t="s">
-        <v>1153</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="27" ht="38.25" spans="1:1">
       <c r="A27" s="17" t="s">
-        <v>1154</v>
+        <v>1169</v>
       </c>
     </row>
   </sheetData>
@@ -8089,21 +8297,21 @@
     <row r="7" ht="18" customHeight="1" spans="1:3">
       <c r="A7" s="19"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="28" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" spans="1:3">
       <c r="A8" s="19"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="28" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="19"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="28" t="s">
         <v>42</v>
       </c>
     </row>
@@ -8154,7 +8362,7 @@
       <c r="B16" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="28" t="s">
         <v>50</v>
       </c>
     </row>
@@ -8196,7 +8404,7 @@
     <row r="22" ht="14" customHeight="1" spans="1:3">
       <c r="A22" s="19"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="28" t="s">
         <v>56</v>
       </c>
     </row>
@@ -8433,7 +8641,7 @@
     <row r="55" ht="21" customHeight="1" spans="1:3">
       <c r="A55" s="19"/>
       <c r="B55" s="23"/>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="28" t="s">
         <v>88</v>
       </c>
     </row>
@@ -8447,7 +8655,7 @@
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="19"/>
       <c r="B57" s="23"/>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="28" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8475,7 +8683,7 @@
     <row r="61" ht="21" customHeight="1" spans="1:3">
       <c r="A61" s="19"/>
       <c r="B61" s="23"/>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="28" t="s">
         <v>94</v>
       </c>
     </row>
@@ -8789,7 +8997,7 @@
     <row r="106" ht="21" customHeight="1" spans="1:3">
       <c r="A106" s="19"/>
       <c r="B106" s="23"/>
-      <c r="C106" s="26" t="s">
+      <c r="C106" s="28" t="s">
         <v>129</v>
       </c>
     </row>
@@ -8803,7 +9011,7 @@
     <row r="108" ht="15" spans="1:3">
       <c r="A108" s="19"/>
       <c r="B108" s="23"/>
-      <c r="C108" s="26" t="s">
+      <c r="C108" s="28" t="s">
         <v>131</v>
       </c>
     </row>
@@ -9089,7 +9297,7 @@
     <row r="149" ht="21" customHeight="1" spans="1:3">
       <c r="A149" s="19"/>
       <c r="B149" s="23"/>
-      <c r="C149" s="26" t="s">
+      <c r="C149" s="28" t="s">
         <v>165</v>
       </c>
     </row>
@@ -9103,7 +9311,7 @@
     <row r="151" ht="15" spans="1:3">
       <c r="A151" s="19"/>
       <c r="B151" s="23"/>
-      <c r="C151" s="26" t="s">
+      <c r="C151" s="28" t="s">
         <v>167</v>
       </c>
     </row>
@@ -12096,14 +12304,14 @@
     <row r="7" ht="18" customHeight="1" spans="1:3">
       <c r="A7" s="19"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="28" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" spans="1:3">
       <c r="A8" s="19"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="28" t="s">
         <v>527</v>
       </c>
     </row>
@@ -12117,7 +12325,7 @@
       <c r="B10" s="23" t="s">
         <v>528</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="28" t="s">
         <v>524</v>
       </c>
     </row>
@@ -12306,7 +12514,7 @@
     <row r="37" ht="21" customHeight="1" spans="1:3">
       <c r="A37" s="19"/>
       <c r="B37" s="23"/>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="28" t="s">
         <v>550</v>
       </c>
     </row>
@@ -12398,14 +12606,14 @@
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="19"/>
       <c r="B50" s="23"/>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="28" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="19"/>
       <c r="B51" s="23"/>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="28" t="s">
         <v>562</v>
       </c>
     </row>
@@ -12419,7 +12627,7 @@
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="19"/>
       <c r="B53" s="23"/>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="28" t="s">
         <v>247</v>
       </c>
     </row>
@@ -12764,14 +12972,14 @@
     <row r="5" ht="18" customHeight="1" spans="1:3">
       <c r="A5" s="51"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="27" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="6" ht="17" customHeight="1" spans="1:3">
       <c r="A6" s="51"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="27" t="s">
         <v>600</v>
       </c>
     </row>
@@ -12785,7 +12993,7 @@
     <row r="8" ht="18" customHeight="1" spans="1:3">
       <c r="A8" s="51"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="28" t="s">
         <v>602</v>
       </c>
     </row>
@@ -12885,14 +13093,14 @@
     <row r="22" ht="18" customHeight="1" spans="1:3">
       <c r="A22" s="19"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="28" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="23" ht="12" customHeight="1" spans="1:3">
       <c r="A23" s="19"/>
       <c r="B23" s="23"/>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="28" t="s">
         <v>615</v>
       </c>
     </row>
@@ -12906,63 +13114,63 @@
     <row r="25" ht="18" customHeight="1" spans="1:3">
       <c r="A25" s="19"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="28" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:3">
       <c r="A26" s="19"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="28" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="27" ht="18" customHeight="1" spans="1:3">
       <c r="A27" s="19"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="28" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:3">
       <c r="A28" s="19"/>
       <c r="B28" s="23"/>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="28" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:3">
       <c r="A29" s="19"/>
       <c r="B29" s="23"/>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="28" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:3">
       <c r="A30" s="19"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="28" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:3">
       <c r="A31" s="19"/>
       <c r="B31" s="23"/>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="28" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="1" spans="1:3">
       <c r="A32" s="19"/>
       <c r="B32" s="23"/>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="28" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="1" spans="1:3">
       <c r="A33" s="19"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="28" t="s">
         <v>625</v>
       </c>
     </row>
@@ -13188,14 +13396,14 @@
     <row r="65" ht="18" customHeight="1" spans="1:3">
       <c r="A65" s="55"/>
       <c r="B65" s="23"/>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="27" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="66" ht="17" customHeight="1" spans="1:3">
       <c r="A66" s="55"/>
       <c r="B66" s="23"/>
-      <c r="C66" s="25" t="s">
+      <c r="C66" s="27" t="s">
         <v>654</v>
       </c>
     </row>
@@ -13209,7 +13417,7 @@
     <row r="68" ht="18" customHeight="1" spans="1:3">
       <c r="A68" s="55"/>
       <c r="B68" s="23"/>
-      <c r="C68" s="26" t="s">
+      <c r="C68" s="28" t="s">
         <v>656</v>
       </c>
     </row>
@@ -13265,14 +13473,14 @@
     <row r="76" ht="18" customHeight="1" spans="1:3">
       <c r="A76" s="55"/>
       <c r="B76" s="23"/>
-      <c r="C76" s="26" t="s">
+      <c r="C76" s="28" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="77" ht="12" customHeight="1" spans="1:3">
       <c r="A77" s="55"/>
       <c r="B77" s="23"/>
-      <c r="C77" s="26" t="s">
+      <c r="C77" s="28" t="s">
         <v>663</v>
       </c>
     </row>
@@ -13286,14 +13494,14 @@
     <row r="79" ht="18" customHeight="1" spans="1:3">
       <c r="A79" s="55"/>
       <c r="B79" s="23"/>
-      <c r="C79" s="26" t="s">
+      <c r="C79" s="28" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="80" ht="18" customHeight="1" spans="1:3">
       <c r="A80" s="55"/>
       <c r="B80" s="23"/>
-      <c r="C80" s="26" t="s">
+      <c r="C80" s="28" t="s">
         <v>666</v>
       </c>
     </row>
@@ -13464,21 +13672,21 @@
     <row r="7" ht="18" customHeight="1" spans="1:3">
       <c r="A7" s="19"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="28" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" spans="1:3">
       <c r="A8" s="19"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="28" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="19"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="28" t="s">
         <v>681</v>
       </c>
     </row>
@@ -13499,7 +13707,7 @@
       <c r="B12" s="23" t="s">
         <v>683</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="28" t="s">
         <v>684</v>
       </c>
     </row>
@@ -13541,7 +13749,7 @@
     <row r="18" ht="22" customHeight="1" spans="1:3">
       <c r="A18" s="19"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="28" t="s">
         <v>690</v>
       </c>
     </row>
@@ -13578,7 +13786,7 @@
       <c r="B23" s="23" t="s">
         <v>695</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="28" t="s">
         <v>696</v>
       </c>
     </row>
@@ -13599,7 +13807,7 @@
     <row r="26" ht="21" customHeight="1" spans="1:3">
       <c r="A26" s="19"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="28" t="s">
         <v>699</v>
       </c>
     </row>
@@ -13613,7 +13821,7 @@
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="19"/>
       <c r="B28" s="23"/>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="28" t="s">
         <v>701</v>
       </c>
     </row>
@@ -13634,7 +13842,7 @@
     <row r="31" ht="21" customHeight="1" spans="1:3">
       <c r="A31" s="19"/>
       <c r="B31" s="23"/>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="28" t="s">
         <v>704</v>
       </c>
     </row>
@@ -15161,14 +15369,14 @@
     <row r="23" ht="20" customHeight="1" spans="1:3">
       <c r="A23" s="19"/>
       <c r="B23" s="32"/>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="27" t="s">
         <v>859</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="19"/>
       <c r="B24" s="32"/>
-      <c r="C24" s="25"/>
+      <c r="C24" s="27"/>
     </row>
     <row r="25" ht="8" customHeight="1" spans="1:3">
       <c r="A25" s="24"/>

</xml_diff>

<commit_message>
Updated Sprint1 evaluation scores
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="22" r:id="rId1"/>
@@ -4206,6 +4206,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">This course is a discovery of the many new features found in CSS3.                                                    </t>
     </r>
     <r>
@@ -4496,7 +4504,7 @@
     <t>Demonstrate passing test cases in IDE.</t>
   </si>
   <si>
-    <t>4th-5th May, 2022</t>
+    <t>7th May, 2022</t>
   </si>
   <si>
     <t>Write correct code to pass JUnit test cases for various modules in Spring Data JPA.</t>
@@ -4601,9 +4609,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="54">
     <font>
@@ -4816,16 +4824,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -4839,6 +4846,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -4847,32 +4862,23 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4887,10 +4893,40 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4903,17 +4939,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4926,35 +4954,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5039,25 +5047,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5075,7 +5083,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5087,7 +5137,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5099,7 +5149,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5111,79 +5197,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5195,31 +5227,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5331,8 +5339,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5352,6 +5360,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -5363,6 +5380,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5382,26 +5419,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -5416,19 +5433,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5446,130 +5454,130 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="47" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="48" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6121,8 +6129,8 @@
   <sheetPr/>
   <dimension ref="A7:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:H24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -9067,10 +9075,10 @@
   <sheetPr/>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Added React.js course materials
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="14" activeTab="19"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="14" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="22" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="1490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="1491">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -5032,7 +5032,10 @@
     <t>1. TypeScript</t>
   </si>
   <si>
-    <t>Hands On Exercises - TypeScript Basics</t>
+    <t>TypeScript Exercises</t>
+  </si>
+  <si>
+    <t>TypeScript Lab</t>
   </si>
   <si>
     <t>Total # of Days for TypeScript</t>
@@ -5501,10 +5504,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="56">
     <font>
@@ -5724,7 +5727,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5738,14 +5741,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5764,14 +5760,6 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5822,8 +5810,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5836,16 +5840,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5859,9 +5856,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5953,7 +5956,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5965,19 +6040,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5989,91 +6106,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6085,55 +6130,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6242,26 +6245,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6290,26 +6293,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6329,6 +6317,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -6342,7 +6345,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -6360,130 +6363,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="27" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -10972,12 +10975,12 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -11359,15 +11362,19 @@
       </c>
       <c r="D52" s="7"/>
     </row>
-    <row r="53" ht="8" customHeight="1" spans="1:4">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="11"/>
-    </row>
-    <row r="54" ht="18" spans="1:2">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
+    <row r="53" ht="18.75" spans="1:4">
+      <c r="A53" s="3"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="7" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" ht="8" customHeight="1" spans="1:4">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="11"/>
     </row>
     <row r="55" ht="18" spans="1:2">
       <c r="A55" s="13"/>
@@ -11377,41 +11384,45 @@
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
     </row>
-    <row r="57" ht="18.75" spans="1:2">
-      <c r="A57" s="12" t="s">
-        <v>1375</v>
-      </c>
-      <c r="B57" s="13">
-        <v>1</v>
-      </c>
+    <row r="57" ht="18" spans="1:2">
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
     </row>
     <row r="58" ht="18.75" spans="1:2">
       <c r="A58" s="12" t="s">
         <v>1376</v>
       </c>
       <c r="B58" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" ht="18.75" spans="1:2">
+      <c r="A59" s="12" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B59" s="13">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" ht="18.75" spans="1:1">
-      <c r="A59" s="3"/>
     </row>
     <row r="60" ht="18.75" spans="1:1">
       <c r="A60" s="3"/>
     </row>
     <row r="61" ht="18.75" spans="1:1">
       <c r="A61" s="3"/>
+    </row>
+    <row r="62" ht="18.75" spans="1:1">
+      <c r="A62" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A54:C54"/>
     <mergeCell ref="A3:A52"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="B15:B24"/>
     <mergeCell ref="B26:B35"/>
     <mergeCell ref="B37:B49"/>
-    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B51:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -11424,7 +11435,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A38" sqref="$A38:$XFD38"/>
     </sheetView>
@@ -11450,14 +11461,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="18" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>36</v>
@@ -11477,35 +11488,35 @@
       <c r="A5" s="3"/>
       <c r="B5" s="15"/>
       <c r="C5" s="7" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="6" ht="18" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="15"/>
       <c r="C6" s="7" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="15"/>
       <c r="C7" s="7" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="8" customFormat="1" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="15"/>
       <c r="C8" s="7" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="9" customFormat="1" ht="15" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="15"/>
       <c r="C9" s="7" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="1:3">
@@ -11516,7 +11527,7 @@
     <row r="11" customFormat="1" ht="15" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="15" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>73</v>
@@ -11526,56 +11537,56 @@
       <c r="A12" s="3"/>
       <c r="B12" s="15"/>
       <c r="C12" s="7" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="13" customFormat="1" ht="15" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="15"/>
       <c r="C13" s="7" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="14" customFormat="1" ht="15" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="15"/>
       <c r="C14" s="7" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="15"/>
       <c r="C15" s="7" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="15" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="15"/>
       <c r="C16" s="7" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="17" customFormat="1" ht="15" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="15"/>
       <c r="C17" s="7" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="15"/>
       <c r="C18" s="7" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="19" customFormat="1" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="15"/>
       <c r="C19" s="7" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="20" customFormat="1" ht="15" spans="1:3">
@@ -11585,45 +11596,45 @@
     <row r="21" customFormat="1" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="15" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="22" customFormat="1" ht="18" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="15"/>
       <c r="C22" s="7" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="23" customFormat="1" ht="15" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="15"/>
       <c r="C23" s="7" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="24" customFormat="1" ht="15" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="15"/>
       <c r="C24" s="7" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="15"/>
       <c r="C25" s="7" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="15"/>
       <c r="C26" s="7" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="27" ht="18" spans="1:3">
@@ -11634,7 +11645,7 @@
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="15" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>73</v>
@@ -11644,35 +11655,35 @@
       <c r="A29" s="3"/>
       <c r="B29" s="15"/>
       <c r="C29" s="7" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="15"/>
       <c r="C30" s="7" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="15"/>
       <c r="C31" s="7" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="15"/>
       <c r="C32" s="7" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="3"/>
       <c r="B33" s="15"/>
       <c r="C33" s="7" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="34" ht="18" spans="1:3">
@@ -11686,21 +11697,21 @@
         <v>22</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="3"/>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="37" ht="21" customHeight="1" spans="1:3">
       <c r="A37" s="3"/>
       <c r="B37" s="8"/>
       <c r="C37" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="38" ht="8" customHeight="1" spans="1:4">
@@ -11723,7 +11734,7 @@
     </row>
     <row r="42" ht="18.75" spans="1:2">
       <c r="A42" s="12" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="B42" s="13">
         <v>1</v>
@@ -11731,7 +11742,7 @@
     </row>
     <row r="43" ht="18.75" spans="1:2">
       <c r="A43" s="12" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="B43" s="13">
         <v>8</v>
@@ -15774,10 +15785,10 @@
   <sheetPr/>
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A88"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -15801,14 +15812,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>36</v>
@@ -15825,80 +15836,80 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="6" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="7" customFormat="1" ht="15" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="8" customFormat="1" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="9" customFormat="1" ht="15" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="10" customFormat="1" ht="15" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="11" customFormat="1" ht="15" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="12" customFormat="1" ht="15" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="13" customFormat="1" ht="15" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="14" customFormat="1" ht="15" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="15" spans="1:3">
@@ -15916,52 +15927,52 @@
     <row r="18" customFormat="1" ht="15" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="6" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="19" customFormat="1" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="20" customFormat="1" ht="15" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="21" customFormat="1" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="22" customFormat="1" ht="15" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="23" customFormat="1" ht="15" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
@@ -15979,59 +15990,59 @@
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="6" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="3"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
       <c r="A29" s="3"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="3"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="3"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="3"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="3"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
@@ -16048,129 +16059,129 @@
     <row r="37" ht="15" spans="1:3">
       <c r="A37" s="3"/>
       <c r="B37" s="6" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="3"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="3"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="3"/>
       <c r="B40" s="6"/>
       <c r="C40" s="7" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="3"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="3"/>
       <c r="B42" s="6"/>
       <c r="C42" s="7" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="3"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="3"/>
       <c r="B44" s="6"/>
       <c r="C44" s="7" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="3"/>
       <c r="B45" s="6"/>
       <c r="C45" s="7" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="3"/>
       <c r="B46" s="6"/>
       <c r="C46" s="7" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="3"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="3"/>
       <c r="B48" s="6"/>
       <c r="C48" s="7" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="3"/>
       <c r="B49" s="6"/>
       <c r="C49" s="7" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="3"/>
       <c r="B50" s="6"/>
       <c r="C50" s="7" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="3"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="3"/>
       <c r="B52" s="6"/>
       <c r="C52" s="7" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="3"/>
       <c r="B53" s="6"/>
       <c r="C53" s="7" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="3"/>
       <c r="B54" s="6"/>
       <c r="C54" s="7" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="55" spans="1:1">
@@ -16179,59 +16190,59 @@
     <row r="56" ht="15" spans="1:3">
       <c r="A56" s="3"/>
       <c r="B56" s="6" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="3"/>
       <c r="B57" s="6"/>
       <c r="C57" s="7" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
       <c r="A58" s="3"/>
       <c r="B58" s="6"/>
       <c r="C58" s="7" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="59" ht="15" spans="1:3">
       <c r="A59" s="3"/>
       <c r="B59" s="6"/>
       <c r="C59" s="7" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="3"/>
       <c r="B60" s="6"/>
       <c r="C60" s="7" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="3"/>
       <c r="B61" s="6"/>
       <c r="C61" s="7" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="3"/>
       <c r="B62" s="6"/>
       <c r="C62" s="7" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="3"/>
       <c r="B63" s="6"/>
       <c r="C63" s="7" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:3">
@@ -16250,161 +16261,161 @@
         <v>22</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:3">
       <c r="A67" s="3"/>
       <c r="B67" s="8"/>
       <c r="C67" s="7" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="68" ht="15" spans="1:3">
       <c r="A68" s="3"/>
       <c r="B68" s="8"/>
       <c r="C68" s="7" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:3">
       <c r="A69" s="3"/>
       <c r="B69" s="8"/>
       <c r="C69" s="7" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:3">
       <c r="A70" s="3"/>
       <c r="B70" s="8"/>
       <c r="C70" s="7" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="71" ht="15" spans="1:3">
       <c r="A71" s="3"/>
       <c r="B71" s="8"/>
       <c r="C71" s="7" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="72" ht="15" spans="1:3">
       <c r="A72" s="3"/>
       <c r="B72" s="8"/>
       <c r="C72" s="5" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="73" ht="15" spans="1:3">
       <c r="A73" s="3"/>
       <c r="B73" s="8"/>
       <c r="C73" s="7" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:3">
       <c r="A74" s="3"/>
       <c r="B74" s="8"/>
       <c r="C74" s="7" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="75" ht="15" spans="1:3">
       <c r="A75" s="3"/>
       <c r="B75" s="8"/>
       <c r="C75" s="7" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="76" ht="15" spans="1:3">
       <c r="A76" s="3"/>
       <c r="B76" s="8"/>
       <c r="C76" s="7" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="77" ht="15" spans="1:3">
       <c r="A77" s="3"/>
       <c r="B77" s="8"/>
       <c r="C77" s="7" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="78" ht="15" spans="1:3">
       <c r="A78" s="3"/>
       <c r="B78" s="8"/>
       <c r="C78" s="7" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="79" ht="15" spans="1:3">
       <c r="A79" s="3"/>
       <c r="B79" s="8"/>
       <c r="C79" s="7" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="80" ht="15" spans="1:3">
       <c r="A80" s="3"/>
       <c r="B80" s="8"/>
       <c r="C80" s="7" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="81" ht="15" spans="1:3">
       <c r="A81" s="3"/>
       <c r="B81" s="8"/>
       <c r="C81" s="7" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="82" ht="15" spans="1:3">
       <c r="A82" s="3"/>
       <c r="B82" s="8"/>
       <c r="C82" s="7" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="83" ht="15" spans="1:3">
       <c r="A83" s="3"/>
       <c r="B83" s="8"/>
       <c r="C83" s="7" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="84" ht="15" spans="1:3">
       <c r="A84" s="3"/>
       <c r="B84" s="8"/>
       <c r="C84" s="7" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="85" ht="15" spans="1:3">
       <c r="A85" s="3"/>
       <c r="B85" s="8"/>
       <c r="C85" s="7" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="86" ht="15" spans="1:3">
       <c r="A86" s="3"/>
       <c r="B86" s="8"/>
       <c r="C86" s="7" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="87" ht="15" spans="1:3">
       <c r="A87" s="3"/>
       <c r="B87" s="8"/>
       <c r="C87" s="7" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="88" ht="15" spans="1:3">
       <c r="A88" s="3"/>
       <c r="B88" s="8"/>
       <c r="C88" s="7" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="89" ht="8" customHeight="1" spans="1:4">
@@ -16415,7 +16426,7 @@
     </row>
     <row r="93" ht="37.5" spans="1:2">
       <c r="A93" s="12" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="B93" s="13">
         <v>1</v>
@@ -16423,7 +16434,7 @@
     </row>
     <row r="94" ht="37.5" spans="1:2">
       <c r="A94" s="12" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="B94" s="13">
         <v>8</v>

</xml_diff>

<commit_message>
Updated course materials for MAterial UI and Full Stack Project
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="17" activeTab="22"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="22" r:id="rId1"/>
@@ -30,13 +30,14 @@
     <sheet name="React with Redux" sheetId="45" r:id="rId21"/>
     <sheet name="TDD with Jest" sheetId="46" r:id="rId22"/>
     <sheet name="Material UI" sheetId="47" r:id="rId23"/>
+    <sheet name="Full Stack Project" sheetId="48" r:id="rId24"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="1689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="1716">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -5894,7 +5895,7 @@
     <t>Total # of Hours for React with Redux</t>
   </si>
   <si>
-    <t>Day 42</t>
+    <t>Day 42-43</t>
   </si>
   <si>
     <r>
@@ -6037,7 +6038,7 @@
     <t>Total # of Hours for TDD with Jest</t>
   </si>
   <si>
-    <t>Day 43</t>
+    <t>Day 44</t>
   </si>
   <si>
     <t>Styling a React App with Material UI</t>
@@ -6134,6 +6135,87 @@
   </si>
   <si>
     <t>Total # of Hours for Material UI</t>
+  </si>
+  <si>
+    <t>Day 45</t>
+  </si>
+  <si>
+    <t>Full Stack Project with React JS and Spring Boot</t>
+  </si>
+  <si>
+    <t>1. Spring Boot Backend</t>
+  </si>
+  <si>
+    <t>1. Create spring boot project</t>
+  </si>
+  <si>
+    <t>2. Add maven dependencies</t>
+  </si>
+  <si>
+    <t>3. Create Database</t>
+  </si>
+  <si>
+    <t>4. Configure Datasource</t>
+  </si>
+  <si>
+    <t>5. Create an Entity class</t>
+  </si>
+  <si>
+    <t>6. Create a Repository</t>
+  </si>
+  <si>
+    <t>7. Create a Controller</t>
+  </si>
+  <si>
+    <t>8. Run the App</t>
+  </si>
+  <si>
+    <t>9. Test API endpoints in Postman</t>
+  </si>
+  <si>
+    <t>2. React JS Frontend</t>
+  </si>
+  <si>
+    <t>1. Create React Project</t>
+  </si>
+  <si>
+    <t>2. Install axios library</t>
+  </si>
+  <si>
+    <t>3. Install React Router DOM library</t>
+  </si>
+  <si>
+    <t>4. Install Bootstrap library</t>
+  </si>
+  <si>
+    <t>6. Configure axios library</t>
+  </si>
+  <si>
+    <t>7. Create Employee Service</t>
+  </si>
+  <si>
+    <t>8. Create EmployeeList Component</t>
+  </si>
+  <si>
+    <t>9. Create Add Employee Component</t>
+  </si>
+  <si>
+    <t>10. Create NotFound Component</t>
+  </si>
+  <si>
+    <t>11. Configure React Router</t>
+  </si>
+  <si>
+    <t>12. Run the React App</t>
+  </si>
+  <si>
+    <t>13. Test the Web application</t>
+  </si>
+  <si>
+    <t>Total # of Days for Full Stack Project</t>
+  </si>
+  <si>
+    <t>Total # of Hours for Full Stack Project</t>
   </si>
 </sst>
 </file>
@@ -6141,10 +6223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="56">
     <font>
@@ -6363,6 +6445,35 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -6371,6 +6482,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -6378,8 +6506,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6394,17 +6523,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6416,16 +6537,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6433,38 +6546,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6479,29 +6561,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6593,7 +6675,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6605,19 +6729,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6629,13 +6765,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6647,7 +6783,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6659,7 +6825,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6677,103 +6843,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6882,6 +6964,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -6897,26 +6999,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6936,22 +7023,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6982,13 +7064,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7000,130 +7082,130 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="48" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="26" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -12072,7 +12154,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A38" sqref="$A38:$XFD38"/>
     </sheetView>
@@ -16423,7 +16505,7 @@
   <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
@@ -17100,9 +17182,9 @@
   <dimension ref="A1:D153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B144" sqref="B144:B147"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -18196,9 +18278,9 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -18592,10 +18674,10 @@
   <sheetPr/>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -18886,6 +18968,254 @@
     <mergeCell ref="B4:B14"/>
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="B27:B34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="35.125" customWidth="1"/>
+    <col min="3" max="3" width="69.75" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.5" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" ht="24.75" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" ht="12" customHeight="1" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" ht="15" spans="1:3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="6" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="5" ht="15" spans="1:3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" ht="15" spans="1:3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" ht="15" spans="1:3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" ht="15" spans="1:3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" ht="15" spans="1:3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" ht="15" spans="1:3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" ht="15" spans="1:3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" ht="15" spans="1:3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" spans="1:3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" ht="15" spans="1:3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="6" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="16" ht="15" spans="1:3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="17" ht="15" spans="1:3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="18" ht="15" spans="1:3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="19" ht="15" spans="1:3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="20" ht="15" spans="1:3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="21" ht="15" spans="1:3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="22" ht="15" spans="1:3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="23" ht="15" spans="1:3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="24" ht="15" spans="1:3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="25" ht="15" spans="1:3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="26" ht="15" spans="1:3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="27" ht="8" customHeight="1" spans="1:4">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" ht="15.75" spans="2:2">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" ht="15.75" spans="2:2">
+      <c r="B29" s="4"/>
+    </row>
+    <row r="31" ht="37.5" spans="1:2">
+      <c r="A31" s="10" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B31" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" ht="37.5" spans="1:2">
+      <c r="A32" s="10" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B32" s="11">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A3:A26"/>
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="B14:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added Slides for Forms in React - final modules
</commit_message>
<xml_diff>
--- a/JEE Full Stack 2.0 with React - TOC.xlsx
+++ b/JEE Full Stack 2.0 with React - TOC.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="1745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="1767">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -6219,29 +6219,21 @@
     <t>Total # of Hours for Full Stack Project</t>
   </si>
   <si>
-    <t>Day 46-47</t>
+    <t>Day 46-48</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">Forms are the primary mode of collecting user input on web apps.                                     </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Learn to create forms for your web app that are not only performant, user friendly, and consistent but are built using components that are reusable and have rock solid data validation.                                                                         First, you will explore how a basic form works with Vanilla React and how to manage its state and handle user input.                                  You will also see how to create a form using a library called Formik to avoid writing a whole lot of boilerplate code that is needed when using Vanilla React.                                                             Next, you will explore adding sync and async data validation to your forms using the various mechanisms provided by Formik and how to create custom self-sufficient form elements that can be reused across screens in your app to provide that consistent look and experience to the end user.                                           Finally, you will learn how to implement uncontrolled forms and alternative ways of implementing forms that rely solely on uncontrolled components like the React Hook Form library and what advantages that brings.                                                                        When you are finished with this course, you will be very comfortable creating forms in React that can not only support a wide variety of user inputs but are smooth, consistent, and air tight when collecting data from the user.</t>
+      <t>Learn to create forms for your web app that are not only performant, user friendly, and consistent but are built using components that are reusable and have rock solid data validation.                                                                         First, you will explore how a basic form works with Vanilla React and how to manage its state and handle user input.                                              You will also see how to create a form using a library called Formik to avoid writing a whole lot of boilerplate code that is needed when using Vanilla React.                                                             Next, you will explore adding sync and async data validation to your forms using the various mechanisms provided by Formik and how to create custom self-sufficient form elements that can be reused across screens in your app to provide that consistent look and experience to the end user.                                           Finally, you will learn how to implement uncontrolled forms and alternative ways of implementing forms that rely solely on uncontrolled components like the React Hook Form library and what advantages that brings.                                                                        When you are finished with this course, you will be very comfortable creating forms in React that can not only support a wide variety of user inputs but are smooth, consistent, and air tight when collecting data from the user.</t>
     </r>
   </si>
   <si>
@@ -6323,7 +6315,73 @@
     <t>1. Creating a Form Using React Hook Form</t>
   </si>
   <si>
-    <t>2.Data Validation in React Hook Form</t>
+    <t>2. Data Validation in React Hook Form</t>
+  </si>
+  <si>
+    <t>8. Creating Dynamic Forms With React Hooks</t>
+  </si>
+  <si>
+    <t>1. Defining a data structure</t>
+  </si>
+  <si>
+    <t>2. Creating the form</t>
+  </si>
+  <si>
+    <t>3. Defining state</t>
+  </si>
+  <si>
+    <t>4. Rendering the form fields</t>
+  </si>
+  <si>
+    <t>5. Handling user input</t>
+  </si>
+  <si>
+    <t>6. Adding navigation</t>
+  </si>
+  <si>
+    <t>7. Conditional fields</t>
+  </si>
+  <si>
+    <t>8. Conditional pages</t>
+  </si>
+  <si>
+    <t>9. Build Dynamic Forms in React</t>
+  </si>
+  <si>
+    <t>1. Create a simple form</t>
+  </si>
+  <si>
+    <t>2. Using React State Hook</t>
+  </si>
+  <si>
+    <t>3. Add the Values from formFields State</t>
+  </si>
+  <si>
+    <t>4. Create a function called handleFormChange</t>
+  </si>
+  <si>
+    <t>6. Create a Submit Button</t>
+  </si>
+  <si>
+    <t>7. Remove the fields using a Remove Button</t>
+  </si>
+  <si>
+    <t>8. Wrapping Up</t>
+  </si>
+  <si>
+    <t>10. Create a Dropdown Menu from Scratch</t>
+  </si>
+  <si>
+    <t>2. WYWL: What You Will Learn</t>
+  </si>
+  <si>
+    <t>3. Building the React Dropdown as a Functional Component</t>
+  </si>
+  <si>
+    <t>Total # of Days for Forms in React</t>
+  </si>
+  <si>
+    <t>Total # of Hours for Forms in React</t>
   </si>
 </sst>
 </file>
@@ -6331,12 +6389,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="57">
+  <fonts count="59">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -6359,7 +6417,7 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -6526,6 +6584,14 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
@@ -6574,6 +6640,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -6582,8 +6685,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6597,11 +6709,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6622,22 +6741,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6652,60 +6771,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -6724,6 +6790,13 @@
       <color theme="1"/>
       <name val="Verdana"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -6790,7 +6863,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6802,25 +7007,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6832,145 +7043,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7079,35 +7152,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7127,6 +7182,44 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -7142,44 +7235,24 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7197,134 +7270,134 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="19" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7477,6 +7550,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -7484,7 +7560,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -7493,7 +7569,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7511,37 +7587,37 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7560,7 +7636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7898,253 +7974,253 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="69" t="s">
+      <c r="G8" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="69" t="s">
+      <c r="H8" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="69" t="s">
+      <c r="I8" s="70" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="70">
+      <c r="F9" s="71">
         <v>1</v>
       </c>
-      <c r="G9" s="71" t="s">
+      <c r="G9" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="72">
+      <c r="H9" s="73">
         <v>10.5</v>
       </c>
-      <c r="I9" s="72">
+      <c r="I9" s="73">
         <v>84</v>
       </c>
     </row>
     <row r="10" ht="30.75" spans="6:9">
-      <c r="F10" s="73">
+      <c r="F10" s="74">
         <v>2</v>
       </c>
-      <c r="G10" s="71" t="s">
+      <c r="G10" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="72">
+      <c r="H10" s="73">
         <v>3</v>
       </c>
-      <c r="I10" s="72">
+      <c r="I10" s="73">
         <v>24</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="6:9">
-      <c r="F11" s="73">
+      <c r="F11" s="74">
         <v>3</v>
       </c>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="72">
+      <c r="H11" s="73">
         <v>2</v>
       </c>
-      <c r="I11" s="72">
+      <c r="I11" s="73">
         <v>16</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="6:9">
-      <c r="F12" s="73">
+      <c r="F12" s="74">
         <v>4</v>
       </c>
-      <c r="G12" s="74" t="s">
+      <c r="G12" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="72">
+      <c r="H12" s="73">
         <v>0.5</v>
       </c>
-      <c r="I12" s="72">
+      <c r="I12" s="73">
         <v>4</v>
       </c>
     </row>
     <row r="13" ht="14" customHeight="1" spans="6:9">
-      <c r="F13" s="73">
+      <c r="F13" s="74">
         <v>5</v>
       </c>
-      <c r="G13" s="71" t="s">
+      <c r="G13" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="72">
+      <c r="H13" s="73">
         <v>2</v>
       </c>
-      <c r="I13" s="72">
+      <c r="I13" s="73">
         <v>16</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="6:9">
-      <c r="F14" s="73">
+      <c r="F14" s="74">
         <v>6</v>
       </c>
-      <c r="G14" s="71" t="s">
+      <c r="G14" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="72">
+      <c r="H14" s="73">
         <v>2</v>
       </c>
-      <c r="I14" s="72">
+      <c r="I14" s="73">
         <v>16</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="6:9">
-      <c r="F15" s="73">
+      <c r="F15" s="74">
         <v>7</v>
       </c>
-      <c r="G15" s="74" t="s">
+      <c r="G15" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="72">
+      <c r="H15" s="73">
         <v>1</v>
       </c>
-      <c r="I15" s="72">
+      <c r="I15" s="73">
         <v>8</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="6:9">
-      <c r="F16" s="73">
+      <c r="F16" s="74">
         <v>8</v>
       </c>
-      <c r="G16" s="75" t="s">
+      <c r="G16" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="72">
+      <c r="H16" s="73">
         <v>6</v>
       </c>
-      <c r="I16" s="72">
+      <c r="I16" s="73">
         <v>40</v>
       </c>
     </row>
     <row r="17" ht="14" customHeight="1" spans="6:9">
-      <c r="F17" s="73">
+      <c r="F17" s="74">
         <v>9</v>
       </c>
-      <c r="G17" s="75" t="s">
+      <c r="G17" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="72">
+      <c r="H17" s="73">
         <v>3</v>
       </c>
-      <c r="I17" s="72">
+      <c r="I17" s="73">
         <v>24</v>
       </c>
     </row>
     <row r="18" ht="14" customHeight="1" spans="6:9">
-      <c r="F18" s="73">
+      <c r="F18" s="74">
         <v>10</v>
       </c>
-      <c r="G18" s="74" t="s">
+      <c r="G18" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="72">
+      <c r="H18" s="73">
         <v>5</v>
       </c>
-      <c r="I18" s="72">
+      <c r="I18" s="73">
         <v>40</v>
       </c>
     </row>
     <row r="19" ht="15.75" spans="6:9">
-      <c r="F19" s="73">
+      <c r="F19" s="74">
         <v>11</v>
       </c>
-      <c r="G19" s="74" t="s">
+      <c r="G19" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="72">
+      <c r="H19" s="73">
         <v>1</v>
       </c>
-      <c r="I19" s="72">
+      <c r="I19" s="73">
         <v>8</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="6:9">
-      <c r="F20" s="73">
+      <c r="F20" s="74">
         <v>12</v>
       </c>
-      <c r="G20" s="71" t="s">
+      <c r="G20" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="72">
+      <c r="H20" s="73">
         <v>4</v>
       </c>
-      <c r="I20" s="72">
+      <c r="I20" s="73">
         <v>32</v>
       </c>
     </row>
     <row r="21" ht="15.75" spans="6:9">
-      <c r="F21" s="73">
+      <c r="F21" s="74">
         <v>13</v>
       </c>
-      <c r="G21" s="71" t="s">
+      <c r="G21" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="72">
+      <c r="H21" s="73">
         <v>1</v>
       </c>
-      <c r="I21" s="72">
+      <c r="I21" s="73">
         <v>16</v>
       </c>
     </row>
     <row r="22" ht="15.75" spans="6:9">
-      <c r="F22" s="73">
+      <c r="F22" s="74">
         <v>14</v>
       </c>
-      <c r="G22" s="71" t="s">
+      <c r="G22" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="72">
+      <c r="H22" s="73">
         <v>6</v>
       </c>
-      <c r="I22" s="72">
+      <c r="I22" s="73">
         <v>48</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="6:9">
-      <c r="F23" s="73">
+      <c r="F23" s="74">
         <v>15</v>
       </c>
-      <c r="G23" s="75" t="s">
+      <c r="G23" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="72">
+      <c r="H23" s="73">
         <v>2</v>
       </c>
-      <c r="I23" s="72">
+      <c r="I23" s="73">
         <v>16</v>
       </c>
     </row>
     <row r="24" ht="30.75" spans="6:9">
-      <c r="F24" s="73">
+      <c r="F24" s="74">
         <v>16</v>
       </c>
-      <c r="G24" s="75" t="s">
+      <c r="G24" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="72">
+      <c r="H24" s="73">
         <v>4</v>
       </c>
-      <c r="I24" s="72">
+      <c r="I24" s="73">
         <v>32</v>
       </c>
     </row>
     <row r="25" ht="15.75" spans="6:9">
-      <c r="F25" s="76"/>
-      <c r="G25" s="77" t="s">
+      <c r="F25" s="77"/>
+      <c r="G25" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="78">
+      <c r="H25" s="79">
         <f>SUM(H9:H24)</f>
         <v>53</v>
       </c>
-      <c r="I25" s="85">
+      <c r="I25" s="86">
         <f>SUM(I9:I24)</f>
         <v>424</v>
       </c>
@@ -8156,58 +8232,58 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="31"/>
-      <c r="B31" s="79" t="s">
+      <c r="B31" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="80"/>
-      <c r="D31" s="80"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="80">
+      <c r="A32" s="81">
         <v>1</v>
       </c>
-      <c r="B32" s="81" t="s">
+      <c r="B32" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="80">
+      <c r="A33" s="81">
         <v>2</v>
       </c>
-      <c r="B33" s="82" t="s">
+      <c r="B33" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="82"/>
-      <c r="D33" s="82"/>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
     </row>
     <row r="34" ht="15" customHeight="1" spans="1:6">
-      <c r="A34" s="80">
+      <c r="A34" s="81">
         <v>3</v>
       </c>
-      <c r="B34" s="83" t="s">
+      <c r="B34" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="84"/>
     </row>
     <row r="36" customFormat="1" spans="1:4">
       <c r="A36" s="31"/>
-      <c r="B36" s="79" t="s">
+      <c r="B36" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81"/>
     </row>
     <row r="37" customFormat="1" ht="30" customHeight="1" spans="1:6">
-      <c r="A37" s="80">
+      <c r="A37" s="81">
         <v>1</v>
       </c>
       <c r="B37" s="23" t="s">
@@ -8219,40 +8295,40 @@
       <c r="F37" s="23"/>
     </row>
     <row r="38" customFormat="1" ht="29" customHeight="1" spans="1:6">
-      <c r="A38" s="84">
+      <c r="A38" s="85">
         <v>2</v>
       </c>
-      <c r="B38" s="83" t="s">
+      <c r="B38" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="84"/>
+      <c r="F38" s="84"/>
     </row>
     <row r="39" customFormat="1" ht="15" customHeight="1" spans="1:6">
-      <c r="A39" s="84">
+      <c r="A39" s="85">
         <v>3</v>
       </c>
-      <c r="B39" s="83" t="s">
+      <c r="B39" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="83"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
     </row>
     <row r="40" ht="54" customHeight="1" spans="1:6">
-      <c r="A40" s="84">
+      <c r="A40" s="85">
         <v>4</v>
       </c>
-      <c r="B40" s="83" t="s">
+      <c r="B40" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="83"/>
-      <c r="D40" s="83"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="84"/>
+      <c r="F40" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -12735,7 +12811,7 @@
       </c>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:3">
-      <c r="A15" s="60"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="4"/>
       <c r="C15" s="7"/>
     </row>
@@ -12818,77 +12894,77 @@
       <c r="B26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="58" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="13"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="58" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="13"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="58" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
       <c r="A29" s="13"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="58" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="13"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="58" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="13"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="58" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="13"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="57" t="s">
+      <c r="C32" s="58" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="13"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="57" t="s">
+      <c r="C33" s="58" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="13"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="57" t="s">
+      <c r="C34" s="58" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="13"/>
       <c r="B35" s="6"/>
-      <c r="C35" s="57" t="s">
+      <c r="C35" s="58" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" ht="18.75" spans="1:3">
       <c r="A36" s="13"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="57"/>
+      <c r="C36" s="58"/>
     </row>
     <row r="37" ht="15" spans="1:3">
       <c r="A37" s="13" t="s">
@@ -12897,77 +12973,77 @@
       <c r="B37" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="13"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="57" t="s">
+      <c r="C38" s="58" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="13"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="57" t="s">
+      <c r="C39" s="58" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="13"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="57" t="s">
+      <c r="C40" s="58" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="13"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="57" t="s">
+      <c r="C41" s="58" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="13"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="57" t="s">
+      <c r="C42" s="58" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="13"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="57" t="s">
+      <c r="C43" s="58" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="13"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="58" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="13"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="57" t="s">
+      <c r="C45" s="58" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="13"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="57" t="s">
+      <c r="C46" s="58" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="47" ht="12" customHeight="1" spans="1:3">
-      <c r="A47" s="60"/>
+      <c r="A47" s="61"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="57"/>
+      <c r="C47" s="58"/>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="13"/>
@@ -13004,7 +13080,7 @@
       <c r="B52" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="57" t="s">
+      <c r="C52" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13074,7 +13150,7 @@
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="13"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="57" t="s">
+      <c r="C62" s="58" t="s">
         <v>70</v>
       </c>
     </row>
@@ -13088,7 +13164,7 @@
       <c r="B64" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="57" t="s">
+      <c r="C64" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13151,7 +13227,7 @@
     <row r="73" ht="15" spans="1:3">
       <c r="A73" s="13"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="57" t="s">
+      <c r="C73" s="58" t="s">
         <v>70</v>
       </c>
     </row>
@@ -13163,7 +13239,7 @@
       <c r="B75" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C75" s="57" t="s">
+      <c r="C75" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13226,21 +13302,21 @@
     <row r="84" ht="16" customHeight="1" spans="1:3">
       <c r="A84" s="13"/>
       <c r="B84" s="6"/>
-      <c r="C84" s="57" t="s">
+      <c r="C84" s="58" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="85" ht="16" customHeight="1" spans="1:3">
       <c r="A85" s="13"/>
       <c r="B85" s="6"/>
-      <c r="C85" s="57"/>
+      <c r="C85" s="58"/>
     </row>
     <row r="86" ht="16" customHeight="1" spans="1:3">
       <c r="A86" s="13"/>
       <c r="B86" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C86" s="57" t="s">
+      <c r="C86" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13303,7 +13379,7 @@
     <row r="95" ht="15" spans="1:3">
       <c r="A95" s="13"/>
       <c r="B95" s="6"/>
-      <c r="C95" s="57" t="s">
+      <c r="C95" s="58" t="s">
         <v>70</v>
       </c>
     </row>
@@ -13360,7 +13436,7 @@
       <c r="B103" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C103" s="57" t="s">
+      <c r="C103" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13423,7 +13499,7 @@
     <row r="112" ht="15" spans="1:3">
       <c r="A112" s="13"/>
       <c r="B112" s="6"/>
-      <c r="C112" s="57" t="s">
+      <c r="C112" s="58" t="s">
         <v>70</v>
       </c>
     </row>
@@ -13437,7 +13513,7 @@
       <c r="B114" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C114" s="57" t="s">
+      <c r="C114" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13505,7 +13581,7 @@
       <c r="B124" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C124" s="57" t="s">
+      <c r="C124" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13547,21 +13623,21 @@
     <row r="130" ht="16" customHeight="1" spans="1:3">
       <c r="A130" s="13"/>
       <c r="B130" s="6"/>
-      <c r="C130" s="57" t="s">
+      <c r="C130" s="58" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="131" ht="16" customHeight="1" spans="1:3">
       <c r="A131" s="13"/>
       <c r="B131" s="6"/>
-      <c r="C131" s="57"/>
+      <c r="C131" s="58"/>
     </row>
     <row r="132" ht="16" customHeight="1" spans="1:3">
       <c r="A132" s="13"/>
       <c r="B132" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C132" s="57" t="s">
+      <c r="C132" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13617,7 +13693,7 @@
     <row r="140" ht="15" spans="1:3">
       <c r="A140" s="13"/>
       <c r="B140" s="6"/>
-      <c r="C140" s="57" t="s">
+      <c r="C140" s="58" t="s">
         <v>58</v>
       </c>
     </row>
@@ -13660,7 +13736,7 @@
       <c r="B146" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C146" s="57" t="s">
+      <c r="C146" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13723,14 +13799,14 @@
     <row r="155" ht="15" spans="1:3">
       <c r="A155" s="13"/>
       <c r="B155" s="6"/>
-      <c r="C155" s="57" t="s">
+      <c r="C155" s="58" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="156" ht="15" spans="1:3">
       <c r="A156" s="13"/>
       <c r="B156" s="6"/>
-      <c r="C156" s="57" t="s">
+      <c r="C156" s="58" t="s">
         <v>47</v>
       </c>
     </row>
@@ -13744,7 +13820,7 @@
       <c r="B158" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C158" s="57" t="s">
+      <c r="C158" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13805,7 +13881,7 @@
       <c r="B167" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C167" s="57" t="s">
+      <c r="C167" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13847,21 +13923,21 @@
     <row r="173" ht="16" customHeight="1" spans="1:3">
       <c r="A173" s="13"/>
       <c r="B173" s="6"/>
-      <c r="C173" s="57" t="s">
+      <c r="C173" s="58" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="174" ht="16" customHeight="1" spans="1:3">
       <c r="A174" s="13"/>
       <c r="B174" s="6"/>
-      <c r="C174" s="57"/>
+      <c r="C174" s="58"/>
     </row>
     <row r="175" ht="16" customHeight="1" spans="1:3">
       <c r="A175" s="13"/>
       <c r="B175" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C175" s="57" t="s">
+      <c r="C175" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13917,35 +13993,35 @@
     <row r="183" ht="15" spans="1:3">
       <c r="A183" s="13"/>
       <c r="B183" s="6"/>
-      <c r="C183" s="57" t="s">
+      <c r="C183" s="58" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="184" customFormat="1" ht="15" spans="1:3">
       <c r="A184" s="13"/>
       <c r="B184" s="6"/>
-      <c r="C184" s="57" t="s">
+      <c r="C184" s="58" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="185" customFormat="1" ht="15" spans="1:3">
       <c r="A185" s="13"/>
       <c r="B185" s="6"/>
-      <c r="C185" s="57" t="s">
+      <c r="C185" s="58" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="186" customFormat="1" ht="15.75" spans="1:3">
       <c r="A186" s="13"/>
       <c r="B186" s="6"/>
-      <c r="C186" s="57"/>
+      <c r="C186" s="58"/>
     </row>
     <row r="187" customFormat="1" ht="15" spans="1:3">
       <c r="A187" s="13"/>
       <c r="B187" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C187" s="57" t="s">
+      <c r="C187" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -13987,14 +14063,14 @@
     <row r="193" customFormat="1" ht="15" spans="1:3">
       <c r="A193" s="13"/>
       <c r="B193" s="6"/>
-      <c r="C193" s="57" t="s">
+      <c r="C193" s="58" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="194" customFormat="1" ht="15.75" spans="1:3">
       <c r="A194" s="13"/>
       <c r="B194" s="6"/>
-      <c r="C194" s="57"/>
+      <c r="C194" s="58"/>
     </row>
     <row r="195" ht="15" spans="1:3">
       <c r="A195" s="13"/>
@@ -14045,49 +14121,49 @@
       <c r="B201" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C201" s="57" t="s">
+      <c r="C201" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="202" ht="20" customHeight="1" spans="1:3">
       <c r="A202" s="13"/>
       <c r="B202" s="6"/>
-      <c r="C202" s="57" t="s">
+      <c r="C202" s="58" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="203" ht="15" spans="1:3">
       <c r="A203" s="13"/>
       <c r="B203" s="6"/>
-      <c r="C203" s="57" t="s">
+      <c r="C203" s="58" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="204" ht="21" customHeight="1" spans="1:3">
       <c r="A204" s="13"/>
       <c r="B204" s="6"/>
-      <c r="C204" s="57" t="s">
+      <c r="C204" s="58" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="205" ht="15" customHeight="1" spans="1:3">
       <c r="A205" s="13"/>
       <c r="B205" s="6"/>
-      <c r="C205" s="57" t="s">
+      <c r="C205" s="58" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="206" ht="15" spans="1:3">
       <c r="A206" s="13"/>
       <c r="B206" s="6"/>
-      <c r="C206" s="57" t="s">
+      <c r="C206" s="58" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="207" ht="17" customHeight="1" spans="1:3">
       <c r="A207" s="13"/>
       <c r="B207" s="6"/>
-      <c r="C207" s="57" t="s">
+      <c r="C207" s="58" t="s">
         <v>149</v>
       </c>
     </row>
@@ -14098,59 +14174,59 @@
     </row>
     <row r="209" ht="15" spans="1:3">
       <c r="A209" s="13"/>
-      <c r="B209" s="61" t="s">
+      <c r="B209" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="C209" s="57" t="s">
+      <c r="C209" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="210" ht="15" spans="1:3">
       <c r="A210" s="13"/>
-      <c r="B210" s="61"/>
-      <c r="C210" s="57" t="s">
+      <c r="B210" s="62"/>
+      <c r="C210" s="58" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="211" ht="15" spans="1:3">
       <c r="A211" s="13"/>
-      <c r="B211" s="61"/>
-      <c r="C211" s="57" t="s">
+      <c r="B211" s="62"/>
+      <c r="C211" s="58" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="212" ht="15" spans="1:3">
       <c r="A212" s="13"/>
-      <c r="B212" s="61"/>
-      <c r="C212" s="57" t="s">
+      <c r="B212" s="62"/>
+      <c r="C212" s="58" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="213" ht="15" spans="1:3">
       <c r="A213" s="13"/>
-      <c r="B213" s="61"/>
-      <c r="C213" s="57" t="s">
+      <c r="B213" s="62"/>
+      <c r="C213" s="58" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="214" ht="15" spans="1:3">
       <c r="A214" s="13"/>
-      <c r="B214" s="61"/>
-      <c r="C214" s="57" t="s">
+      <c r="B214" s="62"/>
+      <c r="C214" s="58" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="215" ht="15" spans="1:3">
       <c r="A215" s="13"/>
-      <c r="B215" s="61"/>
-      <c r="C215" s="57" t="s">
+      <c r="B215" s="62"/>
+      <c r="C215" s="58" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="216" ht="15" spans="1:3">
       <c r="A216" s="13"/>
-      <c r="B216" s="61"/>
-      <c r="C216" s="57" t="s">
+      <c r="B216" s="62"/>
+      <c r="C216" s="58" t="s">
         <v>70</v>
       </c>
     </row>
@@ -14162,7 +14238,7 @@
       <c r="B218" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C218" s="57" t="s">
+      <c r="C218" s="58" t="s">
         <v>73</v>
       </c>
     </row>
@@ -14204,7 +14280,7 @@
     <row r="224" ht="16" customHeight="1" spans="1:3">
       <c r="A224" s="13"/>
       <c r="B224" s="6"/>
-      <c r="C224" s="57" t="s">
+      <c r="C224" s="58" t="s">
         <v>224</v>
       </c>
     </row>
@@ -14218,21 +14294,21 @@
     <row r="226" ht="16" customHeight="1" spans="1:3">
       <c r="A226" s="13"/>
       <c r="B226" s="6"/>
-      <c r="C226" s="57" t="s">
+      <c r="C226" s="58" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="227" ht="16" customHeight="1" spans="1:3">
       <c r="A227" s="13"/>
       <c r="B227" s="6"/>
-      <c r="C227" s="57" t="s">
+      <c r="C227" s="58" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="228" customFormat="1" ht="15.75" spans="1:3">
       <c r="A228" s="13"/>
       <c r="B228" s="6"/>
-      <c r="C228" s="57"/>
+      <c r="C228" s="58"/>
     </row>
     <row r="229" ht="15" spans="1:3">
       <c r="A229" s="13"/>
@@ -14297,49 +14373,49 @@
     <row r="237" ht="9" customHeight="1" spans="1:3">
       <c r="A237" s="13"/>
       <c r="B237" s="17"/>
-      <c r="C237" s="57"/>
+      <c r="C237" s="58"/>
     </row>
     <row r="238" ht="21" customHeight="1" spans="1:3">
       <c r="A238" s="13"/>
       <c r="B238" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C238" s="57" t="s">
+      <c r="C238" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="239" ht="13" customHeight="1" spans="1:3">
       <c r="A239" s="13"/>
       <c r="B239" s="6"/>
-      <c r="C239" s="57" t="s">
+      <c r="C239" s="58" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="240" ht="17" customHeight="1" spans="1:3">
       <c r="A240" s="13"/>
       <c r="B240" s="6"/>
-      <c r="C240" s="57" t="s">
+      <c r="C240" s="58" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="241" ht="15" spans="1:3">
       <c r="A241" s="13"/>
       <c r="B241" s="6"/>
-      <c r="C241" s="57" t="s">
+      <c r="C241" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="242" ht="15" spans="1:3">
       <c r="A242" s="13"/>
       <c r="B242" s="6"/>
-      <c r="C242" s="57" t="s">
+      <c r="C242" s="58" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="243" ht="15" spans="1:3">
       <c r="A243" s="13"/>
       <c r="B243" s="6"/>
-      <c r="C243" s="57" t="s">
+      <c r="C243" s="58" t="s">
         <v>240</v>
       </c>
     </row>
@@ -14351,49 +14427,49 @@
       <c r="B245" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="C245" s="57" t="s">
+      <c r="C245" s="58" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="246" ht="15" spans="1:3">
       <c r="A246" s="13"/>
       <c r="B246" s="6"/>
-      <c r="C246" s="57" t="s">
+      <c r="C246" s="58" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="247" ht="15" spans="1:3">
       <c r="A247" s="13"/>
       <c r="B247" s="6"/>
-      <c r="C247" s="57" t="s">
+      <c r="C247" s="58" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="248" ht="15" spans="1:3">
       <c r="A248" s="13"/>
       <c r="B248" s="6"/>
-      <c r="C248" s="57" t="s">
+      <c r="C248" s="58" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="249" ht="15" spans="1:3">
       <c r="A249" s="13"/>
       <c r="B249" s="6"/>
-      <c r="C249" s="57" t="s">
+      <c r="C249" s="58" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="250" ht="15" spans="1:3">
       <c r="A250" s="13"/>
       <c r="B250" s="6"/>
-      <c r="C250" s="57" t="s">
+      <c r="C250" s="58" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="251" ht="15.75" spans="1:3">
       <c r="A251" s="13"/>
       <c r="B251" s="6"/>
-      <c r="C251" s="57"/>
+      <c r="C251" s="58"/>
     </row>
     <row r="252" ht="15" spans="1:3">
       <c r="A252" s="13"/>
@@ -14988,134 +15064,134 @@
       <c r="C337" s="2"/>
     </row>
     <row r="338" ht="15" spans="1:3">
-      <c r="A338" s="62" t="s">
+      <c r="A338" s="63" t="s">
         <v>319</v>
       </c>
-      <c r="B338" s="61" t="s">
+      <c r="B338" s="62" t="s">
         <v>320</v>
       </c>
-      <c r="C338" s="57" t="s">
+      <c r="C338" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="339" spans="1:3">
-      <c r="A339" s="62"/>
-      <c r="B339" s="61"/>
+      <c r="A339" s="63"/>
+      <c r="B339" s="62"/>
       <c r="C339" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="340" ht="15" spans="1:3">
-      <c r="A340" s="62"/>
-      <c r="B340" s="61"/>
-      <c r="C340" s="57" t="s">
+      <c r="A340" s="63"/>
+      <c r="B340" s="62"/>
+      <c r="C340" s="58" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="341" ht="15" spans="1:3">
-      <c r="A341" s="62"/>
-      <c r="B341" s="61"/>
-      <c r="C341" s="57" t="s">
+      <c r="A341" s="63"/>
+      <c r="B341" s="62"/>
+      <c r="C341" s="58" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="342" ht="15" spans="1:3">
-      <c r="A342" s="62"/>
-      <c r="B342" s="61"/>
-      <c r="C342" s="57" t="s">
+      <c r="A342" s="63"/>
+      <c r="B342" s="62"/>
+      <c r="C342" s="58" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="343" ht="15" spans="1:3">
-      <c r="A343" s="62"/>
-      <c r="B343" s="61"/>
-      <c r="C343" s="57" t="s">
+      <c r="A343" s="63"/>
+      <c r="B343" s="62"/>
+      <c r="C343" s="58" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="344" ht="15" spans="1:3">
-      <c r="A344" s="62"/>
-      <c r="B344" s="61"/>
-      <c r="C344" s="57" t="s">
+      <c r="A344" s="63"/>
+      <c r="B344" s="62"/>
+      <c r="C344" s="58" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="345" ht="15" spans="1:3">
-      <c r="A345" s="62"/>
-      <c r="B345" s="61"/>
-      <c r="C345" s="57" t="s">
+      <c r="A345" s="63"/>
+      <c r="B345" s="62"/>
+      <c r="C345" s="58" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="346" ht="15" spans="1:3">
-      <c r="A346" s="62"/>
-      <c r="B346" s="61"/>
-      <c r="C346" s="57" t="s">
+      <c r="A346" s="63"/>
+      <c r="B346" s="62"/>
+      <c r="C346" s="58" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="347" ht="15" spans="1:3">
-      <c r="A347" s="62"/>
-      <c r="B347" s="61"/>
-      <c r="C347" s="57" t="s">
+      <c r="A347" s="63"/>
+      <c r="B347" s="62"/>
+      <c r="C347" s="58" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="348" ht="15" spans="1:3">
-      <c r="A348" s="62"/>
-      <c r="B348" s="61"/>
-      <c r="C348" s="57" t="s">
+      <c r="A348" s="63"/>
+      <c r="B348" s="62"/>
+      <c r="C348" s="58" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="349" ht="15" spans="1:3">
-      <c r="A349" s="62"/>
-      <c r="B349" s="61"/>
-      <c r="C349" s="57" t="s">
+      <c r="A349" s="63"/>
+      <c r="B349" s="62"/>
+      <c r="C349" s="58" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="350" ht="15" spans="1:3">
-      <c r="A350" s="62"/>
-      <c r="B350" s="61"/>
-      <c r="C350" s="57" t="s">
+      <c r="A350" s="63"/>
+      <c r="B350" s="62"/>
+      <c r="C350" s="58" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="351" ht="15" spans="1:3">
-      <c r="A351" s="62"/>
-      <c r="B351" s="61"/>
-      <c r="C351" s="57" t="s">
+      <c r="A351" s="63"/>
+      <c r="B351" s="62"/>
+      <c r="C351" s="58" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="352" spans="1:3">
-      <c r="A352" s="62"/>
-      <c r="B352" s="61"/>
+      <c r="A352" s="63"/>
+      <c r="B352" s="62"/>
       <c r="C352" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="353" spans="1:3">
-      <c r="A353" s="62"/>
-      <c r="B353" s="61"/>
+      <c r="A353" s="63"/>
+      <c r="B353" s="62"/>
       <c r="C353" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="354" spans="1:3">
-      <c r="A354" s="62"/>
-      <c r="B354" s="61"/>
+      <c r="A354" s="63"/>
+      <c r="B354" s="62"/>
       <c r="C354" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="355" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A355" s="62"/>
-      <c r="B355" s="61"/>
+      <c r="A355" s="63"/>
+      <c r="B355" s="62"/>
     </row>
     <row r="356" ht="15" spans="1:3">
-      <c r="A356" s="62"/>
+      <c r="A356" s="63"/>
       <c r="B356" s="14" t="s">
         <v>22</v>
       </c>
@@ -15124,71 +15200,71 @@
       </c>
     </row>
     <row r="357" spans="1:3">
-      <c r="A357" s="62"/>
+      <c r="A357" s="63"/>
       <c r="B357" s="14"/>
       <c r="C357" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="359" ht="15" spans="1:3">
-      <c r="A359" s="62" t="s">
+      <c r="A359" s="63" t="s">
         <v>339</v>
       </c>
-      <c r="B359" s="61" t="s">
+      <c r="B359" s="62" t="s">
         <v>340</v>
       </c>
-      <c r="C359" s="57" t="s">
+      <c r="C359" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="360" spans="1:3">
-      <c r="A360" s="62"/>
-      <c r="B360" s="61"/>
+      <c r="A360" s="63"/>
+      <c r="B360" s="62"/>
       <c r="C360" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="361" ht="15" spans="1:3">
-      <c r="A361" s="62"/>
-      <c r="B361" s="61"/>
-      <c r="C361" s="57" t="s">
+      <c r="A361" s="63"/>
+      <c r="B361" s="62"/>
+      <c r="C361" s="58" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="362" ht="15" spans="1:3">
-      <c r="A362" s="62"/>
-      <c r="B362" s="61"/>
-      <c r="C362" s="57" t="s">
+      <c r="A362" s="63"/>
+      <c r="B362" s="62"/>
+      <c r="C362" s="58" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="363" ht="15" spans="1:3">
-      <c r="A363" s="62"/>
-      <c r="B363" s="61"/>
-      <c r="C363" s="57" t="s">
+      <c r="A363" s="63"/>
+      <c r="B363" s="62"/>
+      <c r="C363" s="58" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="364" ht="15" spans="1:3">
-      <c r="A364" s="62"/>
-      <c r="B364" s="61"/>
-      <c r="C364" s="57" t="s">
+      <c r="A364" s="63"/>
+      <c r="B364" s="62"/>
+      <c r="C364" s="58" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="365" spans="1:3">
-      <c r="A365" s="62"/>
-      <c r="B365" s="61"/>
+      <c r="A365" s="63"/>
+      <c r="B365" s="62"/>
       <c r="C365" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="366" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A366" s="62"/>
-      <c r="B366" s="61"/>
+      <c r="A366" s="63"/>
+      <c r="B366" s="62"/>
     </row>
     <row r="367" ht="15" spans="1:3">
-      <c r="A367" s="62"/>
+      <c r="A367" s="63"/>
       <c r="B367" s="14" t="s">
         <v>22</v>
       </c>
@@ -15197,7 +15273,7 @@
       </c>
     </row>
     <row r="368" spans="1:3">
-      <c r="A368" s="62"/>
+      <c r="A368" s="63"/>
       <c r="B368" s="14"/>
       <c r="C368" t="s">
         <v>346</v>
@@ -15207,179 +15283,179 @@
       <c r="A370" s="50" t="s">
         <v>347</v>
       </c>
-      <c r="B370" s="63" t="s">
+      <c r="B370" s="64" t="s">
         <v>348</v>
       </c>
-      <c r="C370" s="57" t="s">
+      <c r="C370" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="371" ht="15" spans="1:3">
-      <c r="A371" s="64"/>
-      <c r="B371" s="63"/>
-      <c r="C371" s="57" t="s">
+      <c r="A371" s="65"/>
+      <c r="B371" s="64"/>
+      <c r="C371" s="58" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="372" ht="15" spans="1:3">
-      <c r="A372" s="64"/>
-      <c r="B372" s="63"/>
-      <c r="C372" s="57" t="s">
+      <c r="A372" s="65"/>
+      <c r="B372" s="64"/>
+      <c r="C372" s="58" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="373" ht="15" spans="1:3">
-      <c r="A373" s="64"/>
-      <c r="B373" s="63"/>
-      <c r="C373" s="57" t="s">
+      <c r="A373" s="65"/>
+      <c r="B373" s="64"/>
+      <c r="C373" s="58" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="374" ht="15" spans="1:3">
-      <c r="A374" s="64"/>
-      <c r="B374" s="63"/>
-      <c r="C374" s="57" t="s">
+      <c r="A374" s="65"/>
+      <c r="B374" s="64"/>
+      <c r="C374" s="58" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="375" ht="15" spans="1:3">
-      <c r="A375" s="64"/>
-      <c r="B375" s="63"/>
-      <c r="C375" s="65" t="s">
+      <c r="A375" s="65"/>
+      <c r="B375" s="64"/>
+      <c r="C375" s="66" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="376" ht="15" spans="1:3">
-      <c r="A376" s="64"/>
-      <c r="B376" s="63"/>
-      <c r="C376" s="57" t="s">
+      <c r="A376" s="65"/>
+      <c r="B376" s="64"/>
+      <c r="C376" s="58" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="377" ht="15" spans="1:3">
-      <c r="A377" s="64"/>
-      <c r="B377" s="63"/>
-      <c r="C377" s="65" t="s">
+      <c r="A377" s="65"/>
+      <c r="B377" s="64"/>
+      <c r="C377" s="66" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="378" ht="15" spans="1:3">
-      <c r="A378" s="64"/>
-      <c r="B378" s="63"/>
-      <c r="C378" s="57" t="s">
+      <c r="A378" s="65"/>
+      <c r="B378" s="64"/>
+      <c r="C378" s="58" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="379" ht="15" spans="1:3">
-      <c r="A379" s="64"/>
-      <c r="B379" s="63"/>
-      <c r="C379" s="65" t="s">
+      <c r="A379" s="65"/>
+      <c r="B379" s="64"/>
+      <c r="C379" s="66" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="380" ht="15" spans="1:3">
-      <c r="A380" s="64"/>
-      <c r="B380" s="63"/>
-      <c r="C380" s="57" t="s">
+      <c r="A380" s="65"/>
+      <c r="B380" s="64"/>
+      <c r="C380" s="58" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="381" ht="15" spans="1:3">
-      <c r="A381" s="64"/>
-      <c r="B381" s="63"/>
-      <c r="C381" s="65" t="s">
+      <c r="A381" s="65"/>
+      <c r="B381" s="64"/>
+      <c r="C381" s="66" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="382" ht="15" spans="1:3">
-      <c r="A382" s="64"/>
-      <c r="B382" s="63"/>
-      <c r="C382" s="57" t="s">
+      <c r="A382" s="65"/>
+      <c r="B382" s="64"/>
+      <c r="C382" s="58" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="383" ht="15" spans="1:3">
-      <c r="A383" s="64"/>
-      <c r="B383" s="63"/>
-      <c r="C383" s="57" t="s">
+      <c r="A383" s="65"/>
+      <c r="B383" s="64"/>
+      <c r="C383" s="58" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="384" ht="15" spans="1:3">
-      <c r="A384" s="64"/>
-      <c r="B384" s="63"/>
-      <c r="C384" s="57" t="s">
+      <c r="A384" s="65"/>
+      <c r="B384" s="64"/>
+      <c r="C384" s="58" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="385" ht="15" spans="1:3">
-      <c r="A385" s="64"/>
-      <c r="B385" s="63"/>
-      <c r="C385" s="57" t="s">
+      <c r="A385" s="65"/>
+      <c r="B385" s="64"/>
+      <c r="C385" s="58" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="386" ht="15" spans="1:3">
-      <c r="A386" s="64"/>
-      <c r="B386" s="63"/>
-      <c r="C386" s="57" t="s">
+      <c r="A386" s="65"/>
+      <c r="B386" s="64"/>
+      <c r="C386" s="58" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="387" ht="15" spans="1:3">
-      <c r="A387" s="64"/>
-      <c r="B387" s="63"/>
-      <c r="C387" s="57" t="s">
+      <c r="A387" s="65"/>
+      <c r="B387" s="64"/>
+      <c r="C387" s="58" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="388" ht="15" spans="1:3">
-      <c r="A388" s="64"/>
-      <c r="B388" s="63"/>
-      <c r="C388" s="57" t="s">
+      <c r="A388" s="65"/>
+      <c r="B388" s="64"/>
+      <c r="C388" s="58" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="389" ht="15" spans="1:3">
-      <c r="A389" s="64"/>
-      <c r="B389" s="63"/>
-      <c r="C389" s="57" t="s">
+      <c r="A389" s="65"/>
+      <c r="B389" s="64"/>
+      <c r="C389" s="58" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="390" spans="1:3">
-      <c r="A390" s="64"/>
-      <c r="B390" s="63"/>
+      <c r="A390" s="65"/>
+      <c r="B390" s="64"/>
       <c r="C390" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="391" spans="1:3">
-      <c r="A391" s="64"/>
-      <c r="B391" s="63"/>
+      <c r="A391" s="65"/>
+      <c r="B391" s="64"/>
       <c r="C391" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="392" spans="1:3">
-      <c r="A392" s="64"/>
-      <c r="B392" s="63"/>
+      <c r="A392" s="65"/>
+      <c r="B392" s="64"/>
       <c r="C392" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="393" spans="1:3">
-      <c r="A393" s="64"/>
-      <c r="B393" s="63"/>
+      <c r="A393" s="65"/>
+      <c r="B393" s="64"/>
       <c r="C393" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="394" customFormat="1" spans="1:1">
-      <c r="A394" s="64"/>
+      <c r="A394" s="65"/>
     </row>
     <row r="395" ht="15" spans="1:3">
-      <c r="A395" s="64"/>
+      <c r="A395" s="65"/>
       <c r="B395" s="14" t="s">
         <v>22</v>
       </c>
@@ -15388,42 +15464,42 @@
       </c>
     </row>
     <row r="396" ht="15" spans="1:3">
-      <c r="A396" s="64"/>
+      <c r="A396" s="65"/>
       <c r="B396" s="14"/>
       <c r="C396" s="7" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="397" ht="15" spans="1:3">
-      <c r="A397" s="64"/>
+      <c r="A397" s="65"/>
       <c r="B397" s="14"/>
       <c r="C397" s="7" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="398" ht="15" spans="1:3">
-      <c r="A398" s="64"/>
+      <c r="A398" s="65"/>
       <c r="B398" s="14"/>
       <c r="C398" s="7" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="399" ht="15" spans="1:3">
-      <c r="A399" s="64"/>
+      <c r="A399" s="65"/>
       <c r="B399" s="14"/>
       <c r="C399" s="7" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="400" ht="15" spans="1:3">
-      <c r="A400" s="64"/>
+      <c r="A400" s="65"/>
       <c r="B400" s="14"/>
       <c r="C400" s="7" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="401" ht="15" spans="1:3">
-      <c r="A401" s="64"/>
+      <c r="A401" s="65"/>
       <c r="B401" s="14"/>
       <c r="C401" s="7" t="s">
         <v>378</v>
@@ -15442,345 +15518,345 @@
       <c r="C403" s="2"/>
     </row>
     <row r="404" ht="15" spans="1:3">
-      <c r="A404" s="66" t="s">
+      <c r="A404" s="67" t="s">
         <v>380</v>
       </c>
-      <c r="B404" s="63" t="s">
+      <c r="B404" s="64" t="s">
         <v>381</v>
       </c>
-      <c r="C404" s="57" t="s">
+      <c r="C404" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="405" ht="15" spans="1:3">
-      <c r="A405" s="66"/>
-      <c r="B405" s="63"/>
-      <c r="C405" s="57" t="s">
+      <c r="A405" s="67"/>
+      <c r="B405" s="64"/>
+      <c r="C405" s="58" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="406" ht="15" spans="1:3">
-      <c r="A406" s="66"/>
-      <c r="B406" s="63"/>
-      <c r="C406" s="57" t="s">
+      <c r="A406" s="67"/>
+      <c r="B406" s="64"/>
+      <c r="C406" s="58" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="407" ht="15" spans="1:3">
-      <c r="A407" s="66"/>
-      <c r="B407" s="63"/>
-      <c r="C407" s="57" t="s">
+      <c r="A407" s="67"/>
+      <c r="B407" s="64"/>
+      <c r="C407" s="58" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="408" ht="15" spans="1:3">
-      <c r="A408" s="66"/>
-      <c r="B408" s="63"/>
-      <c r="C408" s="57" t="s">
+      <c r="A408" s="67"/>
+      <c r="B408" s="64"/>
+      <c r="C408" s="58" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="409" ht="15" spans="1:3">
-      <c r="A409" s="66"/>
-      <c r="B409" s="63"/>
-      <c r="C409" s="57" t="s">
+      <c r="A409" s="67"/>
+      <c r="B409" s="64"/>
+      <c r="C409" s="58" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="410" ht="15" spans="1:3">
-      <c r="A410" s="66"/>
-      <c r="B410" s="63"/>
-      <c r="C410" s="57" t="s">
+      <c r="A410" s="67"/>
+      <c r="B410" s="64"/>
+      <c r="C410" s="58" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="411" ht="15" spans="1:3">
-      <c r="A411" s="66"/>
-      <c r="B411" s="63"/>
-      <c r="C411" s="57" t="s">
+      <c r="A411" s="67"/>
+      <c r="B411" s="64"/>
+      <c r="C411" s="58" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="412" ht="15" spans="1:3">
-      <c r="A412" s="66"/>
-      <c r="B412" s="63"/>
-      <c r="C412" s="57" t="s">
+      <c r="A412" s="67"/>
+      <c r="B412" s="64"/>
+      <c r="C412" s="58" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="413" ht="15" spans="1:3">
-      <c r="A413" s="66"/>
-      <c r="B413" s="63"/>
-      <c r="C413" s="57" t="s">
+      <c r="A413" s="67"/>
+      <c r="B413" s="64"/>
+      <c r="C413" s="58" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="414" ht="15" spans="1:3">
-      <c r="A414" s="66"/>
-      <c r="B414" s="63"/>
-      <c r="C414" s="57" t="s">
+      <c r="A414" s="67"/>
+      <c r="B414" s="64"/>
+      <c r="C414" s="58" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="415" ht="15" spans="1:3">
-      <c r="A415" s="66"/>
-      <c r="B415" s="63"/>
-      <c r="C415" s="57" t="s">
+      <c r="A415" s="67"/>
+      <c r="B415" s="64"/>
+      <c r="C415" s="58" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="416" ht="15" spans="1:3">
-      <c r="A416" s="66"/>
-      <c r="B416" s="63"/>
-      <c r="C416" s="57" t="s">
+      <c r="A416" s="67"/>
+      <c r="B416" s="64"/>
+      <c r="C416" s="58" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="417" ht="15" spans="1:3">
-      <c r="A417" s="66"/>
-      <c r="B417" s="63"/>
-      <c r="C417" s="57" t="s">
+      <c r="A417" s="67"/>
+      <c r="B417" s="64"/>
+      <c r="C417" s="58" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="418" ht="15" spans="1:3">
-      <c r="A418" s="66"/>
-      <c r="B418" s="63"/>
-      <c r="C418" s="57" t="s">
+      <c r="A418" s="67"/>
+      <c r="B418" s="64"/>
+      <c r="C418" s="58" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="419" ht="15" spans="1:3">
-      <c r="A419" s="66"/>
-      <c r="B419" s="63"/>
-      <c r="C419" s="57" t="s">
+      <c r="A419" s="67"/>
+      <c r="B419" s="64"/>
+      <c r="C419" s="58" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="420" ht="15" spans="1:3">
-      <c r="A420" s="66"/>
-      <c r="B420" s="63"/>
-      <c r="C420" s="57" t="s">
+      <c r="A420" s="67"/>
+      <c r="B420" s="64"/>
+      <c r="C420" s="58" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="421" ht="15" spans="1:3">
-      <c r="A421" s="66"/>
-      <c r="B421" s="63"/>
-      <c r="C421" s="57" t="s">
+      <c r="A421" s="67"/>
+      <c r="B421" s="64"/>
+      <c r="C421" s="58" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="422" ht="18" spans="1:3">
-      <c r="A422" s="66"/>
-      <c r="B422" s="63"/>
-      <c r="C422" s="57"/>
+      <c r="A422" s="67"/>
+      <c r="B422" s="64"/>
+      <c r="C422" s="58"/>
     </row>
     <row r="423" ht="15" spans="1:3">
-      <c r="A423" s="66"/>
-      <c r="B423" s="63" t="s">
+      <c r="A423" s="67"/>
+      <c r="B423" s="64" t="s">
         <v>399</v>
       </c>
-      <c r="C423" s="57" t="s">
+      <c r="C423" s="58" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="424" ht="15" spans="1:3">
-      <c r="A424" s="66"/>
-      <c r="B424" s="63"/>
-      <c r="C424" s="57" t="s">
+      <c r="A424" s="67"/>
+      <c r="B424" s="64"/>
+      <c r="C424" s="58" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="425" ht="15" spans="1:3">
-      <c r="A425" s="66"/>
-      <c r="B425" s="63"/>
-      <c r="C425" s="57" t="s">
+      <c r="A425" s="67"/>
+      <c r="B425" s="64"/>
+      <c r="C425" s="58" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="426" ht="15" spans="1:3">
-      <c r="A426" s="66"/>
-      <c r="B426" s="63"/>
-      <c r="C426" s="57" t="s">
+      <c r="A426" s="67"/>
+      <c r="B426" s="64"/>
+      <c r="C426" s="58" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="427" ht="15" spans="1:3">
-      <c r="A427" s="66"/>
-      <c r="B427" s="63"/>
-      <c r="C427" s="57" t="s">
+      <c r="A427" s="67"/>
+      <c r="B427" s="64"/>
+      <c r="C427" s="58" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="428" ht="15" spans="1:3">
-      <c r="A428" s="66"/>
-      <c r="B428" s="63"/>
-      <c r="C428" s="57" t="s">
+      <c r="A428" s="67"/>
+      <c r="B428" s="64"/>
+      <c r="C428" s="58" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="429" ht="15" spans="1:3">
-      <c r="A429" s="66"/>
-      <c r="B429" s="63"/>
-      <c r="C429" s="57" t="s">
+      <c r="A429" s="67"/>
+      <c r="B429" s="64"/>
+      <c r="C429" s="58" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="430" ht="15" spans="1:3">
-      <c r="A430" s="66"/>
-      <c r="B430" s="63"/>
-      <c r="C430" s="57" t="s">
+      <c r="A430" s="67"/>
+      <c r="B430" s="64"/>
+      <c r="C430" s="58" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="431" ht="15" spans="1:3">
-      <c r="A431" s="66"/>
-      <c r="B431" s="63"/>
-      <c r="C431" s="57" t="s">
+      <c r="A431" s="67"/>
+      <c r="B431" s="64"/>
+      <c r="C431" s="58" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="432" ht="15" spans="1:3">
-      <c r="A432" s="66"/>
-      <c r="B432" s="63"/>
-      <c r="C432" s="57" t="s">
+      <c r="A432" s="67"/>
+      <c r="B432" s="64"/>
+      <c r="C432" s="58" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="433" ht="15" spans="1:3">
-      <c r="A433" s="66"/>
-      <c r="B433" s="63"/>
-      <c r="C433" s="57" t="s">
+      <c r="A433" s="67"/>
+      <c r="B433" s="64"/>
+      <c r="C433" s="58" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="434" ht="15" spans="1:3">
-      <c r="A434" s="66"/>
-      <c r="B434" s="63"/>
-      <c r="C434" s="57" t="s">
+      <c r="A434" s="67"/>
+      <c r="B434" s="64"/>
+      <c r="C434" s="58" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="435" ht="15" spans="1:3">
-      <c r="A435" s="66"/>
-      <c r="B435" s="63"/>
-      <c r="C435" s="57" t="s">
+      <c r="A435" s="67"/>
+      <c r="B435" s="64"/>
+      <c r="C435" s="58" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="436" ht="15" spans="1:3">
-      <c r="A436" s="66"/>
-      <c r="B436" s="63"/>
-      <c r="C436" s="57" t="s">
+      <c r="A436" s="67"/>
+      <c r="B436" s="64"/>
+      <c r="C436" s="58" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="437" ht="15" spans="1:3">
-      <c r="A437" s="66"/>
-      <c r="B437" s="63"/>
-      <c r="C437" s="57" t="s">
+      <c r="A437" s="67"/>
+      <c r="B437" s="64"/>
+      <c r="C437" s="58" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="438" ht="15" spans="1:3">
-      <c r="A438" s="66"/>
-      <c r="B438" s="63"/>
-      <c r="C438" s="57" t="s">
+      <c r="A438" s="67"/>
+      <c r="B438" s="64"/>
+      <c r="C438" s="58" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="439" ht="15" spans="1:3">
-      <c r="A439" s="66"/>
-      <c r="B439" s="63"/>
-      <c r="C439" s="57" t="s">
+      <c r="A439" s="67"/>
+      <c r="B439" s="64"/>
+      <c r="C439" s="58" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="440" ht="18" spans="1:3">
-      <c r="A440" s="66"/>
-      <c r="B440" s="63"/>
-      <c r="C440" s="57"/>
+      <c r="A440" s="67"/>
+      <c r="B440" s="64"/>
+      <c r="C440" s="58"/>
     </row>
     <row r="441" ht="15" spans="1:3">
-      <c r="A441" s="66"/>
-      <c r="B441" s="63" t="s">
+      <c r="A441" s="67"/>
+      <c r="B441" s="64" t="s">
         <v>416</v>
       </c>
-      <c r="C441" s="57" t="s">
+      <c r="C441" s="58" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="442" ht="15" spans="1:3">
-      <c r="A442" s="66"/>
-      <c r="B442" s="63"/>
-      <c r="C442" s="57" t="s">
+      <c r="A442" s="67"/>
+      <c r="B442" s="64"/>
+      <c r="C442" s="58" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="443" ht="15" spans="1:3">
-      <c r="A443" s="66"/>
-      <c r="B443" s="63"/>
-      <c r="C443" s="57" t="s">
+      <c r="A443" s="67"/>
+      <c r="B443" s="64"/>
+      <c r="C443" s="58" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="444" ht="15" spans="1:3">
-      <c r="A444" s="66"/>
-      <c r="B444" s="63"/>
-      <c r="C444" s="57" t="s">
+      <c r="A444" s="67"/>
+      <c r="B444" s="64"/>
+      <c r="C444" s="58" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="445" ht="15" spans="1:3">
-      <c r="A445" s="66"/>
-      <c r="B445" s="63"/>
-      <c r="C445" s="57" t="s">
+      <c r="A445" s="67"/>
+      <c r="B445" s="64"/>
+      <c r="C445" s="58" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="446" ht="15" spans="1:3">
-      <c r="A446" s="66"/>
-      <c r="B446" s="63"/>
-      <c r="C446" s="57" t="s">
+      <c r="A446" s="67"/>
+      <c r="B446" s="64"/>
+      <c r="C446" s="58" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="447" ht="15" spans="1:3">
-      <c r="A447" s="66"/>
-      <c r="B447" s="63"/>
-      <c r="C447" s="57" t="s">
+      <c r="A447" s="67"/>
+      <c r="B447" s="64"/>
+      <c r="C447" s="58" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="448" ht="15" spans="1:3">
-      <c r="A448" s="66"/>
-      <c r="B448" s="63"/>
-      <c r="C448" s="57" t="s">
+      <c r="A448" s="67"/>
+      <c r="B448" s="64"/>
+      <c r="C448" s="58" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="449" ht="15" spans="1:3">
-      <c r="A449" s="66"/>
-      <c r="B449" s="63"/>
-      <c r="C449" s="57" t="s">
+      <c r="A449" s="67"/>
+      <c r="B449" s="64"/>
+      <c r="C449" s="58" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="450" ht="15" spans="1:3">
-      <c r="A450" s="66"/>
-      <c r="B450" s="63"/>
-      <c r="C450" s="57" t="s">
+      <c r="A450" s="67"/>
+      <c r="B450" s="64"/>
+      <c r="C450" s="58" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="451" ht="18" spans="1:3">
-      <c r="A451" s="66"/>
-      <c r="B451" s="67"/>
-      <c r="C451" s="57"/>
+      <c r="A451" s="67"/>
+      <c r="B451" s="68"/>
+      <c r="C451" s="58"/>
     </row>
     <row r="452" ht="15" spans="1:3">
-      <c r="A452" s="66"/>
+      <c r="A452" s="67"/>
       <c r="B452" s="14" t="s">
         <v>22</v>
       </c>
@@ -15789,35 +15865,35 @@
       </c>
     </row>
     <row r="453" ht="15" spans="1:3">
-      <c r="A453" s="66"/>
+      <c r="A453" s="67"/>
       <c r="B453" s="14"/>
       <c r="C453" s="7" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="454" ht="15" spans="1:3">
-      <c r="A454" s="66"/>
+      <c r="A454" s="67"/>
       <c r="B454" s="14"/>
       <c r="C454" s="15" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="455" ht="15" spans="1:3">
-      <c r="A455" s="66"/>
+      <c r="A455" s="67"/>
       <c r="B455" s="14"/>
       <c r="C455" s="7" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="456" ht="15" spans="1:3">
-      <c r="A456" s="66"/>
+      <c r="A456" s="67"/>
       <c r="B456" s="14"/>
       <c r="C456" s="15" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="457" ht="15" spans="1:3">
-      <c r="A457" s="66"/>
+      <c r="A457" s="67"/>
       <c r="B457" s="14"/>
       <c r="C457" s="7" t="s">
         <v>430</v>
@@ -16141,115 +16217,115 @@
     </row>
     <row r="503" ht="15" spans="1:3">
       <c r="A503" s="13"/>
-      <c r="B503" s="63" t="s">
+      <c r="B503" s="64" t="s">
         <v>472</v>
       </c>
-      <c r="C503" s="57" t="s">
+      <c r="C503" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="504" spans="1:3">
       <c r="A504" s="13"/>
-      <c r="B504" s="63"/>
+      <c r="B504" s="64"/>
       <c r="C504" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="505" ht="15" spans="1:3">
       <c r="A505" s="13"/>
-      <c r="B505" s="63"/>
-      <c r="C505" s="57" t="s">
+      <c r="B505" s="64"/>
+      <c r="C505" s="58" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="506" ht="15" spans="1:3">
       <c r="A506" s="13"/>
-      <c r="B506" s="63"/>
-      <c r="C506" s="57" t="s">
+      <c r="B506" s="64"/>
+      <c r="C506" s="58" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="507" ht="15" spans="1:3">
       <c r="A507" s="13"/>
-      <c r="B507" s="63"/>
-      <c r="C507" s="57" t="s">
+      <c r="B507" s="64"/>
+      <c r="C507" s="58" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="508" ht="15" spans="1:3">
       <c r="A508" s="13"/>
-      <c r="B508" s="63"/>
-      <c r="C508" s="57" t="s">
+      <c r="B508" s="64"/>
+      <c r="C508" s="58" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="509" ht="18" spans="1:3">
       <c r="A509" s="13"/>
-      <c r="B509" s="63"/>
-      <c r="C509" s="57"/>
+      <c r="B509" s="64"/>
+      <c r="C509" s="58"/>
     </row>
     <row r="510" ht="15" spans="1:3">
       <c r="A510" s="13"/>
-      <c r="B510" s="63" t="s">
+      <c r="B510" s="64" t="s">
         <v>478</v>
       </c>
-      <c r="C510" s="58" t="s">
+      <c r="C510" s="59" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="511" ht="15" spans="1:3">
       <c r="A511" s="13"/>
-      <c r="B511" s="63"/>
-      <c r="C511" s="57" t="s">
+      <c r="B511" s="64"/>
+      <c r="C511" s="58" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="512" ht="15" spans="1:3">
       <c r="A512" s="13"/>
-      <c r="B512" s="63"/>
-      <c r="C512" s="57" t="s">
+      <c r="B512" s="64"/>
+      <c r="C512" s="58" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="513" ht="15" spans="1:3">
       <c r="A513" s="13"/>
-      <c r="B513" s="63"/>
-      <c r="C513" s="57" t="s">
+      <c r="B513" s="64"/>
+      <c r="C513" s="58" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="514" ht="15" spans="1:3">
       <c r="A514" s="13"/>
-      <c r="B514" s="63"/>
-      <c r="C514" s="57" t="s">
+      <c r="B514" s="64"/>
+      <c r="C514" s="58" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="515" ht="15" spans="1:3">
       <c r="A515" s="13"/>
-      <c r="B515" s="63"/>
-      <c r="C515" s="57" t="s">
+      <c r="B515" s="64"/>
+      <c r="C515" s="58" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="516" ht="15" spans="1:3">
       <c r="A516" s="13"/>
-      <c r="B516" s="63"/>
-      <c r="C516" s="57" t="s">
+      <c r="B516" s="64"/>
+      <c r="C516" s="58" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="517" ht="15" spans="1:3">
       <c r="A517" s="13"/>
-      <c r="B517" s="63"/>
-      <c r="C517" s="57" t="s">
+      <c r="B517" s="64"/>
+      <c r="C517" s="58" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="518" ht="18" spans="1:3">
       <c r="A518" s="13"/>
-      <c r="B518" s="63"/>
-      <c r="C518" s="57"/>
+      <c r="B518" s="64"/>
+      <c r="C518" s="58"/>
     </row>
     <row r="519" ht="15" spans="1:3">
       <c r="A519" s="13"/>
@@ -16263,28 +16339,28 @@
     <row r="520" ht="15" spans="1:3">
       <c r="A520" s="13"/>
       <c r="B520" s="6"/>
-      <c r="C520" s="57" t="s">
+      <c r="C520" s="58" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="521" ht="15" spans="1:3">
       <c r="A521" s="13"/>
       <c r="B521" s="6"/>
-      <c r="C521" s="57" t="s">
+      <c r="C521" s="58" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="522" ht="15" spans="1:3">
       <c r="A522" s="13"/>
       <c r="B522" s="6"/>
-      <c r="C522" s="57" t="s">
+      <c r="C522" s="58" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="523" ht="18" spans="1:3">
       <c r="A523" s="13"/>
       <c r="B523" s="17"/>
-      <c r="C523" s="57"/>
+      <c r="C523" s="58"/>
     </row>
     <row r="524" ht="15" spans="1:3">
       <c r="A524" s="13"/>
@@ -16325,77 +16401,77 @@
     </row>
     <row r="529" ht="15" spans="1:3">
       <c r="A529" s="13"/>
-      <c r="B529" s="63" t="s">
+      <c r="B529" s="64" t="s">
         <v>495</v>
       </c>
-      <c r="C529" s="57" t="s">
+      <c r="C529" s="58" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="530" spans="1:3">
       <c r="A530" s="13"/>
-      <c r="B530" s="63"/>
+      <c r="B530" s="64"/>
       <c r="C530" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="531" ht="15" spans="1:3">
       <c r="A531" s="13"/>
-      <c r="B531" s="63"/>
-      <c r="C531" s="57" t="s">
+      <c r="B531" s="64"/>
+      <c r="C531" s="58" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="532" ht="15" spans="1:3">
       <c r="A532" s="13"/>
-      <c r="B532" s="63"/>
-      <c r="C532" s="57" t="s">
+      <c r="B532" s="64"/>
+      <c r="C532" s="58" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="533" ht="15" spans="1:3">
       <c r="A533" s="13"/>
-      <c r="B533" s="63"/>
-      <c r="C533" s="57" t="s">
+      <c r="B533" s="64"/>
+      <c r="C533" s="58" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="534" ht="12" customHeight="1" spans="1:3">
       <c r="A534" s="13"/>
-      <c r="B534" s="63"/>
-      <c r="C534" s="57"/>
+      <c r="B534" s="64"/>
+      <c r="C534" s="58"/>
     </row>
     <row r="535" ht="15" spans="1:3">
       <c r="A535" s="13"/>
-      <c r="B535" s="63" t="s">
+      <c r="B535" s="64" t="s">
         <v>501</v>
       </c>
-      <c r="C535" s="58" t="s">
+      <c r="C535" s="59" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="536" ht="15" spans="1:3">
       <c r="A536" s="13"/>
-      <c r="B536" s="63"/>
-      <c r="C536" s="57" t="s">
+      <c r="B536" s="64"/>
+      <c r="C536" s="58" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="537" ht="15" spans="1:3">
       <c r="A537" s="13"/>
-      <c r="B537" s="63"/>
-      <c r="C537" s="57" t="s">
+      <c r="B537" s="64"/>
+      <c r="C537" s="58" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="538" ht="11" customHeight="1" spans="1:3">
       <c r="A538" s="13"/>
-      <c r="B538" s="63"/>
-      <c r="C538" s="57"/>
+      <c r="B538" s="64"/>
+      <c r="C538" s="58"/>
     </row>
     <row r="539" ht="15" spans="1:3">
       <c r="A539" s="13"/>
-      <c r="B539" s="63" t="s">
+      <c r="B539" s="64" t="s">
         <v>505</v>
       </c>
       <c r="C539" s="54" t="s">
@@ -16404,47 +16480,47 @@
     </row>
     <row r="540" ht="15" spans="1:3">
       <c r="A540" s="13"/>
-      <c r="B540" s="63"/>
-      <c r="C540" s="57" t="s">
+      <c r="B540" s="64"/>
+      <c r="C540" s="58" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="541" ht="15" spans="1:3">
       <c r="A541" s="13"/>
-      <c r="B541" s="63"/>
-      <c r="C541" s="57" t="s">
+      <c r="B541" s="64"/>
+      <c r="C541" s="58" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="542" ht="15" spans="1:3">
       <c r="A542" s="13"/>
-      <c r="B542" s="63"/>
-      <c r="C542" s="57" t="s">
+      <c r="B542" s="64"/>
+      <c r="C542" s="58" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="543" ht="15" spans="1:3">
       <c r="A543" s="13"/>
-      <c r="B543" s="63"/>
-      <c r="C543" s="57" t="s">
+      <c r="B543" s="64"/>
+      <c r="C543" s="58" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="544" ht="15" spans="1:3">
       <c r="A544" s="13"/>
-      <c r="B544" s="63"/>
-      <c r="C544" s="57" t="s">
+      <c r="B544" s="64"/>
+      <c r="C544" s="58" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="545" ht="15.75" spans="1:3">
       <c r="A545" s="13"/>
       <c r="B545" s="6"/>
-      <c r="C545" s="57"/>
+      <c r="C545" s="58"/>
     </row>
     <row r="546" ht="15" spans="1:3">
       <c r="A546" s="13"/>
-      <c r="B546" s="63" t="s">
+      <c r="B546" s="64" t="s">
         <v>512</v>
       </c>
       <c r="C546" s="54" t="s">
@@ -16453,29 +16529,29 @@
     </row>
     <row r="547" ht="15" spans="1:3">
       <c r="A547" s="13"/>
-      <c r="B547" s="63"/>
-      <c r="C547" s="57" t="s">
+      <c r="B547" s="64"/>
+      <c r="C547" s="58" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="548" ht="15" spans="1:3">
       <c r="A548" s="13"/>
-      <c r="B548" s="63"/>
-      <c r="C548" s="57" t="s">
+      <c r="B548" s="64"/>
+      <c r="C548" s="58" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="549" ht="15" spans="1:3">
       <c r="A549" s="13"/>
-      <c r="B549" s="63"/>
-      <c r="C549" s="57" t="s">
+      <c r="B549" s="64"/>
+      <c r="C549" s="58" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="550" ht="18" spans="1:3">
       <c r="A550" s="13"/>
       <c r="B550" s="17"/>
-      <c r="C550" s="57"/>
+      <c r="C550" s="58"/>
     </row>
     <row r="551" ht="15" spans="1:3">
       <c r="A551" s="13"/>
@@ -19343,12 +19419,12 @@
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -19605,46 +19681,215 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="35" ht="8" customHeight="1" spans="1:4">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" ht="12" customHeight="1" spans="2:3">
-      <c r="B36" s="4"/>
-      <c r="C36" s="10"/>
-    </row>
-    <row r="37" ht="15.75" spans="2:2">
-      <c r="B37" s="4"/>
-    </row>
-    <row r="39" ht="37.5" spans="1:2">
-      <c r="A39" s="11" t="s">
-        <v>1714</v>
-      </c>
-      <c r="B39" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" ht="37.5" spans="1:2">
-      <c r="A40" s="11" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B40" s="12">
-        <v>16</v>
+    <row r="35" ht="12" customHeight="1" spans="1:3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" ht="12" customHeight="1" spans="1:3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="6" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="37" ht="12" customHeight="1" spans="1:3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="38" ht="12" customHeight="1" spans="1:3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="39" ht="12" customHeight="1" spans="1:3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="40" ht="12" customHeight="1" spans="1:3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="41" ht="12" customHeight="1" spans="1:3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="42" ht="12" customHeight="1" spans="1:3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="43" ht="12" customHeight="1" spans="1:3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="44" ht="12" customHeight="1" spans="1:3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" ht="12" customHeight="1" spans="1:3">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" ht="12" customHeight="1" spans="1:3">
+      <c r="A46" s="3"/>
+      <c r="B46" s="6" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="47" ht="12" customHeight="1" spans="1:3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="48" ht="12" customHeight="1" spans="1:3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="7" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="49" ht="12" customHeight="1" spans="1:3">
+      <c r="A49" s="3"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="50" ht="12" customHeight="1" spans="1:3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="51" ht="12" customHeight="1" spans="1:3">
+      <c r="A51" s="3"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="52" ht="12" customHeight="1" spans="1:3">
+      <c r="A52" s="3"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="7" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="53" ht="12" customHeight="1" spans="1:3">
+      <c r="A53" s="3"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" ht="12" customHeight="1" spans="1:3">
+      <c r="A54" s="3"/>
+      <c r="B54" s="6" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" ht="12" customHeight="1" spans="1:3">
+      <c r="A55" s="3"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="7" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="56" ht="12" customHeight="1" spans="1:3">
+      <c r="A56" s="3"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="57" ht="12" customHeight="1" spans="1:3">
+      <c r="A57" s="3"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="58" ht="8" customHeight="1" spans="1:4">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" ht="12" customHeight="1" spans="2:3">
+      <c r="B59" s="4"/>
+      <c r="C59" s="10"/>
+    </row>
+    <row r="60" ht="12" customHeight="1" spans="2:3">
+      <c r="B60" s="4"/>
+      <c r="C60" s="10"/>
+    </row>
+    <row r="61" ht="12" customHeight="1" spans="2:3">
+      <c r="B61" s="4"/>
+      <c r="C61" s="10"/>
+    </row>
+    <row r="62" ht="37.5" spans="1:2">
+      <c r="A62" s="11" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B62" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" ht="37.5" spans="1:2">
+      <c r="A63" s="11" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B63" s="12">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A3:A34"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A3:A57"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B36:B44"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="B54:B57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -19785,133 +20030,133 @@
       <c r="B16" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="58" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="13"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="58" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="13"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="58" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="13"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="58" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="13"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="58" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="13"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="58" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="13"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="58" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="13"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="58" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="1:3">
       <c r="A24" s="13"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="57"/>
+      <c r="C24" s="58"/>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="13"/>
       <c r="B25" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="58" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="13"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="58" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="13"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="58" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="13"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="58" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
       <c r="A29" s="13"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="58" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="13"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="58" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="13"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="58" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="13"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="57" t="s">
+      <c r="C32" s="58" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="33" ht="12" customHeight="1" spans="1:3">
       <c r="A33" s="13"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="57"/>
+      <c r="C33" s="58"/>
     </row>
     <row r="34" ht="16" customHeight="1" spans="1:3">
       <c r="A34" s="13"/>
       <c r="B34" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="C34" s="57" t="s">
+      <c r="C34" s="58" t="s">
         <v>524</v>
       </c>
     </row>
@@ -19953,7 +20198,7 @@
       <c r="B40" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="57" t="s">
+      <c r="C40" s="58" t="s">
         <v>551</v>
       </c>
     </row>
@@ -20059,203 +20304,203 @@
       <c r="B55" s="6" t="s">
         <v>564</v>
       </c>
-      <c r="C55" s="57" t="s">
+      <c r="C55" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:3">
       <c r="A56" s="13"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="57" t="s">
+      <c r="C56" s="58" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="13"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="57" t="s">
+      <c r="C57" s="58" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
       <c r="A58" s="13"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="57" t="s">
+      <c r="C58" s="58" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="59" ht="15" spans="1:3">
       <c r="A59" s="13"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="57" t="s">
+      <c r="C59" s="58" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="13"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="57" t="s">
+      <c r="C60" s="58" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="13"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="57" t="s">
+      <c r="C61" s="58" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="62" ht="15.75" spans="1:3">
       <c r="A62" s="13"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="57"/>
+      <c r="C62" s="58"/>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="13"/>
       <c r="B63" s="6" t="s">
         <v>570</v>
       </c>
-      <c r="C63" s="57" t="s">
+      <c r="C63" s="58" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:3">
       <c r="A64" s="13"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="57" t="s">
+      <c r="C64" s="58" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:3">
       <c r="A65" s="13"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="57" t="s">
+      <c r="C65" s="58" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:3">
       <c r="A66" s="13"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="57" t="s">
+      <c r="C66" s="58" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="67" ht="15.75" spans="1:3">
       <c r="A67" s="13"/>
       <c r="B67" s="6"/>
-      <c r="C67" s="57"/>
+      <c r="C67" s="58"/>
     </row>
     <row r="68" ht="15" spans="1:3">
       <c r="A68" s="13"/>
       <c r="B68" s="6" t="s">
         <v>574</v>
       </c>
-      <c r="C68" s="58" t="s">
+      <c r="C68" s="59" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:3">
       <c r="A69" s="13"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="57" t="s">
+      <c r="C69" s="58" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:3">
       <c r="A70" s="13"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="57" t="s">
+      <c r="C70" s="58" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="71" ht="15" spans="1:3">
       <c r="A71" s="13"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="57" t="s">
+      <c r="C71" s="58" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="72" ht="15" spans="1:3">
       <c r="A72" s="13"/>
       <c r="B72" s="6"/>
-      <c r="C72" s="57" t="s">
+      <c r="C72" s="58" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="73" ht="15" spans="1:3">
       <c r="A73" s="13"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="57" t="s">
+      <c r="C73" s="58" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:3">
       <c r="A74" s="13"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="57" t="s">
+      <c r="C74" s="58" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="75" ht="15" spans="1:3">
       <c r="A75" s="13"/>
       <c r="B75" s="6"/>
-      <c r="C75" s="58" t="s">
+      <c r="C75" s="59" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="76" ht="15" spans="1:3">
       <c r="A76" s="13"/>
       <c r="B76" s="6"/>
-      <c r="C76" s="58" t="s">
+      <c r="C76" s="59" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="77" ht="15" spans="1:3">
       <c r="A77" s="13"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="58" t="s">
+      <c r="C77" s="59" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="78" ht="15" spans="1:3">
       <c r="A78" s="13"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="58" t="s">
+      <c r="C78" s="59" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="79" ht="15" spans="1:3">
       <c r="A79" s="13"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="58" t="s">
+      <c r="C79" s="59" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="80" ht="15" spans="1:3">
       <c r="A80" s="13"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="58" t="s">
+      <c r="C80" s="59" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="81" ht="15" spans="1:3">
       <c r="A81" s="13"/>
       <c r="B81" s="6"/>
-      <c r="C81" s="58" t="s">
+      <c r="C81" s="59" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="82" ht="15" spans="1:3">
       <c r="A82" s="13"/>
       <c r="B82" s="6"/>
-      <c r="C82" s="58" t="s">
+      <c r="C82" s="59" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="83" ht="15.75" spans="1:3">
       <c r="A83" s="13"/>
       <c r="B83" s="6"/>
-      <c r="C83" s="58"/>
+      <c r="C83" s="59"/>
     </row>
     <row r="84" ht="15" spans="1:3">
       <c r="A84" s="13"/>
@@ -20370,97 +20615,97 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="56" t="s">
         <v>595</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>596</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="57" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="6"/>
       <c r="C4" s="41" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="5" ht="18" customHeight="1" spans="1:3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="6"/>
       <c r="C5" s="37" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="6" ht="17" customHeight="1" spans="1:3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="6"/>
       <c r="C6" s="37" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="8" ht="18" customHeight="1" spans="1:3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="6"/>
       <c r="C8" s="38" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1" spans="1:3">
-      <c r="A9" s="3"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="10" ht="17" customHeight="1" spans="1:3">
-      <c r="A10" s="3"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="11" ht="18" customHeight="1" spans="1:3">
-      <c r="A11" s="3"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
-      <c r="A12" s="3"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
-      <c r="A13" s="3"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
-      <c r="A14" s="3"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="58" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="58" t="s">
         <v>609</v>
       </c>
     </row>
@@ -20602,161 +20847,161 @@
       <c r="B35" s="6" t="s">
         <v>626</v>
       </c>
-      <c r="C35" s="57" t="s">
+      <c r="C35" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="13"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="57" t="s">
+      <c r="C36" s="58" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
       <c r="A37" s="13"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="58" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="13"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="57" t="s">
+      <c r="C38" s="58" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="13"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="57" t="s">
+      <c r="C39" s="58" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="13"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="57" t="s">
+      <c r="C40" s="58" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="13"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="57" t="s">
+      <c r="C41" s="58" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="13"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="57" t="s">
+      <c r="C42" s="58" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="13"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="57" t="s">
+      <c r="C43" s="58" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="13"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="58" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="1:3">
       <c r="A45" s="13"/>
       <c r="B45" s="6"/>
-      <c r="C45" s="57"/>
+      <c r="C45" s="58"/>
     </row>
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="13"/>
       <c r="B46" s="6" t="s">
         <v>635</v>
       </c>
-      <c r="C46" s="57" t="s">
+      <c r="C46" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="13"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="57" t="s">
+      <c r="C47" s="58" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="13"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="57" t="s">
+      <c r="C48" s="58" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="13"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="57" t="s">
+      <c r="C49" s="58" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="50" ht="18" customHeight="1" spans="1:3">
       <c r="A50" s="13"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="57" t="s">
+      <c r="C50" s="58" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="51" ht="16" customHeight="1" spans="1:3">
       <c r="A51" s="13"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="58" t="s">
+      <c r="C51" s="59" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1" spans="1:3">
       <c r="A52" s="13"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="57" t="s">
+      <c r="C52" s="58" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="13"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="57" t="s">
+      <c r="C53" s="58" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="54" ht="21" customHeight="1" spans="1:3">
       <c r="A54" s="13"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="57" t="s">
+      <c r="C54" s="58" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="55" ht="21" customHeight="1" spans="1:3">
       <c r="A55" s="13"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="57" t="s">
+      <c r="C55" s="58" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="56" ht="21" customHeight="1" spans="1:3">
       <c r="A56" s="13"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="57" t="s">
+      <c r="C56" s="58" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="57" ht="21" customHeight="1" spans="1:3">
       <c r="A57" s="13"/>
       <c r="B57" s="4"/>
-      <c r="C57" s="57"/>
+      <c r="C57" s="58"/>
     </row>
     <row r="58" ht="21" customHeight="1" spans="1:3">
       <c r="A58" s="13"/>
@@ -20794,53 +21039,53 @@
       <c r="C62" s="2"/>
     </row>
     <row r="63" ht="15" spans="1:3">
-      <c r="A63" s="59" t="s">
+      <c r="A63" s="60" t="s">
         <v>649</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>650</v>
       </c>
-      <c r="C63" s="56" t="s">
+      <c r="C63" s="57" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="59"/>
+      <c r="A64" s="60"/>
       <c r="B64" s="6"/>
       <c r="C64" s="41" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="65" ht="18" customHeight="1" spans="1:3">
-      <c r="A65" s="59"/>
+      <c r="A65" s="60"/>
       <c r="B65" s="6"/>
       <c r="C65" s="37" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="66" ht="17" customHeight="1" spans="1:3">
-      <c r="A66" s="59"/>
+      <c r="A66" s="60"/>
       <c r="B66" s="6"/>
       <c r="C66" s="37" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="67" ht="14" customHeight="1" spans="1:3">
-      <c r="A67" s="59"/>
+      <c r="A67" s="60"/>
       <c r="B67" s="6"/>
       <c r="C67" s="5" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="68" ht="18" customHeight="1" spans="1:3">
-      <c r="A68" s="59"/>
+      <c r="A68" s="60"/>
       <c r="B68" s="6"/>
       <c r="C68" s="38" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="69" ht="16" customHeight="1" spans="1:3">
-      <c r="A69" s="59"/>
+      <c r="A69" s="60"/>
       <c r="B69" s="6"/>
       <c r="C69" s="5" t="s">
         <v>657</v>
@@ -20857,7 +21102,7 @@
       <c r="C71" s="53"/>
     </row>
     <row r="72" ht="15.75" spans="1:3">
-      <c r="A72" s="59" t="s">
+      <c r="A72" s="60" t="s">
         <v>659</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -20868,12 +21113,12 @@
       </c>
     </row>
     <row r="73" ht="10" customHeight="1" spans="1:3">
-      <c r="A73" s="59"/>
+      <c r="A73" s="60"/>
       <c r="B73" s="4"/>
       <c r="C73" s="55"/>
     </row>
     <row r="74" ht="19" customHeight="1" spans="1:3">
-      <c r="A74" s="59"/>
+      <c r="A74" s="60"/>
       <c r="B74" s="6" t="s">
         <v>660</v>
       </c>
@@ -20882,79 +21127,79 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="59"/>
+      <c r="A75" s="60"/>
       <c r="B75" s="6"/>
       <c r="C75" s="40" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="76" ht="18" customHeight="1" spans="1:3">
-      <c r="A76" s="59"/>
+      <c r="A76" s="60"/>
       <c r="B76" s="6"/>
       <c r="C76" s="38" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="77" ht="12" customHeight="1" spans="1:3">
-      <c r="A77" s="59"/>
+      <c r="A77" s="60"/>
       <c r="B77" s="6"/>
       <c r="C77" s="38" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="78" ht="14" customHeight="1" spans="1:3">
-      <c r="A78" s="59"/>
+      <c r="A78" s="60"/>
       <c r="B78" s="6"/>
       <c r="C78" s="7" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="79" ht="18" customHeight="1" spans="1:3">
-      <c r="A79" s="59"/>
+      <c r="A79" s="60"/>
       <c r="B79" s="6"/>
       <c r="C79" s="38" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="80" ht="18" customHeight="1" spans="1:3">
-      <c r="A80" s="59"/>
+      <c r="A80" s="60"/>
       <c r="B80" s="6"/>
       <c r="C80" s="38" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="81" ht="15.75" spans="1:3">
-      <c r="A81" s="59"/>
+      <c r="A81" s="60"/>
       <c r="B81" s="6"/>
       <c r="C81" s="7"/>
     </row>
     <row r="82" ht="15" spans="1:3">
-      <c r="A82" s="59"/>
+      <c r="A82" s="60"/>
       <c r="B82" s="6" t="s">
         <v>667</v>
       </c>
-      <c r="C82" s="57" t="s">
+      <c r="C82" s="58" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="83" ht="15" spans="1:3">
-      <c r="A83" s="59"/>
+      <c r="A83" s="60"/>
       <c r="B83" s="6"/>
-      <c r="C83" s="57" t="s">
+      <c r="C83" s="58" t="s">
         <v>669</v>
       </c>
     </row>
     <row r="84" ht="15" spans="1:3">
-      <c r="A84" s="59"/>
+      <c r="A84" s="60"/>
       <c r="B84" s="6"/>
-      <c r="C84" s="57" t="s">
+      <c r="C84" s="58" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="85" ht="15" spans="1:3">
-      <c r="A85" s="59"/>
+      <c r="A85" s="60"/>
       <c r="B85" s="6"/>
-      <c r="C85" s="57" t="s">
+      <c r="C85" s="58" t="s">
         <v>671</v>
       </c>
     </row>

</xml_diff>